<commit_message>
Add new bugs: 34-49
</commit_message>
<xml_diff>
--- a/Testing of the Registration Form.xlsx
+++ b/Testing of the Registration Form.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="752" uniqueCount="387">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="859" uniqueCount="433">
   <si>
     <t>http://itcareer.pythonanywhere.com/</t>
   </si>
@@ -785,9 +785,6 @@
 password: 0cAI3l</t>
   </si>
   <si>
-    <t>Можна зареєструватись</t>
-  </si>
-  <si>
     <t>Register by entering the name of the domain part separated by a hyphen</t>
   </si>
   <si>
@@ -950,7 +947,7 @@
 password: %|lhGI</t>
   </si>
   <si>
-    <t>Register by entering a password of 6 characters but special characters</t>
+    <t>Register by entering a password of 6 characters but without special characters</t>
   </si>
   <si>
     <t>name: Viola
@@ -1408,9 +1405,6 @@
     <t>The field frame is highlighted in red. A message appears with a hint that the surname can only be in Latin</t>
   </si>
   <si>
-    <t>Major</t>
-  </si>
-  <si>
     <t>It is possible to register by entering the surname in digits</t>
   </si>
   <si>
@@ -1949,7 +1943,389 @@
 3. Pay attention to the message about successful registration.</t>
   </si>
   <si>
-    <t>It is possible to register by entering</t>
+    <t>It is possible to register by entering the domain name with two hyphens in a row</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Marcos
+surname: Veum
+email: email@domain--name.com
+password: 0cAI3l
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering the domain name with two consecutive dots</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Fredy
+surname: Batz
+email: email@domain..com
+password: 0cAI3l
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering the domain name with hyphens at the beginning and end</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Dorthy
+surname: Watsica
+email: email@-domain-.com
+password: 0cAI3l
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering all data except password</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Ariel
+surname: Sanford
+email: email1@domain.com
+password: 
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>The field frame is highlighted in red. A message appears with a hint that you need to enter the password</t>
+  </si>
+  <si>
+    <t>High</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering a password of five characters</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Raleigh
+surname: Volkman
+email: email35@domain.com
+password: 0cAI3
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>The field frame is highlighted in red. A message appears with a hint that the password must consist of at least six characters</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering a password of 25 characters</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Armando
+surname: Klein
+email: email37@domain.com
+password: |0Ckm0B;OI8IA4|l)0l6l|)ed
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>The field frame is highlighted in red. A message appears with a hint that the password must consist of a maximum of 25 characters</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering a password of 6 Cyrillic characters</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Michaela
+surname: Jones
+email: email38@domain.com
+password: ждлзщш
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>The field frame is highlighted in red. A message appears with a hint that the password must consist of at least one Latin letter, a number, a special character</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering a password of 6 digits</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Emmie
+surname: Braun
+email: email39@domain.com
+password: 123456
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering a password of 6 special characters</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Betsy
+surname: Bergnaum
+email: email40@domain.com
+password: !@#$%^
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering a valid password with spaces at the beginning and end</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Linwood
+surname: Kunde
+email: email41@domain.com
+password:  !F#1%^ 
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>The field frame is highlighted in red. A message appears with a hint that the password must not contain spaces</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering a password of 6 characters but without lowercase Latin letters</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Helen
+surname: Daugherty
+email: email42@domain.com
+password: |04&amp;OM
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering a password of 6 characters but without uppercase Latin letters</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Terence
+surname: Hintz
+email: email43@domain.com
+password: 5|l0y(
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering a password of 6 characters but without numbers</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Shane
+surname: Sauer
+email: email44@domain.com
+password: %|lhGI
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>It is possible to register with password of 6 characters but no special characters required</t>
+  </si>
+  <si>
+    <r>
+      <rPr/>
+      <t xml:space="preserve">The page of the registration form is opened:
+</t>
+    </r>
+    <r>
+      <rPr>
+        <color rgb="FF1155CC"/>
+        <u/>
+      </rPr>
+      <t>http://itcareer.pythonanywhere.com/</t>
+    </r>
+  </si>
+  <si>
+    <t>1. Enter the following credentials in the form fields:
+name: Viola
+surname: Lubowitz
+email: email45@domain.com
+password: 1B9sOl
+2. Submit the form.
+3. Pay attention to the message about successful registration.</t>
+  </si>
+  <si>
+    <t>It is possible to register by entering a password of 6 characters but special characters</t>
   </si>
 </sst>
 </file>
@@ -6843,16 +7219,16 @@
       <c r="D72" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E72" s="29" t="s">
-        <v>194</v>
+      <c r="E72" s="19">
+        <v>35.0</v>
       </c>
     </row>
     <row r="73">
       <c r="B73" s="17" t="s">
+        <v>194</v>
+      </c>
+      <c r="C73" s="3" t="s">
         <v>195</v>
-      </c>
-      <c r="C73" s="3" t="s">
-        <v>196</v>
       </c>
       <c r="D73" s="21" t="s">
         <v>67</v>
@@ -6861,24 +7237,24 @@
     </row>
     <row r="74">
       <c r="B74" s="17" t="s">
+        <v>196</v>
+      </c>
+      <c r="C74" s="3" t="s">
         <v>197</v>
-      </c>
-      <c r="C74" s="3" t="s">
-        <v>198</v>
       </c>
       <c r="D74" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E74" s="29" t="s">
-        <v>194</v>
+      <c r="E74" s="19">
+        <v>36.0</v>
       </c>
     </row>
     <row r="75">
       <c r="B75" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="C75" s="3" t="s">
         <v>199</v>
-      </c>
-      <c r="C75" s="3" t="s">
-        <v>200</v>
       </c>
       <c r="D75" s="21" t="s">
         <v>67</v>
@@ -6887,38 +7263,38 @@
     </row>
     <row r="76">
       <c r="B76" s="17" t="s">
+        <v>200</v>
+      </c>
+      <c r="C76" s="24" t="s">
         <v>201</v>
-      </c>
-      <c r="C76" s="24" t="s">
-        <v>202</v>
       </c>
       <c r="D76" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E76" s="29" t="s">
-        <v>194</v>
+      <c r="E76" s="19">
+        <v>37.0</v>
       </c>
     </row>
     <row r="77">
       <c r="B77" s="17" t="s">
+        <v>202</v>
+      </c>
+      <c r="C77" s="3" t="s">
         <v>203</v>
-      </c>
-      <c r="C77" s="3" t="s">
-        <v>204</v>
       </c>
       <c r="D77" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E77" s="29" t="s">
-        <v>194</v>
+      <c r="E77" s="19">
+        <v>38.0</v>
       </c>
     </row>
     <row r="78">
       <c r="B78" s="17" t="s">
+        <v>204</v>
+      </c>
+      <c r="C78" s="24" t="s">
         <v>205</v>
-      </c>
-      <c r="C78" s="24" t="s">
-        <v>206</v>
       </c>
       <c r="D78" s="21" t="s">
         <v>67</v>
@@ -6928,7 +7304,7 @@
     </row>
     <row r="79">
       <c r="B79" s="17" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C79" s="24"/>
       <c r="D79" s="21" t="s">
@@ -6939,41 +7315,41 @@
     </row>
     <row r="80">
       <c r="B80" s="17" t="s">
+        <v>207</v>
+      </c>
+      <c r="C80" s="24" t="s">
         <v>208</v>
-      </c>
-      <c r="C80" s="24" t="s">
-        <v>209</v>
       </c>
       <c r="D80" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E80" s="29" t="s">
-        <v>194</v>
+      <c r="E80" s="19">
+        <v>39.0</v>
       </c>
       <c r="F80" s="33" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="81">
       <c r="B81" s="17" t="s">
+        <v>210</v>
+      </c>
+      <c r="C81" s="3" t="s">
         <v>211</v>
-      </c>
-      <c r="C81" s="3" t="s">
-        <v>212</v>
       </c>
       <c r="D81" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E81" s="29" t="s">
-        <v>194</v>
+      <c r="E81" s="19">
+        <v>40.0</v>
       </c>
     </row>
     <row r="82">
       <c r="B82" s="17" t="s">
+        <v>212</v>
+      </c>
+      <c r="C82" s="24" t="s">
         <v>213</v>
-      </c>
-      <c r="C82" s="24" t="s">
-        <v>214</v>
       </c>
       <c r="D82" s="21" t="s">
         <v>67</v>
@@ -6982,128 +7358,128 @@
     </row>
     <row r="83">
       <c r="B83" s="17" t="s">
+        <v>214</v>
+      </c>
+      <c r="C83" s="3" t="s">
         <v>215</v>
-      </c>
-      <c r="C83" s="3" t="s">
-        <v>216</v>
       </c>
       <c r="D83" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E83" s="29" t="s">
-        <v>194</v>
+      <c r="E83" s="19">
+        <v>41.0</v>
       </c>
     </row>
     <row r="84">
       <c r="B84" s="17" t="s">
+        <v>216</v>
+      </c>
+      <c r="C84" s="24" t="s">
         <v>217</v>
-      </c>
-      <c r="C84" s="24" t="s">
-        <v>218</v>
       </c>
       <c r="D84" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E84" s="29" t="s">
-        <v>194</v>
+      <c r="E84" s="19">
+        <v>42.0</v>
       </c>
     </row>
     <row r="85">
       <c r="B85" s="17" t="s">
+        <v>218</v>
+      </c>
+      <c r="C85" s="24" t="s">
         <v>219</v>
-      </c>
-      <c r="C85" s="24" t="s">
-        <v>220</v>
       </c>
       <c r="D85" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E85" s="29" t="s">
-        <v>194</v>
+      <c r="E85" s="19">
+        <v>43.0</v>
       </c>
     </row>
     <row r="86">
       <c r="B86" s="17" t="s">
+        <v>220</v>
+      </c>
+      <c r="C86" s="24" t="s">
         <v>221</v>
-      </c>
-      <c r="C86" s="24" t="s">
-        <v>222</v>
       </c>
       <c r="D86" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E86" s="29" t="s">
-        <v>194</v>
+      <c r="E86" s="19">
+        <v>44.0</v>
       </c>
     </row>
     <row r="87">
       <c r="B87" s="17" t="s">
+        <v>222</v>
+      </c>
+      <c r="C87" s="24" t="s">
         <v>223</v>
-      </c>
-      <c r="C87" s="24" t="s">
-        <v>224</v>
       </c>
       <c r="D87" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E87" s="29" t="s">
-        <v>194</v>
+      <c r="E87" s="19">
+        <v>45.0</v>
       </c>
     </row>
     <row r="88">
       <c r="B88" s="17" t="s">
+        <v>224</v>
+      </c>
+      <c r="C88" s="24" t="s">
         <v>225</v>
-      </c>
-      <c r="C88" s="24" t="s">
-        <v>226</v>
       </c>
       <c r="D88" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E88" s="29" t="s">
-        <v>194</v>
+      <c r="E88" s="19">
+        <v>46.0</v>
       </c>
     </row>
     <row r="89">
       <c r="B89" s="17" t="s">
+        <v>226</v>
+      </c>
+      <c r="C89" s="24" t="s">
         <v>227</v>
-      </c>
-      <c r="C89" s="24" t="s">
-        <v>228</v>
       </c>
       <c r="D89" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E89" s="29" t="s">
-        <v>194</v>
+      <c r="E89" s="19">
+        <v>47.0</v>
       </c>
     </row>
     <row r="90">
       <c r="B90" s="17" t="s">
+        <v>228</v>
+      </c>
+      <c r="C90" s="20" t="s">
         <v>229</v>
-      </c>
-      <c r="C90" s="20" t="s">
-        <v>230</v>
       </c>
       <c r="D90" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E90" s="29" t="s">
-        <v>194</v>
+      <c r="E90" s="19">
+        <v>48.0</v>
       </c>
     </row>
     <row r="91">
       <c r="B91" s="17" t="s">
+        <v>230</v>
+      </c>
+      <c r="C91" s="20" t="s">
         <v>231</v>
-      </c>
-      <c r="C91" s="20" t="s">
-        <v>232</v>
       </c>
       <c r="D91" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="E91" s="29" t="s">
-        <v>194</v>
+      <c r="E91" s="19">
+        <v>49.0</v>
       </c>
     </row>
     <row r="94">
@@ -10812,34 +11188,34 @@
   <sheetData>
     <row r="1">
       <c r="A1" s="35" t="s">
+        <v>232</v>
+      </c>
+      <c r="B1" s="36" t="s">
         <v>233</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="C1" s="37" t="s">
         <v>234</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="D1" s="36" t="s">
         <v>235</v>
       </c>
-      <c r="D1" s="36" t="s">
+      <c r="E1" s="36" t="s">
         <v>236</v>
       </c>
-      <c r="E1" s="36" t="s">
+      <c r="F1" s="37" t="s">
         <v>237</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="G1" s="37" t="s">
         <v>238</v>
       </c>
-      <c r="G1" s="37" t="s">
+      <c r="H1" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="I1" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="J1" s="37" t="s">
         <v>241</v>
-      </c>
-      <c r="J1" s="37" t="s">
-        <v>242</v>
       </c>
     </row>
     <row r="2">
@@ -10847,31 +11223,31 @@
         <v>1.0</v>
       </c>
       <c r="B2" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="C2" s="38" t="s">
         <v>243</v>
       </c>
-      <c r="C2" s="38" t="s">
+      <c r="D2" s="17" t="s">
         <v>244</v>
       </c>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="17" t="s">
+        <v>242</v>
+      </c>
+      <c r="F2" s="17" t="s">
         <v>245</v>
       </c>
-      <c r="E2" s="17" t="s">
-        <v>243</v>
-      </c>
-      <c r="F2" s="17" t="s">
+      <c r="G2" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="H2" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="I2" s="17" t="s">
         <v>248</v>
       </c>
-      <c r="I2" s="17" t="s">
+      <c r="J2" s="38" t="s">
         <v>249</v>
-      </c>
-      <c r="J2" s="38" t="s">
-        <v>250</v>
       </c>
     </row>
     <row r="3">
@@ -10879,31 +11255,31 @@
         <v>2.0</v>
       </c>
       <c r="B3" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="C3" s="38" t="s">
         <v>251</v>
       </c>
-      <c r="C3" s="38" t="s">
+      <c r="D3" s="17" t="s">
         <v>252</v>
       </c>
-      <c r="D3" s="17" t="s">
+      <c r="E3" s="17" t="s">
+        <v>250</v>
+      </c>
+      <c r="F3" s="17" t="s">
         <v>253</v>
       </c>
-      <c r="E3" s="17" t="s">
-        <v>251</v>
-      </c>
-      <c r="F3" s="17" t="s">
+      <c r="G3" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H3" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="I3" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J3" s="38" t="s">
         <v>254</v>
-      </c>
-      <c r="G3" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H3" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="I3" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J3" s="38" t="s">
-        <v>255</v>
       </c>
     </row>
     <row r="4">
@@ -10911,31 +11287,31 @@
         <v>3.0</v>
       </c>
       <c r="B4" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="C4" s="38" t="s">
         <v>256</v>
       </c>
-      <c r="C4" s="38" t="s">
+      <c r="D4" s="17" t="s">
         <v>257</v>
       </c>
-      <c r="D4" s="17" t="s">
+      <c r="E4" s="17" t="s">
+        <v>255</v>
+      </c>
+      <c r="F4" s="17" t="s">
         <v>258</v>
       </c>
-      <c r="E4" s="17" t="s">
-        <v>256</v>
-      </c>
-      <c r="F4" s="17" t="s">
+      <c r="G4" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H4" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="I4" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J4" s="33" t="s">
         <v>259</v>
-      </c>
-      <c r="G4" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H4" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="I4" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J4" s="33" t="s">
-        <v>260</v>
       </c>
     </row>
     <row r="5">
@@ -10943,31 +11319,31 @@
         <v>4.0</v>
       </c>
       <c r="B5" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="C5" s="38" t="s">
         <v>261</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="D5" s="17" t="s">
         <v>262</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="E5" s="17" t="s">
+        <v>260</v>
+      </c>
+      <c r="F5" s="17" t="s">
         <v>263</v>
       </c>
-      <c r="E5" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="F5" s="17" t="s">
+      <c r="G5" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H5" s="24" t="s">
+        <v>247</v>
+      </c>
+      <c r="I5" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J5" s="33" t="s">
         <v>264</v>
-      </c>
-      <c r="G5" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H5" s="24" t="s">
-        <v>248</v>
-      </c>
-      <c r="I5" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J5" s="33" t="s">
-        <v>265</v>
       </c>
     </row>
     <row r="6">
@@ -10975,31 +11351,31 @@
         <v>5.0</v>
       </c>
       <c r="B6" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="C6" s="38" t="s">
         <v>266</v>
       </c>
-      <c r="C6" s="38" t="s">
+      <c r="D6" s="17" t="s">
         <v>267</v>
       </c>
-      <c r="D6" s="17" t="s">
+      <c r="E6" s="17" t="s">
+        <v>265</v>
+      </c>
+      <c r="F6" s="17" t="s">
         <v>268</v>
       </c>
-      <c r="E6" s="17" t="s">
-        <v>266</v>
-      </c>
-      <c r="F6" s="17" t="s">
+      <c r="G6" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H6" s="24" t="s">
         <v>269</v>
       </c>
-      <c r="G6" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H6" s="24" t="s">
+      <c r="I6" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J6" s="38" t="s">
         <v>270</v>
-      </c>
-      <c r="I6" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J6" s="38" t="s">
-        <v>271</v>
       </c>
     </row>
     <row r="7">
@@ -11007,31 +11383,31 @@
         <v>6.0</v>
       </c>
       <c r="B7" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" s="38" t="s">
         <v>272</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="D7" s="17" t="s">
         <v>273</v>
       </c>
-      <c r="D7" s="17" t="s">
+      <c r="E7" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="F7" s="17" t="s">
         <v>274</v>
       </c>
-      <c r="E7" s="17" t="s">
-        <v>272</v>
-      </c>
-      <c r="F7" s="17" t="s">
+      <c r="G7" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H7" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I7" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J7" s="38" t="s">
         <v>275</v>
-      </c>
-      <c r="G7" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H7" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="I7" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J7" s="38" t="s">
-        <v>276</v>
       </c>
     </row>
     <row r="8">
@@ -11039,31 +11415,31 @@
         <v>7.0</v>
       </c>
       <c r="B8" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="C8" s="38" t="s">
         <v>277</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="D8" s="7" t="s">
         <v>278</v>
       </c>
-      <c r="D8" s="7" t="s">
+      <c r="E8" s="17" t="s">
         <v>279</v>
       </c>
-      <c r="E8" s="17" t="s">
+      <c r="F8" s="17" t="s">
         <v>280</v>
       </c>
-      <c r="F8" s="17" t="s">
+      <c r="G8" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H8" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I8" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J8" s="38" t="s">
         <v>281</v>
-      </c>
-      <c r="G8" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H8" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="I8" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J8" s="38" t="s">
-        <v>282</v>
       </c>
     </row>
     <row r="9">
@@ -11071,31 +11447,31 @@
         <v>8.0</v>
       </c>
       <c r="B9" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="C9" s="38" t="s">
         <v>283</v>
       </c>
-      <c r="C9" s="38" t="s">
+      <c r="D9" s="7" t="s">
         <v>284</v>
       </c>
-      <c r="D9" s="7" t="s">
+      <c r="E9" s="17" t="s">
+        <v>282</v>
+      </c>
+      <c r="F9" s="17" t="s">
         <v>285</v>
       </c>
-      <c r="E9" s="17" t="s">
-        <v>283</v>
-      </c>
-      <c r="F9" s="17" t="s">
+      <c r="G9" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H9" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I9" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J9" s="38" t="s">
         <v>286</v>
-      </c>
-      <c r="G9" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H9" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="I9" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J9" s="38" t="s">
-        <v>287</v>
       </c>
     </row>
     <row r="10">
@@ -11103,31 +11479,31 @@
         <v>9.0</v>
       </c>
       <c r="B10" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="C10" s="38" t="s">
         <v>288</v>
       </c>
-      <c r="C10" s="38" t="s">
+      <c r="D10" s="7" t="s">
         <v>289</v>
       </c>
-      <c r="D10" s="7" t="s">
+      <c r="E10" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="F10" s="17" t="s">
         <v>290</v>
       </c>
-      <c r="E10" s="17" t="s">
-        <v>288</v>
-      </c>
-      <c r="F10" s="17" t="s">
+      <c r="G10" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H10" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J10" s="38" t="s">
         <v>291</v>
-      </c>
-      <c r="G10" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H10" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="I10" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J10" s="38" t="s">
-        <v>292</v>
       </c>
     </row>
     <row r="11">
@@ -11135,31 +11511,31 @@
         <v>10.0</v>
       </c>
       <c r="B11" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="C11" s="38" t="s">
         <v>293</v>
       </c>
-      <c r="C11" s="38" t="s">
+      <c r="D11" s="7" t="s">
         <v>294</v>
       </c>
-      <c r="D11" s="7" t="s">
+      <c r="E11" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="F11" s="17" t="s">
         <v>295</v>
       </c>
-      <c r="E11" s="17" t="s">
-        <v>293</v>
-      </c>
-      <c r="F11" s="17" t="s">
+      <c r="G11" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H11" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I11" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J11" s="38" t="s">
         <v>296</v>
-      </c>
-      <c r="G11" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H11" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="I11" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J11" s="38" t="s">
-        <v>297</v>
       </c>
     </row>
     <row r="12">
@@ -11167,31 +11543,31 @@
         <v>11.0</v>
       </c>
       <c r="B12" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="C12" s="38" t="s">
         <v>298</v>
       </c>
-      <c r="C12" s="38" t="s">
+      <c r="D12" s="7" t="s">
         <v>299</v>
       </c>
-      <c r="D12" s="7" t="s">
+      <c r="E12" s="17" t="s">
+        <v>297</v>
+      </c>
+      <c r="F12" s="17" t="s">
         <v>300</v>
       </c>
-      <c r="E12" s="17" t="s">
-        <v>298</v>
-      </c>
-      <c r="F12" s="17" t="s">
+      <c r="G12" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H12" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I12" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J12" s="33" t="s">
         <v>301</v>
-      </c>
-      <c r="G12" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H12" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="I12" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J12" s="33" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="13">
@@ -11199,31 +11575,31 @@
         <v>12.0</v>
       </c>
       <c r="B13" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="C13" s="38" t="s">
         <v>303</v>
       </c>
-      <c r="C13" s="38" t="s">
+      <c r="D13" s="17" t="s">
         <v>304</v>
       </c>
-      <c r="D13" s="17" t="s">
+      <c r="E13" s="17" t="s">
+        <v>302</v>
+      </c>
+      <c r="F13" s="17" t="s">
         <v>305</v>
       </c>
-      <c r="E13" s="17" t="s">
-        <v>303</v>
-      </c>
-      <c r="F13" s="17" t="s">
+      <c r="G13" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H13" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I13" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J13" s="38" t="s">
         <v>306</v>
-      </c>
-      <c r="G13" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H13" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="I13" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J13" s="38" t="s">
-        <v>307</v>
       </c>
     </row>
     <row r="14">
@@ -11231,31 +11607,31 @@
         <v>13.0</v>
       </c>
       <c r="B14" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="C14" s="38" t="s">
         <v>308</v>
       </c>
-      <c r="C14" s="38" t="s">
+      <c r="D14" s="17" t="s">
         <v>309</v>
       </c>
-      <c r="D14" s="17" t="s">
+      <c r="E14" s="17" t="s">
+        <v>307</v>
+      </c>
+      <c r="F14" s="17" t="s">
         <v>310</v>
       </c>
-      <c r="E14" s="17" t="s">
-        <v>308</v>
-      </c>
-      <c r="F14" s="17" t="s">
+      <c r="G14" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H14" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I14" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J14" s="38" t="s">
         <v>311</v>
-      </c>
-      <c r="G14" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H14" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="I14" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J14" s="38" t="s">
-        <v>312</v>
       </c>
     </row>
     <row r="15">
@@ -11263,31 +11639,31 @@
         <v>14.0</v>
       </c>
       <c r="B15" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="C15" s="38" t="s">
         <v>313</v>
       </c>
-      <c r="C15" s="38" t="s">
+      <c r="D15" s="17" t="s">
         <v>314</v>
       </c>
-      <c r="D15" s="17" t="s">
+      <c r="E15" s="17" t="s">
+        <v>312</v>
+      </c>
+      <c r="F15" s="17" t="s">
         <v>315</v>
       </c>
-      <c r="E15" s="17" t="s">
-        <v>313</v>
-      </c>
-      <c r="F15" s="17" t="s">
-        <v>316</v>
-      </c>
       <c r="G15" s="24" t="s">
-        <v>317</v>
+        <v>246</v>
       </c>
       <c r="H15" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I15" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J15" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K15" s="25"/>
     </row>
@@ -11296,31 +11672,31 @@
         <v>15.0</v>
       </c>
       <c r="B16" s="17" t="s">
+        <v>316</v>
+      </c>
+      <c r="C16" s="38" t="s">
+        <v>317</v>
+      </c>
+      <c r="D16" s="17" t="s">
         <v>318</v>
       </c>
-      <c r="C16" s="38" t="s">
-        <v>319</v>
-      </c>
-      <c r="D16" s="17" t="s">
-        <v>320</v>
-      </c>
       <c r="E16" s="17" t="s">
-        <v>318</v>
+        <v>316</v>
       </c>
       <c r="F16" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G16" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H16" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I16" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J16" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="17">
@@ -11328,31 +11704,31 @@
         <v>16.0</v>
       </c>
       <c r="B17" s="17" t="s">
+        <v>319</v>
+      </c>
+      <c r="C17" s="38" t="s">
+        <v>320</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>321</v>
       </c>
-      <c r="C17" s="38" t="s">
-        <v>322</v>
-      </c>
-      <c r="D17" s="17" t="s">
-        <v>323</v>
-      </c>
       <c r="E17" s="17" t="s">
-        <v>321</v>
+        <v>319</v>
       </c>
       <c r="F17" s="17" t="s">
-        <v>316</v>
+        <v>315</v>
       </c>
       <c r="G17" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H17" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I17" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J17" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="18">
@@ -11360,31 +11736,31 @@
         <v>17.0</v>
       </c>
       <c r="B18" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="C18" s="38" t="s">
+        <v>323</v>
+      </c>
+      <c r="D18" s="17" t="s">
         <v>324</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="E18" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="F18" s="17" t="s">
         <v>325</v>
       </c>
-      <c r="D18" s="17" t="s">
-        <v>326</v>
-      </c>
-      <c r="E18" s="17" t="s">
-        <v>324</v>
-      </c>
-      <c r="F18" s="17" t="s">
-        <v>327</v>
-      </c>
       <c r="G18" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H18" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I18" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J18" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="19">
@@ -11392,31 +11768,31 @@
         <v>18.0</v>
       </c>
       <c r="B19" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="C19" s="38" t="s">
+        <v>327</v>
+      </c>
+      <c r="D19" s="17" t="s">
         <v>328</v>
       </c>
-      <c r="C19" s="38" t="s">
+      <c r="E19" s="17" t="s">
+        <v>326</v>
+      </c>
+      <c r="F19" s="17" t="s">
         <v>329</v>
       </c>
-      <c r="D19" s="17" t="s">
-        <v>330</v>
-      </c>
-      <c r="E19" s="17" t="s">
-        <v>328</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>331</v>
-      </c>
       <c r="G19" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H19" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I19" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J19" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="20">
@@ -11424,31 +11800,31 @@
         <v>19.0</v>
       </c>
       <c r="B20" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="C20" s="38" t="s">
+        <v>331</v>
+      </c>
+      <c r="D20" s="17" t="s">
         <v>332</v>
       </c>
-      <c r="C20" s="38" t="s">
-        <v>333</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>334</v>
-      </c>
       <c r="E20" s="17" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="F20" s="17" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G20" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H20" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I20" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J20" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="21">
@@ -11456,31 +11832,31 @@
         <v>20.0</v>
       </c>
       <c r="B21" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="C21" s="38" t="s">
+        <v>334</v>
+      </c>
+      <c r="D21" s="17" t="s">
         <v>335</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="E21" s="17" t="s">
+        <v>333</v>
+      </c>
+      <c r="F21" s="17" t="s">
         <v>336</v>
       </c>
-      <c r="D21" s="17" t="s">
-        <v>337</v>
-      </c>
-      <c r="E21" s="17" t="s">
-        <v>335</v>
-      </c>
-      <c r="F21" s="17" t="s">
-        <v>338</v>
-      </c>
       <c r="G21" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H21" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I21" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J21" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="22">
@@ -11488,31 +11864,31 @@
         <v>21.0</v>
       </c>
       <c r="B22" s="17" t="s">
+        <v>337</v>
+      </c>
+      <c r="C22" s="38" t="s">
+        <v>338</v>
+      </c>
+      <c r="D22" s="7" t="s">
         <v>339</v>
       </c>
-      <c r="C22" s="38" t="s">
+      <c r="E22" s="17" t="s">
         <v>340</v>
       </c>
-      <c r="D22" s="7" t="s">
-        <v>341</v>
-      </c>
-      <c r="E22" s="17" t="s">
-        <v>342</v>
-      </c>
       <c r="F22" s="17" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="G22" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H22" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I22" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J22" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="23">
@@ -11520,31 +11896,31 @@
         <v>22.0</v>
       </c>
       <c r="B23" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="C23" s="38" t="s">
+        <v>342</v>
+      </c>
+      <c r="D23" s="7" t="s">
         <v>343</v>
       </c>
-      <c r="C23" s="38" t="s">
+      <c r="E23" s="17" t="s">
+        <v>341</v>
+      </c>
+      <c r="F23" s="17" t="s">
         <v>344</v>
       </c>
-      <c r="D23" s="7" t="s">
-        <v>345</v>
-      </c>
-      <c r="E23" s="17" t="s">
-        <v>343</v>
-      </c>
-      <c r="F23" s="17" t="s">
-        <v>346</v>
-      </c>
       <c r="G23" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H23" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I23" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J23" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="24">
@@ -11552,31 +11928,31 @@
         <v>23.0</v>
       </c>
       <c r="B24" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="C24" s="38" t="s">
+        <v>346</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>347</v>
       </c>
-      <c r="C24" s="38" t="s">
-        <v>348</v>
-      </c>
-      <c r="D24" s="7" t="s">
-        <v>349</v>
-      </c>
       <c r="E24" s="17" t="s">
-        <v>347</v>
+        <v>345</v>
       </c>
       <c r="F24" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G24" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H24" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I24" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J24" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="25">
@@ -11584,31 +11960,31 @@
         <v>24.0</v>
       </c>
       <c r="B25" s="17" t="s">
+        <v>348</v>
+      </c>
+      <c r="C25" s="38" t="s">
+        <v>349</v>
+      </c>
+      <c r="D25" s="7" t="s">
         <v>350</v>
       </c>
-      <c r="C25" s="38" t="s">
-        <v>351</v>
-      </c>
-      <c r="D25" s="7" t="s">
-        <v>352</v>
-      </c>
       <c r="E25" s="17" t="s">
-        <v>350</v>
+        <v>348</v>
       </c>
       <c r="F25" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G25" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H25" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I25" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J25" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="26">
@@ -11616,31 +11992,31 @@
         <v>25.0</v>
       </c>
       <c r="B26" s="17" t="s">
+        <v>351</v>
+      </c>
+      <c r="C26" s="38" t="s">
+        <v>352</v>
+      </c>
+      <c r="D26" s="7" t="s">
         <v>353</v>
       </c>
-      <c r="C26" s="38" t="s">
-        <v>354</v>
-      </c>
-      <c r="D26" s="7" t="s">
-        <v>355</v>
-      </c>
       <c r="E26" s="17" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F26" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G26" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H26" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I26" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J26" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="27">
@@ -11648,31 +12024,31 @@
         <v>26.0</v>
       </c>
       <c r="B27" s="17" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="C27" s="38" t="s">
-        <v>356</v>
+        <v>354</v>
       </c>
       <c r="D27" s="7" t="s">
-        <v>357</v>
+        <v>355</v>
       </c>
       <c r="E27" s="17" t="s">
-        <v>353</v>
+        <v>351</v>
       </c>
       <c r="F27" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G27" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H27" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I27" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J27" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="28">
@@ -11680,31 +12056,31 @@
         <v>27.0</v>
       </c>
       <c r="B28" s="17" t="s">
+        <v>356</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>357</v>
+      </c>
+      <c r="D28" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="C28" s="38" t="s">
+      <c r="E28" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="D28" s="7" t="s">
-        <v>360</v>
-      </c>
-      <c r="E28" s="17" t="s">
-        <v>361</v>
-      </c>
       <c r="F28" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G28" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H28" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I28" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J28" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="29">
@@ -11712,31 +12088,31 @@
         <v>28.0</v>
       </c>
       <c r="B29" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="C29" s="38" t="s">
+        <v>361</v>
+      </c>
+      <c r="D29" s="7" t="s">
         <v>362</v>
       </c>
-      <c r="C29" s="38" t="s">
+      <c r="E29" s="17" t="s">
         <v>363</v>
       </c>
-      <c r="D29" s="7" t="s">
-        <v>364</v>
-      </c>
-      <c r="E29" s="17" t="s">
-        <v>365</v>
-      </c>
       <c r="F29" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G29" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H29" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I29" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J29" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="30">
@@ -11744,31 +12120,31 @@
         <v>29.0</v>
       </c>
       <c r="B30" s="17" t="s">
+        <v>364</v>
+      </c>
+      <c r="C30" s="38" t="s">
+        <v>365</v>
+      </c>
+      <c r="D30" s="7" t="s">
         <v>366</v>
       </c>
-      <c r="C30" s="38" t="s">
-        <v>367</v>
-      </c>
-      <c r="D30" s="7" t="s">
-        <v>368</v>
-      </c>
       <c r="E30" s="17" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="F30" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G30" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H30" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I30" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J30" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="31">
@@ -11776,31 +12152,31 @@
         <v>30.0</v>
       </c>
       <c r="B31" s="17" t="s">
+        <v>367</v>
+      </c>
+      <c r="C31" s="38" t="s">
+        <v>368</v>
+      </c>
+      <c r="D31" s="17" t="s">
+        <v>366</v>
+      </c>
+      <c r="E31" s="17" t="s">
         <v>369</v>
       </c>
-      <c r="C31" s="38" t="s">
-        <v>370</v>
-      </c>
-      <c r="D31" s="17" t="s">
-        <v>368</v>
-      </c>
-      <c r="E31" s="17" t="s">
-        <v>371</v>
-      </c>
       <c r="F31" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G31" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H31" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I31" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J31" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="32">
@@ -11808,31 +12184,31 @@
         <v>31.0</v>
       </c>
       <c r="B32" s="17" t="s">
+        <v>370</v>
+      </c>
+      <c r="C32" s="38" t="s">
+        <v>371</v>
+      </c>
+      <c r="D32" s="17" t="s">
         <v>372</v>
       </c>
-      <c r="C32" s="38" t="s">
-        <v>373</v>
-      </c>
-      <c r="D32" s="17" t="s">
-        <v>374</v>
-      </c>
       <c r="E32" s="17" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="F32" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G32" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H32" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I32" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J32" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="33">
@@ -11840,31 +12216,31 @@
         <v>32.0</v>
       </c>
       <c r="B33" s="17" t="s">
+        <v>373</v>
+      </c>
+      <c r="C33" s="38" t="s">
+        <v>374</v>
+      </c>
+      <c r="D33" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="C33" s="38" t="s">
-        <v>376</v>
-      </c>
-      <c r="D33" s="17" t="s">
-        <v>377</v>
-      </c>
       <c r="E33" s="17" t="s">
-        <v>375</v>
+        <v>373</v>
       </c>
       <c r="F33" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G33" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H33" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I33" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J33" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K33" s="25"/>
     </row>
@@ -11873,31 +12249,31 @@
         <v>33.0</v>
       </c>
       <c r="B34" s="17" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="C34" s="38" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="D34" s="17" t="s">
-        <v>377</v>
+        <v>375</v>
       </c>
       <c r="E34" s="17" t="s">
-        <v>378</v>
+        <v>376</v>
       </c>
       <c r="F34" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G34" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H34" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I34" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J34" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K34" s="25"/>
     </row>
@@ -11906,31 +12282,31 @@
         <v>34.0</v>
       </c>
       <c r="B35" s="17" t="s">
+        <v>378</v>
+      </c>
+      <c r="C35" s="38" t="s">
+        <v>379</v>
+      </c>
+      <c r="D35" s="17" t="s">
         <v>380</v>
       </c>
-      <c r="C35" s="38" t="s">
-        <v>381</v>
-      </c>
-      <c r="D35" s="17" t="s">
-        <v>382</v>
-      </c>
       <c r="E35" s="17" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="F35" s="17" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="G35" s="24" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="H35" s="24" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I35" s="17" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="J35" s="38" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="K35" s="25"/>
     </row>
@@ -11939,53 +12315,495 @@
         <v>35.0</v>
       </c>
       <c r="B36" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="C36" s="38" t="s">
+        <v>382</v>
+      </c>
+      <c r="D36" s="17" t="s">
         <v>383</v>
       </c>
-      <c r="C36" s="38" t="s">
+      <c r="E36" s="17" t="s">
+        <v>381</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="G36" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H36" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I36" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J36" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K36" s="25"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="24">
+        <v>36.0</v>
+      </c>
+      <c r="B37" s="17" t="s">
         <v>384</v>
       </c>
-      <c r="D36" s="17" t="s">
+      <c r="C37" s="38" t="s">
         <v>385</v>
       </c>
-      <c r="E36" s="17" t="s">
-        <v>383</v>
-      </c>
-      <c r="F36" s="17" t="s">
-        <v>346</v>
-      </c>
-      <c r="G36" s="24" t="s">
-        <v>247</v>
-      </c>
-      <c r="H36" s="24" t="s">
-        <v>270</v>
-      </c>
-      <c r="I36" s="17" t="s">
-        <v>249</v>
-      </c>
-      <c r="J36" s="38" t="s">
-        <v>312</v>
-      </c>
-      <c r="K36" s="25"/>
-    </row>
-    <row r="37">
-      <c r="B37" s="3" t="s">
+      <c r="D37" s="17" t="s">
         <v>386</v>
       </c>
+      <c r="E37" s="17" t="s">
+        <v>384</v>
+      </c>
+      <c r="F37" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="G37" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H37" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I37" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J37" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K37" s="25"/>
     </row>
     <row r="38">
-      <c r="B38" s="3" t="s">
-        <v>386</v>
-      </c>
+      <c r="A38" s="24">
+        <v>37.0</v>
+      </c>
+      <c r="B38" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="C38" s="38" t="s">
+        <v>388</v>
+      </c>
+      <c r="D38" s="17" t="s">
+        <v>389</v>
+      </c>
+      <c r="E38" s="17" t="s">
+        <v>387</v>
+      </c>
+      <c r="F38" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="G38" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H38" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I38" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J38" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K38" s="25"/>
     </row>
     <row r="39">
-      <c r="B39" s="3" t="s">
-        <v>386</v>
-      </c>
+      <c r="A39" s="24">
+        <v>38.0</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>390</v>
+      </c>
+      <c r="C39" s="38" t="s">
+        <v>391</v>
+      </c>
+      <c r="D39" s="17" t="s">
+        <v>392</v>
+      </c>
+      <c r="E39" s="17" t="s">
+        <v>390</v>
+      </c>
+      <c r="F39" s="17" t="s">
+        <v>344</v>
+      </c>
+      <c r="G39" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H39" s="24" t="s">
+        <v>269</v>
+      </c>
+      <c r="I39" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J39" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K39" s="25"/>
     </row>
     <row r="40">
-      <c r="B40" s="3" t="s">
-        <v>386</v>
-      </c>
+      <c r="A40" s="24">
+        <v>39.0</v>
+      </c>
+      <c r="B40" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="C40" s="38" t="s">
+        <v>394</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>395</v>
+      </c>
+      <c r="E40" s="17" t="s">
+        <v>393</v>
+      </c>
+      <c r="F40" s="17" t="s">
+        <v>396</v>
+      </c>
+      <c r="G40" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H40" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="I40" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J40" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="K40" s="25"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="24">
+        <v>40.0</v>
+      </c>
+      <c r="B41" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="C41" s="38" t="s">
+        <v>399</v>
+      </c>
+      <c r="D41" s="17" t="s">
+        <v>400</v>
+      </c>
+      <c r="E41" s="17" t="s">
+        <v>398</v>
+      </c>
+      <c r="F41" s="17" t="s">
+        <v>401</v>
+      </c>
+      <c r="G41" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H41" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="I41" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J41" s="33" t="s">
+        <v>209</v>
+      </c>
+      <c r="K41" s="25"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="24">
+        <v>41.0</v>
+      </c>
+      <c r="B42" s="17" t="s">
+        <v>402</v>
+      </c>
+      <c r="C42" s="38" t="s">
+        <v>403</v>
+      </c>
+      <c r="D42" s="17" t="s">
+        <v>404</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>402</v>
+      </c>
+      <c r="F42" s="17" t="s">
+        <v>405</v>
+      </c>
+      <c r="G42" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H42" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="I42" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J42" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K42" s="25"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="24">
+        <v>42.0</v>
+      </c>
+      <c r="B43" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="C43" s="38" t="s">
+        <v>407</v>
+      </c>
+      <c r="D43" s="17" t="s">
+        <v>408</v>
+      </c>
+      <c r="E43" s="17" t="s">
+        <v>406</v>
+      </c>
+      <c r="F43" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="G43" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H43" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="I43" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J43" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K43" s="25"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="24">
+        <v>43.0</v>
+      </c>
+      <c r="B44" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="C44" s="38" t="s">
+        <v>411</v>
+      </c>
+      <c r="D44" s="17" t="s">
+        <v>412</v>
+      </c>
+      <c r="E44" s="17" t="s">
+        <v>410</v>
+      </c>
+      <c r="F44" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="G44" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H44" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="I44" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J44" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K44" s="25"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="24">
+        <v>44.0</v>
+      </c>
+      <c r="B45" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="C45" s="38" t="s">
+        <v>414</v>
+      </c>
+      <c r="D45" s="17" t="s">
+        <v>415</v>
+      </c>
+      <c r="E45" s="17" t="s">
+        <v>413</v>
+      </c>
+      <c r="F45" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="G45" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H45" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="I45" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J45" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K45" s="25"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="24">
+        <v>45.0</v>
+      </c>
+      <c r="B46" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="C46" s="38" t="s">
+        <v>417</v>
+      </c>
+      <c r="D46" s="17" t="s">
+        <v>418</v>
+      </c>
+      <c r="E46" s="17" t="s">
+        <v>416</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>419</v>
+      </c>
+      <c r="G46" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H46" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="I46" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J46" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K46" s="25"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="24">
+        <v>46.0</v>
+      </c>
+      <c r="B47" s="17" t="s">
+        <v>420</v>
+      </c>
+      <c r="C47" s="38" t="s">
+        <v>421</v>
+      </c>
+      <c r="D47" s="17" t="s">
+        <v>422</v>
+      </c>
+      <c r="E47" s="17" t="s">
+        <v>420</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="G47" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H47" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="I47" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J47" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K47" s="25"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="24">
+        <v>47.0</v>
+      </c>
+      <c r="B48" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="C48" s="38" t="s">
+        <v>424</v>
+      </c>
+      <c r="D48" s="17" t="s">
+        <v>425</v>
+      </c>
+      <c r="E48" s="17" t="s">
+        <v>423</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="G48" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H48" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="I48" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J48" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K48" s="25"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="24">
+        <v>48.0</v>
+      </c>
+      <c r="B49" s="17" t="s">
+        <v>426</v>
+      </c>
+      <c r="C49" s="38" t="s">
+        <v>427</v>
+      </c>
+      <c r="D49" s="17" t="s">
+        <v>428</v>
+      </c>
+      <c r="E49" s="17" t="s">
+        <v>426</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="G49" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H49" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="I49" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J49" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K49" s="25"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="24">
+        <v>49.0</v>
+      </c>
+      <c r="B50" s="17" t="s">
+        <v>429</v>
+      </c>
+      <c r="C50" s="38" t="s">
+        <v>430</v>
+      </c>
+      <c r="D50" s="17" t="s">
+        <v>431</v>
+      </c>
+      <c r="E50" s="17" t="s">
+        <v>432</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>409</v>
+      </c>
+      <c r="G50" s="24" t="s">
+        <v>246</v>
+      </c>
+      <c r="H50" s="24" t="s">
+        <v>397</v>
+      </c>
+      <c r="I50" s="17" t="s">
+        <v>248</v>
+      </c>
+      <c r="J50" s="38" t="s">
+        <v>311</v>
+      </c>
+      <c r="K50" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -12059,7 +12877,35 @@
     <hyperlink r:id="rId68" ref="J35"/>
     <hyperlink r:id="rId69" ref="C36"/>
     <hyperlink r:id="rId70" ref="J36"/>
+    <hyperlink r:id="rId71" ref="C37"/>
+    <hyperlink r:id="rId72" ref="J37"/>
+    <hyperlink r:id="rId73" ref="C38"/>
+    <hyperlink r:id="rId74" ref="J38"/>
+    <hyperlink r:id="rId75" ref="C39"/>
+    <hyperlink r:id="rId76" ref="J39"/>
+    <hyperlink r:id="rId77" ref="C40"/>
+    <hyperlink r:id="rId78" ref="J40"/>
+    <hyperlink r:id="rId79" ref="C41"/>
+    <hyperlink r:id="rId80" ref="J41"/>
+    <hyperlink r:id="rId81" ref="C42"/>
+    <hyperlink r:id="rId82" ref="J42"/>
+    <hyperlink r:id="rId83" ref="C43"/>
+    <hyperlink r:id="rId84" ref="J43"/>
+    <hyperlink r:id="rId85" ref="C44"/>
+    <hyperlink r:id="rId86" ref="J44"/>
+    <hyperlink r:id="rId87" ref="C45"/>
+    <hyperlink r:id="rId88" ref="J45"/>
+    <hyperlink r:id="rId89" ref="C46"/>
+    <hyperlink r:id="rId90" ref="J46"/>
+    <hyperlink r:id="rId91" ref="C47"/>
+    <hyperlink r:id="rId92" ref="J47"/>
+    <hyperlink r:id="rId93" ref="C48"/>
+    <hyperlink r:id="rId94" ref="J48"/>
+    <hyperlink r:id="rId95" ref="C49"/>
+    <hyperlink r:id="rId96" ref="J49"/>
+    <hyperlink r:id="rId97" ref="C50"/>
+    <hyperlink r:id="rId98" ref="J50"/>
   </hyperlinks>
-  <drawing r:id="rId71"/>
+  <drawing r:id="rId99"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Add ids for checks on Checklist sheet
</commit_message>
<xml_diff>
--- a/Testing of the Registration Form.xlsx
+++ b/Testing of the Registration Form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" state="visible" r:id="rId2"/>
@@ -1767,12 +1767,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -1815,7 +1822,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="31">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1872,55 +1879,71 @@
       <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2003,14 +2026,14 @@
   </sheetPr>
   <dimension ref="A1:B1021"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I76" activeCellId="0" sqref="I76"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.88"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.13"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5504,11 +5527,11 @@
   </sheetPr>
   <dimension ref="A1:F1009"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G90" activeCellId="0" sqref="G90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.88"/>
@@ -5550,1182 +5573,1449 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="6" t="s">
+    <row r="5" s="19" customFormat="true" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="14" t="n">
+        <v>1</v>
+      </c>
+      <c r="B5" s="15" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="16" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="4" t="s">
+      <c r="D5" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="8"/>
-    </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" s="19" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="14" t="n">
+        <v>2</v>
+      </c>
       <c r="B6" s="15" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="C6" s="14"/>
+      <c r="D6" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="17" t="n">
+      <c r="E6" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="15"/>
-    </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="14" t="n">
+        <v>3</v>
+      </c>
       <c r="B7" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="18"/>
-      <c r="D7" s="18" t="s">
+      <c r="C7" s="17"/>
+      <c r="D7" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="19"/>
-    </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="23"/>
+    </row>
+    <row r="8" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="14" t="n">
+        <v>4</v>
+      </c>
       <c r="B8" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="18"/>
-      <c r="D8" s="16" t="s">
+      <c r="C8" s="17"/>
+      <c r="D8" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="17" t="n">
+      <c r="E8" s="21" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="6" t="s">
+    <row r="9" s="19" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="14" t="n">
+        <v>5</v>
+      </c>
+      <c r="B9" s="15" t="s">
         <v>72</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="C9" s="14"/>
+      <c r="D9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="17" t="n">
+      <c r="E9" s="21" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="6" t="s">
+    <row r="10" s="19" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="14" t="n">
+        <v>6</v>
+      </c>
+      <c r="B10" s="15" t="s">
         <v>73</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="C10" s="14"/>
+      <c r="D10" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="8"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="6" t="s">
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="14" t="n">
+        <v>7</v>
+      </c>
+      <c r="B11" s="15" t="s">
         <v>74</v>
       </c>
-      <c r="D11" s="4" t="s">
+      <c r="C11" s="14"/>
+      <c r="D11" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="8"/>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="6" t="s">
+      <c r="E11" s="18"/>
+    </row>
+    <row r="12" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="14" t="n">
+        <v>8</v>
+      </c>
+      <c r="B12" s="15" t="s">
         <v>75</v>
       </c>
-      <c r="D12" s="4" t="s">
+      <c r="C12" s="14"/>
+      <c r="D12" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="8"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="14" t="n">
+        <v>9</v>
+      </c>
       <c r="B13" s="15" t="s">
         <v>76</v>
       </c>
       <c r="C13" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="D13" s="18" t="s">
+      <c r="D13" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="8"/>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E13" s="18"/>
+    </row>
+    <row r="14" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="14" t="n">
+        <v>10</v>
+      </c>
       <c r="B14" s="15" t="s">
         <v>78</v>
       </c>
       <c r="C14" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="16" t="s">
+      <c r="D14" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="17" t="n">
+      <c r="E14" s="21" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="6" t="s">
+    <row r="15" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="14" t="n">
+        <v>11</v>
+      </c>
+      <c r="B15" s="15" t="s">
         <v>79</v>
       </c>
-      <c r="D15" s="4" t="s">
+      <c r="C15" s="14"/>
+      <c r="D15" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="8"/>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="14" t="n">
+        <v>12</v>
+      </c>
       <c r="B16" s="15" t="s">
         <v>80</v>
       </c>
       <c r="C16" s="15" t="s">
         <v>81</v>
       </c>
-      <c r="D16" s="18" t="s">
+      <c r="D16" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="8"/>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="14" t="n">
+        <v>13</v>
+      </c>
       <c r="B17" s="15" t="s">
         <v>82</v>
       </c>
       <c r="C17" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="D17" s="18" t="s">
+      <c r="D17" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="8"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" s="19" customFormat="true" ht="98.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="14" t="n">
+        <v>14</v>
+      </c>
       <c r="B18" s="15" t="s">
         <v>84</v>
       </c>
       <c r="C18" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="16" t="s">
+      <c r="D18" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="17" t="n">
+      <c r="E18" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="F18" s="18"/>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="14" t="n">
+        <v>15</v>
+      </c>
       <c r="B19" s="15" t="s">
         <v>86</v>
       </c>
       <c r="C19" s="15" t="s">
         <v>87</v>
       </c>
-      <c r="D19" s="18" t="s">
+      <c r="D19" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="20"/>
-      <c r="F19" s="18"/>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E19" s="18"/>
+      <c r="F19" s="24"/>
+    </row>
+    <row r="20" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="14" t="n">
+        <v>16</v>
+      </c>
       <c r="B20" s="15" t="s">
         <v>88</v>
       </c>
       <c r="C20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="16" t="s">
+      <c r="D20" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="17" t="n">
+      <c r="E20" s="21" t="n">
         <v>7</v>
       </c>
-      <c r="F20" s="18"/>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F20" s="24"/>
+    </row>
+    <row r="21" s="19" customFormat="true" ht="200.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="14" t="n">
+        <v>17</v>
+      </c>
       <c r="B21" s="15" t="s">
         <v>90</v>
       </c>
       <c r="C21" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="16" t="s">
+      <c r="D21" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="17" t="n">
+      <c r="E21" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="F21" s="18"/>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F21" s="24"/>
+    </row>
+    <row r="22" s="19" customFormat="true" ht="200.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="14" t="n">
+        <v>18</v>
+      </c>
       <c r="B22" s="15" t="s">
         <v>92</v>
       </c>
       <c r="C22" s="15" t="s">
         <v>93</v>
       </c>
-      <c r="D22" s="18" t="s">
+      <c r="D22" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="20"/>
-      <c r="F22" s="18"/>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="18"/>
+      <c r="F22" s="24"/>
+    </row>
+    <row r="23" s="19" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="14" t="n">
+        <v>19</v>
+      </c>
       <c r="B23" s="15" t="s">
         <v>94</v>
       </c>
       <c r="C23" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="16" t="s">
+      <c r="D23" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="17" t="n">
+      <c r="E23" s="21" t="n">
         <v>9</v>
       </c>
-      <c r="F23" s="18"/>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F23" s="24"/>
+    </row>
+    <row r="24" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="14" t="n">
+        <v>20</v>
+      </c>
       <c r="B24" s="15" t="s">
         <v>96</v>
       </c>
       <c r="C24" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="16" t="s">
+      <c r="D24" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="17" t="n">
+      <c r="E24" s="21" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" s="19" customFormat="true" ht="162.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="14" t="n">
+        <v>21</v>
+      </c>
       <c r="B25" s="15" t="s">
         <v>98</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="20" t="s">
+      <c r="D25" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="20"/>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="14" t="n">
+        <v>22</v>
+      </c>
       <c r="B26" s="15" t="s">
         <v>100</v>
       </c>
       <c r="C26" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="20" t="s">
+      <c r="D26" s="18" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="20"/>
-      <c r="F26" s="18"/>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E26" s="18"/>
+      <c r="F26" s="24"/>
+    </row>
+    <row r="27" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="14" t="n">
+        <v>23</v>
+      </c>
       <c r="B27" s="15" t="s">
         <v>102</v>
       </c>
       <c r="C27" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="16" t="s">
+      <c r="D27" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="17" t="n">
+      <c r="E27" s="21" t="n">
         <v>11</v>
       </c>
-      <c r="F27" s="18"/>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F27" s="24"/>
+    </row>
+    <row r="28" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="14" t="n">
+        <v>24</v>
+      </c>
       <c r="B28" s="15" t="s">
         <v>104</v>
       </c>
       <c r="C28" s="15" t="s">
         <v>105</v>
       </c>
-      <c r="D28" s="18" t="s">
+      <c r="D28" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="20"/>
-      <c r="F28" s="18"/>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E28" s="18"/>
+      <c r="F28" s="24"/>
+    </row>
+    <row r="29" s="19" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="14" t="n">
+        <v>25</v>
+      </c>
       <c r="B29" s="15" t="s">
         <v>106</v>
       </c>
       <c r="C29" s="15" t="s">
         <v>107</v>
       </c>
-      <c r="D29" s="18" t="s">
+      <c r="D29" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="20"/>
-      <c r="F29" s="18"/>
-    </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E29" s="18"/>
+      <c r="F29" s="24"/>
+    </row>
+    <row r="30" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="14" t="n">
+        <v>26</v>
+      </c>
       <c r="B30" s="15" t="s">
         <v>108</v>
       </c>
       <c r="C30" s="15" t="s">
         <v>109</v>
       </c>
-      <c r="D30" s="18" t="s">
+      <c r="D30" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="20"/>
-      <c r="F30" s="18"/>
-    </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E30" s="18"/>
+      <c r="F30" s="24"/>
+    </row>
+    <row r="31" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="14" t="n">
+        <v>27</v>
+      </c>
       <c r="B31" s="15" t="s">
         <v>110</v>
       </c>
       <c r="C31" s="15" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="18" t="s">
+      <c r="D31" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="20"/>
-      <c r="F31" s="18"/>
-    </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E31" s="18"/>
+      <c r="F31" s="24"/>
+    </row>
+    <row r="32" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="14" t="n">
+        <v>28</v>
+      </c>
       <c r="B32" s="15" t="s">
         <v>112</v>
       </c>
       <c r="C32" s="15" t="s">
         <v>113</v>
       </c>
-      <c r="D32" s="18" t="s">
+      <c r="D32" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="20"/>
-      <c r="F32" s="18"/>
-    </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E32" s="18"/>
+      <c r="F32" s="24"/>
+    </row>
+    <row r="33" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="14" t="n">
+        <v>29</v>
+      </c>
       <c r="B33" s="15" t="s">
         <v>114</v>
       </c>
       <c r="C33" s="15" t="s">
         <v>115</v>
       </c>
-      <c r="D33" s="18" t="s">
+      <c r="D33" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="20"/>
-      <c r="F33" s="18"/>
-    </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E33" s="18"/>
+      <c r="F33" s="24"/>
+    </row>
+    <row r="34" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="14" t="n">
+        <v>30</v>
+      </c>
       <c r="B34" s="15" t="s">
         <v>116</v>
       </c>
       <c r="C34" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="16" t="s">
+      <c r="D34" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="17" t="n">
+      <c r="E34" s="21" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="14" t="n">
+        <v>31</v>
+      </c>
       <c r="B35" s="15" t="s">
         <v>118</v>
       </c>
       <c r="C35" s="15" t="s">
         <v>119</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E35" s="20"/>
-      <c r="F35" s="18"/>
-    </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E35" s="18"/>
+      <c r="F35" s="24"/>
+    </row>
+    <row r="36" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="14" t="n">
+        <v>32</v>
+      </c>
       <c r="B36" s="15" t="s">
         <v>120</v>
       </c>
       <c r="C36" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="20"/>
-      <c r="F36" s="18"/>
-    </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E36" s="18"/>
+      <c r="F36" s="24"/>
+    </row>
+    <row r="37" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="14" t="n">
+        <v>33</v>
+      </c>
       <c r="B37" s="15" t="s">
         <v>122</v>
       </c>
       <c r="C37" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D37" s="16" t="s">
+      <c r="D37" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="17" t="n">
+      <c r="E37" s="21" t="n">
         <v>13</v>
       </c>
-      <c r="F37" s="18"/>
-    </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F37" s="24"/>
+    </row>
+    <row r="38" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="14" t="n">
+        <v>34</v>
+      </c>
       <c r="B38" s="15" t="s">
         <v>124</v>
       </c>
       <c r="C38" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D38" s="16" t="s">
+      <c r="D38" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="17" t="n">
+      <c r="E38" s="21" t="n">
         <v>14</v>
       </c>
-      <c r="F38" s="18"/>
-    </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="21" t="s">
+      <c r="F38" s="24"/>
+    </row>
+    <row r="39" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="14" t="n">
+        <v>35</v>
+      </c>
+      <c r="B39" s="25" t="s">
         <v>126</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D39" s="16" t="s">
+      <c r="D39" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="17" t="n">
+      <c r="E39" s="21" t="n">
         <v>15</v>
       </c>
-      <c r="F39" s="18"/>
-    </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F39" s="24"/>
+    </row>
+    <row r="40" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="14" t="n">
+        <v>36</v>
+      </c>
       <c r="B40" s="15" t="s">
         <v>128</v>
       </c>
       <c r="C40" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="D40" s="16" t="s">
+      <c r="D40" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E40" s="17" t="n">
+      <c r="E40" s="21" t="n">
         <v>16</v>
       </c>
-      <c r="F40" s="18"/>
-    </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F40" s="24"/>
+    </row>
+    <row r="41" s="19" customFormat="true" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="14" t="n">
+        <v>37</v>
+      </c>
       <c r="B41" s="15" t="s">
         <v>130</v>
       </c>
       <c r="C41" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="D41" s="18" t="s">
+      <c r="D41" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E41" s="22"/>
-      <c r="F41" s="18"/>
-    </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E41" s="23"/>
+      <c r="F41" s="24"/>
+    </row>
+    <row r="42" s="19" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="14" t="n">
+        <v>38</v>
+      </c>
       <c r="B42" s="15" t="s">
         <v>132</v>
       </c>
       <c r="C42" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="D42" s="18" t="s">
+      <c r="D42" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="20"/>
-      <c r="F42" s="18"/>
-    </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E42" s="18"/>
+      <c r="F42" s="24"/>
+    </row>
+    <row r="43" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="14" t="n">
+        <v>39</v>
+      </c>
       <c r="B43" s="15" t="s">
         <v>134</v>
       </c>
       <c r="C43" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="D43" s="18" t="s">
+      <c r="D43" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="20"/>
-      <c r="F43" s="18"/>
-    </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E43" s="18"/>
+      <c r="F43" s="24"/>
+    </row>
+    <row r="44" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="14" t="n">
+        <v>40</v>
+      </c>
       <c r="B44" s="15" t="s">
         <v>136</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="D44" s="18" t="s">
+      <c r="D44" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="8"/>
-    </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E44" s="18"/>
+    </row>
+    <row r="45" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="14" t="n">
+        <v>41</v>
+      </c>
       <c r="B45" s="15" t="s">
         <v>138</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="D45" s="18" t="s">
+      <c r="D45" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E45" s="8"/>
-    </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E45" s="18"/>
+    </row>
+    <row r="46" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="14" t="n">
+        <v>42</v>
+      </c>
       <c r="B46" s="15" t="s">
         <v>140</v>
       </c>
       <c r="C46" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="D46" s="18" t="s">
+      <c r="D46" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E46" s="20"/>
-      <c r="F46" s="18"/>
-    </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E46" s="18"/>
+      <c r="F46" s="24"/>
+    </row>
+    <row r="47" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="14" t="n">
+        <v>43</v>
+      </c>
       <c r="B47" s="15" t="s">
         <v>142</v>
       </c>
       <c r="C47" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D47" s="16" t="s">
+      <c r="D47" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E47" s="17" t="n">
+      <c r="E47" s="21" t="n">
         <v>17</v>
       </c>
-      <c r="F47" s="18"/>
-    </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F47" s="24"/>
+    </row>
+    <row r="48" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="14" t="n">
+        <v>44</v>
+      </c>
       <c r="B48" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="C48" s="23" t="s">
+      <c r="C48" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="16" t="s">
+      <c r="D48" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E48" s="17" t="n">
+      <c r="E48" s="21" t="n">
         <v>18</v>
       </c>
-      <c r="F48" s="18"/>
-    </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F48" s="24"/>
+    </row>
+    <row r="49" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="14" t="n">
+        <v>45</v>
+      </c>
       <c r="B49" s="15" t="s">
         <v>146</v>
       </c>
       <c r="C49" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="D49" s="16" t="s">
+      <c r="D49" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E49" s="17" t="n">
+      <c r="E49" s="21" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="14" t="n">
+        <v>46</v>
+      </c>
       <c r="B50" s="15" t="s">
         <v>148</v>
       </c>
       <c r="C50" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D50" s="16" t="s">
+      <c r="D50" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E50" s="17" t="n">
+      <c r="E50" s="21" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A51" s="14" t="n">
+        <v>47</v>
+      </c>
       <c r="B51" s="15" t="s">
         <v>150</v>
       </c>
       <c r="C51" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D51" s="16" t="s">
+      <c r="D51" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E51" s="17" t="n">
+      <c r="E51" s="21" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="14" t="n">
+        <v>48</v>
+      </c>
       <c r="B52" s="15" t="s">
         <v>152</v>
       </c>
       <c r="C52" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="D52" s="16" t="s">
+      <c r="D52" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="17" t="n">
+      <c r="E52" s="21" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A53" s="14" t="n">
+        <v>49</v>
+      </c>
       <c r="B53" s="15" t="s">
         <v>154</v>
       </c>
       <c r="C53" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="D53" s="18" t="s">
+      <c r="D53" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E53" s="20"/>
-    </row>
-    <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E53" s="18"/>
+    </row>
+    <row r="54" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A54" s="14" t="n">
+        <v>50</v>
+      </c>
       <c r="B54" s="15" t="s">
         <v>156</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="15" t="s">
         <v>157</v>
       </c>
-      <c r="D54" s="18" t="s">
+      <c r="D54" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E54" s="8"/>
-    </row>
-    <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E54" s="18"/>
+    </row>
+    <row r="55" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A55" s="14" t="n">
+        <v>51</v>
+      </c>
       <c r="B55" s="15" t="s">
         <v>158</v>
       </c>
-      <c r="C55" s="6" t="s">
+      <c r="C55" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="D55" s="16" t="s">
+      <c r="D55" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="17" t="n">
+      <c r="E55" s="21" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A56" s="14" t="n">
+        <v>52</v>
+      </c>
       <c r="B56" s="15" t="s">
         <v>160</v>
       </c>
       <c r="C56" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="D56" s="16" t="s">
+      <c r="D56" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="17" t="n">
+      <c r="E56" s="21" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="14" t="n">
+        <v>53</v>
+      </c>
       <c r="B57" s="15" t="s">
         <v>162</v>
       </c>
       <c r="C57" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="D57" s="16" t="s">
+      <c r="D57" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E57" s="17" t="n">
+      <c r="E57" s="21" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="58" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A58" s="14" t="n">
+        <v>54</v>
+      </c>
       <c r="B58" s="15" t="s">
         <v>164</v>
       </c>
       <c r="C58" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="D58" s="16" t="s">
+      <c r="D58" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E58" s="17" t="n">
+      <c r="E58" s="21" t="n">
         <v>26</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="59" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="14" t="n">
+        <v>55</v>
+      </c>
       <c r="B59" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="D59" s="16" t="s">
+      <c r="D59" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E59" s="17" t="n">
+      <c r="E59" s="21" t="n">
         <v>27</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="60" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A60" s="14" t="n">
+        <v>56</v>
+      </c>
       <c r="B60" s="15" t="s">
         <v>168</v>
       </c>
       <c r="C60" s="15" t="s">
         <v>169</v>
       </c>
-      <c r="D60" s="18" t="s">
+      <c r="D60" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E60" s="20"/>
-    </row>
-    <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="18"/>
+    </row>
+    <row r="61" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A61" s="14" t="n">
+        <v>57</v>
+      </c>
       <c r="B61" s="15" t="s">
         <v>170</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="D61" s="16" t="s">
+      <c r="D61" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E61" s="17" t="n">
+      <c r="E61" s="21" t="n">
         <v>28</v>
       </c>
     </row>
-    <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="62" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A62" s="14" t="n">
+        <v>58</v>
+      </c>
       <c r="B62" s="15" t="s">
         <v>172</v>
       </c>
       <c r="C62" s="15" t="s">
         <v>173</v>
       </c>
-      <c r="D62" s="18" t="s">
+      <c r="D62" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="20"/>
-    </row>
-    <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E62" s="18"/>
+    </row>
+    <row r="63" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="14" t="n">
+        <v>59</v>
+      </c>
       <c r="B63" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="D63" s="16" t="s">
+      <c r="D63" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E63" s="17" t="n">
+      <c r="E63" s="21" t="n">
         <v>29</v>
       </c>
     </row>
-    <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="64" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A64" s="14" t="n">
+        <v>60</v>
+      </c>
       <c r="B64" s="15" t="s">
         <v>176</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="D64" s="16" t="s">
+      <c r="D64" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E64" s="17" t="n">
+      <c r="E64" s="21" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="65" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A65" s="14" t="n">
+        <v>61</v>
+      </c>
       <c r="B65" s="15" t="s">
         <v>178</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="D65" s="16" t="s">
+      <c r="D65" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E65" s="17" t="n">
+      <c r="E65" s="21" t="n">
         <v>31</v>
       </c>
     </row>
-    <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="66" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="14" t="n">
+        <v>62</v>
+      </c>
       <c r="B66" s="15" t="s">
         <v>180</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="D66" s="16" t="s">
+      <c r="D66" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E66" s="17" t="n">
+      <c r="E66" s="21" t="n">
         <v>32</v>
       </c>
     </row>
-    <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="67" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A67" s="14" t="n">
+        <v>63</v>
+      </c>
       <c r="B67" s="15" t="s">
         <v>182</v>
       </c>
-      <c r="C67" s="6" t="s">
+      <c r="C67" s="15" t="s">
         <v>183</v>
       </c>
-      <c r="D67" s="18" t="s">
+      <c r="D67" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E67" s="8"/>
-    </row>
-    <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E67" s="18"/>
+    </row>
+    <row r="68" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="14" t="n">
+        <v>64</v>
+      </c>
       <c r="B68" s="15" t="s">
         <v>184</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="15" t="s">
         <v>185</v>
       </c>
-      <c r="D68" s="18" t="s">
+      <c r="D68" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E68" s="8"/>
-    </row>
-    <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E68" s="18"/>
+    </row>
+    <row r="69" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A69" s="14" t="n">
+        <v>65</v>
+      </c>
       <c r="B69" s="15" t="s">
         <v>186</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="D69" s="16" t="s">
+      <c r="D69" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E69" s="17" t="n">
+      <c r="E69" s="21" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="70" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="14" t="n">
+        <v>66</v>
+      </c>
       <c r="B70" s="15" t="s">
         <v>188</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="D70" s="18" t="s">
+      <c r="D70" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E70" s="8"/>
-    </row>
-    <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E70" s="18"/>
+    </row>
+    <row r="71" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A71" s="14" t="n">
+        <v>67</v>
+      </c>
       <c r="B71" s="15" t="s">
         <v>190</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="D71" s="16" t="s">
+      <c r="D71" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E71" s="17" t="n">
+      <c r="E71" s="21" t="n">
         <v>34</v>
       </c>
     </row>
-    <row r="72" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="72" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A72" s="14" t="n">
+        <v>68</v>
+      </c>
       <c r="B72" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="D72" s="16" t="s">
+      <c r="D72" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E72" s="17" t="n">
+      <c r="E72" s="21" t="n">
         <v>35</v>
       </c>
     </row>
-    <row r="73" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="73" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="14" t="n">
+        <v>69</v>
+      </c>
       <c r="B73" s="15" t="s">
         <v>194</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C73" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="D73" s="18" t="s">
+      <c r="D73" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E73" s="8"/>
-    </row>
-    <row r="74" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E73" s="18"/>
+    </row>
+    <row r="74" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A74" s="14" t="n">
+        <v>70</v>
+      </c>
       <c r="B74" s="15" t="s">
         <v>196</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C74" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="D74" s="16" t="s">
+      <c r="D74" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E74" s="17" t="n">
+      <c r="E74" s="21" t="n">
         <v>36</v>
       </c>
     </row>
-    <row r="75" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="75" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="14" t="n">
+        <v>71</v>
+      </c>
       <c r="B75" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="C75" s="6" t="s">
+      <c r="C75" s="15" t="s">
         <v>199</v>
       </c>
-      <c r="D75" s="18" t="s">
+      <c r="D75" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E75" s="8"/>
-    </row>
-    <row r="76" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E75" s="18"/>
+    </row>
+    <row r="76" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A76" s="14" t="n">
+        <v>72</v>
+      </c>
       <c r="B76" s="15" t="s">
         <v>200</v>
       </c>
       <c r="C76" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="D76" s="16" t="s">
+      <c r="D76" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E76" s="17" t="n">
+      <c r="E76" s="21" t="n">
         <v>37</v>
       </c>
     </row>
-    <row r="77" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="77" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="14" t="n">
+        <v>73</v>
+      </c>
       <c r="B77" s="15" t="s">
         <v>202</v>
       </c>
-      <c r="C77" s="6" t="s">
+      <c r="C77" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="D77" s="16" t="s">
+      <c r="D77" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E77" s="17" t="n">
+      <c r="E77" s="21" t="n">
         <v>38</v>
       </c>
     </row>
-    <row r="78" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="78" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A78" s="14" t="n">
+        <v>74</v>
+      </c>
       <c r="B78" s="15" t="s">
         <v>204</v>
       </c>
       <c r="C78" s="15" t="s">
         <v>205</v>
       </c>
-      <c r="D78" s="18" t="s">
+      <c r="D78" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E78" s="20"/>
-      <c r="F78" s="18"/>
-    </row>
-    <row r="79" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E78" s="18"/>
+      <c r="F78" s="24"/>
+    </row>
+    <row r="79" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="14" t="n">
+        <v>75</v>
+      </c>
       <c r="B79" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C79" s="18"/>
-      <c r="D79" s="18" t="s">
+      <c r="C79" s="17"/>
+      <c r="D79" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E79" s="20"/>
-      <c r="F79" s="18"/>
-    </row>
-    <row r="80" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E79" s="18"/>
+      <c r="F79" s="24"/>
+    </row>
+    <row r="80" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A80" s="14" t="n">
+        <v>76</v>
+      </c>
       <c r="B80" s="15" t="s">
         <v>207</v>
       </c>
       <c r="C80" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="D80" s="16" t="s">
+      <c r="D80" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E80" s="17" t="n">
+      <c r="E80" s="21" t="n">
         <v>39</v>
       </c>
-      <c r="F80" s="23" t="s">
+      <c r="F80" s="27" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="81" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="81" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A81" s="14" t="n">
+        <v>77</v>
+      </c>
       <c r="B81" s="15" t="s">
         <v>210</v>
       </c>
-      <c r="C81" s="6" t="s">
+      <c r="C81" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="D81" s="16" t="s">
+      <c r="D81" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E81" s="17" t="n">
+      <c r="E81" s="21" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="82" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="82" s="19" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A82" s="14" t="n">
+        <v>78</v>
+      </c>
       <c r="B82" s="15" t="s">
         <v>212</v>
       </c>
       <c r="C82" s="15" t="s">
         <v>213</v>
       </c>
-      <c r="D82" s="18" t="s">
+      <c r="D82" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E82" s="20"/>
-    </row>
-    <row r="83" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E82" s="18"/>
+    </row>
+    <row r="83" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="14" t="n">
+        <v>79</v>
+      </c>
       <c r="B83" s="15" t="s">
         <v>214</v>
       </c>
-      <c r="C83" s="6" t="s">
+      <c r="C83" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="D83" s="16" t="s">
+      <c r="D83" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E83" s="17" t="n">
+      <c r="E83" s="21" t="n">
         <v>41</v>
       </c>
     </row>
-    <row r="84" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="84" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A84" s="14" t="n">
+        <v>80</v>
+      </c>
       <c r="B84" s="15" t="s">
         <v>216</v>
       </c>
       <c r="C84" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="D84" s="16" t="s">
+      <c r="D84" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E84" s="17" t="n">
+      <c r="E84" s="21" t="n">
         <v>42</v>
       </c>
     </row>
-    <row r="85" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="85" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="14" t="n">
+        <v>81</v>
+      </c>
       <c r="B85" s="15" t="s">
         <v>218</v>
       </c>
       <c r="C85" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="D85" s="16" t="s">
+      <c r="D85" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E85" s="17" t="n">
+      <c r="E85" s="21" t="n">
         <v>43</v>
       </c>
     </row>
-    <row r="86" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="86" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A86" s="14" t="n">
+        <v>82</v>
+      </c>
       <c r="B86" s="15" t="s">
         <v>220</v>
       </c>
       <c r="C86" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="D86" s="16" t="s">
+      <c r="D86" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E86" s="17" t="n">
+      <c r="E86" s="21" t="n">
         <v>44</v>
       </c>
     </row>
-    <row r="87" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="87" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A87" s="14" t="n">
+        <v>83</v>
+      </c>
       <c r="B87" s="15" t="s">
         <v>222</v>
       </c>
       <c r="C87" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="D87" s="16" t="s">
+      <c r="D87" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E87" s="17" t="n">
+      <c r="E87" s="21" t="n">
         <v>45</v>
       </c>
     </row>
-    <row r="88" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="88" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="14" t="n">
+        <v>84</v>
+      </c>
       <c r="B88" s="15" t="s">
         <v>224</v>
       </c>
       <c r="C88" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="D88" s="16" t="s">
+      <c r="D88" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E88" s="17" t="n">
+      <c r="E88" s="21" t="n">
         <v>46</v>
       </c>
     </row>
-    <row r="89" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="89" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A89" s="14" t="n">
+        <v>85</v>
+      </c>
       <c r="B89" s="15" t="s">
         <v>226</v>
       </c>
       <c r="C89" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="D89" s="16" t="s">
+      <c r="D89" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E89" s="17" t="n">
+      <c r="E89" s="21" t="n">
         <v>47</v>
       </c>
     </row>
-    <row r="90" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="90" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A90" s="14" t="n">
+        <v>86</v>
+      </c>
       <c r="B90" s="15" t="s">
         <v>228</v>
       </c>
       <c r="C90" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="D90" s="16" t="s">
+      <c r="D90" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E90" s="17" t="n">
+      <c r="E90" s="21" t="n">
         <v>48</v>
       </c>
     </row>
-    <row r="91" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="91" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A91" s="14" t="n">
+        <v>87</v>
+      </c>
       <c r="B91" s="15" t="s">
         <v>230</v>
       </c>
       <c r="C91" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="D91" s="16" t="s">
+      <c r="D91" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E91" s="17" t="n">
+      <c r="E91" s="21" t="n">
         <v>49</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="6"/>
-      <c r="C94" s="18"/>
+      <c r="C94" s="24"/>
       <c r="E94" s="8"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="6"/>
-      <c r="C95" s="18"/>
+      <c r="C95" s="24"/>
       <c r="E95" s="8"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="6"/>
-      <c r="C96" s="18"/>
+      <c r="C96" s="24"/>
       <c r="E96" s="8"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="6"/>
-      <c r="C97" s="18"/>
+      <c r="C97" s="24"/>
       <c r="E97" s="8"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="6"/>
-      <c r="C98" s="18"/>
+      <c r="C98" s="24"/>
       <c r="E98" s="8"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="6"/>
-      <c r="C99" s="18"/>
+      <c r="C99" s="24"/>
       <c r="E99" s="8"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10404,7 +10694,7 @@
       <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.640625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.38"/>
@@ -10412,1623 +10702,1623 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="28" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="25" t="s">
+      <c r="B1" s="29" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="26" t="s">
+      <c r="C1" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="25" t="s">
+      <c r="D1" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="E1" s="25" t="s">
+      <c r="E1" s="29" t="s">
         <v>236</v>
       </c>
-      <c r="F1" s="26" t="s">
+      <c r="F1" s="30" t="s">
         <v>237</v>
       </c>
-      <c r="G1" s="26" t="s">
+      <c r="G1" s="30" t="s">
         <v>238</v>
       </c>
-      <c r="H1" s="26" t="s">
+      <c r="H1" s="30" t="s">
         <v>239</v>
       </c>
-      <c r="I1" s="26" t="s">
+      <c r="I1" s="30" t="s">
         <v>240</v>
       </c>
-      <c r="J1" s="26" t="s">
+      <c r="J1" s="30" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="18" t="n">
+      <c r="A2" s="24" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="22" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="22" t="s">
         <v>242</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="22" t="s">
         <v>245</v>
       </c>
-      <c r="G2" s="18" t="s">
+      <c r="G2" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="18" t="s">
+      <c r="H2" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J2" s="23" t="s">
+      <c r="J2" s="27" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="18" t="n">
+      <c r="A3" s="24" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D3" s="15" t="s">
+      <c r="D3" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="E3" s="22" t="s">
         <v>250</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="22" t="s">
         <v>252</v>
       </c>
-      <c r="G3" s="18" t="s">
+      <c r="G3" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H3" s="18" t="s">
+      <c r="H3" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="I3" s="15" t="s">
+      <c r="I3" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J3" s="23" t="s">
+      <c r="J3" s="27" t="s">
         <v>253</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="18" t="n">
+      <c r="A4" s="24" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="22" t="s">
         <v>254</v>
       </c>
-      <c r="C4" s="23" t="s">
+      <c r="C4" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D4" s="15" t="s">
+      <c r="D4" s="22" t="s">
         <v>255</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="E4" s="22" t="s">
         <v>254</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="22" t="s">
         <v>256</v>
       </c>
-      <c r="G4" s="18" t="s">
+      <c r="G4" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H4" s="18" t="s">
+      <c r="H4" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="I4" s="15" t="s">
+      <c r="I4" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J4" s="23" t="s">
+      <c r="J4" s="27" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="18" t="n">
+      <c r="A5" s="24" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="22" t="s">
         <v>258</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="D5" s="22" t="s">
         <v>259</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="22" t="s">
         <v>258</v>
       </c>
-      <c r="F5" s="15" t="s">
+      <c r="F5" s="22" t="s">
         <v>260</v>
       </c>
-      <c r="G5" s="18" t="s">
+      <c r="G5" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H5" s="18" t="s">
+      <c r="H5" s="24" t="s">
         <v>247</v>
       </c>
-      <c r="I5" s="15" t="s">
+      <c r="I5" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="23" t="s">
+      <c r="J5" s="27" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="18" t="n">
+      <c r="A6" s="24" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="15" t="s">
+      <c r="B6" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="C6" s="23" t="s">
+      <c r="C6" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D6" s="15" t="s">
+      <c r="D6" s="22" t="s">
         <v>263</v>
       </c>
-      <c r="E6" s="15" t="s">
+      <c r="E6" s="22" t="s">
         <v>262</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="22" t="s">
         <v>264</v>
       </c>
-      <c r="G6" s="18" t="s">
+      <c r="G6" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H6" s="18" t="s">
+      <c r="H6" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I6" s="15" t="s">
+      <c r="I6" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J6" s="23" t="s">
+      <c r="J6" s="27" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="18" t="n">
+      <c r="A7" s="24" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="C7" s="23" t="s">
+      <c r="C7" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D7" s="15" t="s">
+      <c r="D7" s="22" t="s">
         <v>268</v>
       </c>
-      <c r="E7" s="15" t="s">
+      <c r="E7" s="22" t="s">
         <v>267</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="22" t="s">
         <v>269</v>
       </c>
-      <c r="G7" s="18" t="s">
+      <c r="G7" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H7" s="18" t="s">
+      <c r="H7" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I7" s="15" t="s">
+      <c r="I7" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="27" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="18" t="n">
+      <c r="A8" s="24" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="22" t="s">
         <v>271</v>
       </c>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="15" t="s">
+      <c r="E8" s="22" t="s">
         <v>273</v>
       </c>
-      <c r="F8" s="15" t="s">
+      <c r="F8" s="22" t="s">
         <v>274</v>
       </c>
-      <c r="G8" s="18" t="s">
+      <c r="G8" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H8" s="18" t="s">
+      <c r="H8" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I8" s="15" t="s">
+      <c r="I8" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J8" s="23" t="s">
+      <c r="J8" s="27" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="18" t="n">
+      <c r="A9" s="24" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="22" t="s">
         <v>276</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>277</v>
       </c>
-      <c r="E9" s="15" t="s">
+      <c r="E9" s="22" t="s">
         <v>276</v>
       </c>
-      <c r="F9" s="15" t="s">
+      <c r="F9" s="22" t="s">
         <v>278</v>
       </c>
-      <c r="G9" s="18" t="s">
+      <c r="G9" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H9" s="18" t="s">
+      <c r="H9" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I9" s="15" t="s">
+      <c r="I9" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J9" s="23" t="s">
+      <c r="J9" s="27" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="18" t="n">
+      <c r="A10" s="24" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="C10" s="23" t="s">
+      <c r="C10" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>281</v>
       </c>
-      <c r="E10" s="15" t="s">
+      <c r="E10" s="22" t="s">
         <v>280</v>
       </c>
-      <c r="F10" s="15" t="s">
+      <c r="F10" s="22" t="s">
         <v>282</v>
       </c>
-      <c r="G10" s="18" t="s">
+      <c r="G10" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H10" s="18" t="s">
+      <c r="H10" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I10" s="15" t="s">
+      <c r="I10" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J10" s="23" t="s">
+      <c r="J10" s="27" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="18" t="n">
+      <c r="A11" s="24" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>285</v>
       </c>
-      <c r="E11" s="15" t="s">
+      <c r="E11" s="22" t="s">
         <v>284</v>
       </c>
-      <c r="F11" s="15" t="s">
+      <c r="F11" s="22" t="s">
         <v>286</v>
       </c>
-      <c r="G11" s="18" t="s">
+      <c r="G11" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H11" s="18" t="s">
+      <c r="H11" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I11" s="15" t="s">
+      <c r="I11" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="27" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="18" t="n">
+      <c r="A12" s="24" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="C12" s="23" t="s">
+      <c r="C12" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>289</v>
       </c>
-      <c r="E12" s="15" t="s">
+      <c r="E12" s="22" t="s">
         <v>288</v>
       </c>
-      <c r="F12" s="15" t="s">
+      <c r="F12" s="22" t="s">
         <v>290</v>
       </c>
-      <c r="G12" s="18" t="s">
+      <c r="G12" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H12" s="18" t="s">
+      <c r="H12" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I12" s="15" t="s">
+      <c r="I12" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="27" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="18" t="n">
+      <c r="A13" s="24" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="C13" s="23" t="s">
+      <c r="C13" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="22" t="s">
         <v>293</v>
       </c>
-      <c r="E13" s="15" t="s">
+      <c r="E13" s="22" t="s">
         <v>292</v>
       </c>
-      <c r="F13" s="15" t="s">
+      <c r="F13" s="22" t="s">
         <v>294</v>
       </c>
-      <c r="G13" s="18" t="s">
+      <c r="G13" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H13" s="18" t="s">
+      <c r="H13" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I13" s="15" t="s">
+      <c r="I13" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J13" s="23" t="s">
+      <c r="J13" s="27" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="18" t="n">
+      <c r="A14" s="24" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="C14" s="23" t="s">
+      <c r="C14" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D14" s="15" t="s">
+      <c r="D14" s="22" t="s">
         <v>297</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="22" t="s">
         <v>296</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="22" t="s">
         <v>298</v>
       </c>
-      <c r="G14" s="18" t="s">
+      <c r="G14" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H14" s="18" t="s">
+      <c r="H14" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I14" s="15" t="s">
+      <c r="I14" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J14" s="23" t="s">
+      <c r="J14" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="18" t="n">
+      <c r="A15" s="24" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D15" s="15" t="s">
+      <c r="D15" s="22" t="s">
         <v>301</v>
       </c>
-      <c r="E15" s="15" t="s">
+      <c r="E15" s="22" t="s">
         <v>300</v>
       </c>
-      <c r="F15" s="15" t="s">
+      <c r="F15" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="G15" s="18" t="s">
+      <c r="G15" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H15" s="18" t="s">
+      <c r="H15" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I15" s="15" t="s">
+      <c r="I15" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="J15" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K15" s="18"/>
+      <c r="K15" s="24"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="18" t="n">
+      <c r="A16" s="24" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="C16" s="23" t="s">
+      <c r="C16" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D16" s="15" t="s">
+      <c r="D16" s="22" t="s">
         <v>304</v>
       </c>
-      <c r="E16" s="15" t="s">
+      <c r="E16" s="22" t="s">
         <v>303</v>
       </c>
-      <c r="F16" s="15" t="s">
+      <c r="F16" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="G16" s="18" t="s">
+      <c r="G16" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H16" s="18" t="s">
+      <c r="H16" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I16" s="15" t="s">
+      <c r="I16" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="18" t="n">
+      <c r="A17" s="24" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="22" t="s">
         <v>305</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D17" s="15" t="s">
+      <c r="D17" s="22" t="s">
         <v>306</v>
       </c>
-      <c r="E17" s="15" t="s">
+      <c r="E17" s="22" t="s">
         <v>305</v>
       </c>
-      <c r="F17" s="15" t="s">
+      <c r="F17" s="22" t="s">
         <v>302</v>
       </c>
-      <c r="G17" s="18" t="s">
+      <c r="G17" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H17" s="18" t="s">
+      <c r="H17" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I17" s="15" t="s">
+      <c r="I17" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J17" s="23" t="s">
+      <c r="J17" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="18" t="n">
+      <c r="A18" s="24" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="22" t="s">
         <v>307</v>
       </c>
-      <c r="C18" s="23" t="s">
+      <c r="C18" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="22" t="s">
         <v>308</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="22" t="s">
         <v>307</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="22" t="s">
         <v>309</v>
       </c>
-      <c r="G18" s="18" t="s">
+      <c r="G18" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H18" s="18" t="s">
+      <c r="H18" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I18" s="15" t="s">
+      <c r="I18" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J18" s="23" t="s">
+      <c r="J18" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="18" t="n">
+      <c r="A19" s="24" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="C19" s="23" t="s">
+      <c r="C19" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="22" t="s">
         <v>311</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="22" t="s">
         <v>310</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="22" t="s">
         <v>312</v>
       </c>
-      <c r="G19" s="18" t="s">
+      <c r="G19" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H19" s="18" t="s">
+      <c r="H19" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I19" s="15" t="s">
+      <c r="I19" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J19" s="23" t="s">
+      <c r="J19" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="18" t="n">
+      <c r="A20" s="24" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="C20" s="23" t="s">
+      <c r="C20" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="22" t="s">
         <v>314</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="22" t="s">
         <v>312</v>
       </c>
-      <c r="G20" s="18" t="s">
+      <c r="G20" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H20" s="18" t="s">
+      <c r="H20" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I20" s="15" t="s">
+      <c r="I20" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J20" s="23" t="s">
+      <c r="J20" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="18" t="n">
+      <c r="A21" s="24" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="C21" s="23" t="s">
+      <c r="C21" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="22" t="s">
         <v>316</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="22" t="s">
         <v>317</v>
       </c>
-      <c r="G21" s="18" t="s">
+      <c r="G21" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H21" s="18" t="s">
+      <c r="H21" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I21" s="15" t="s">
+      <c r="I21" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J21" s="23" t="s">
+      <c r="J21" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="18" t="n">
+      <c r="A22" s="24" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="22" t="s">
         <v>318</v>
       </c>
-      <c r="C22" s="23" t="s">
+      <c r="C22" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D22" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="22" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="22" t="s">
         <v>312</v>
       </c>
-      <c r="G22" s="18" t="s">
+      <c r="G22" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H22" s="18" t="s">
+      <c r="H22" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I22" s="15" t="s">
+      <c r="I22" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J22" s="23" t="s">
+      <c r="J22" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="18" t="n">
+      <c r="A23" s="24" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="C23" s="23" t="s">
+      <c r="C23" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D23" s="6" t="s">
         <v>322</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="22" t="s">
         <v>321</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G23" s="18" t="s">
+      <c r="G23" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H23" s="18" t="s">
+      <c r="H23" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I23" s="15" t="s">
+      <c r="I23" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J23" s="23" t="s">
+      <c r="J23" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="18" t="n">
+      <c r="A24" s="24" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="22" t="s">
         <v>324</v>
       </c>
-      <c r="C24" s="23" t="s">
+      <c r="C24" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D24" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="E24" s="15" t="s">
+      <c r="E24" s="22" t="s">
         <v>324</v>
       </c>
-      <c r="F24" s="15" t="s">
+      <c r="F24" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G24" s="18" t="s">
+      <c r="G24" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I24" s="15" t="s">
+      <c r="I24" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J24" s="23" t="s">
+      <c r="J24" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="18" t="n">
+      <c r="A25" s="24" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="22" t="s">
         <v>326</v>
       </c>
-      <c r="C25" s="23" t="s">
+      <c r="C25" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>327</v>
       </c>
-      <c r="E25" s="15" t="s">
+      <c r="E25" s="22" t="s">
         <v>326</v>
       </c>
-      <c r="F25" s="15" t="s">
+      <c r="F25" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G25" s="18" t="s">
+      <c r="G25" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H25" s="18" t="s">
+      <c r="H25" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I25" s="15" t="s">
+      <c r="I25" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J25" s="23" t="s">
+      <c r="J25" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="18" t="n">
+      <c r="A26" s="24" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="15" t="s">
+      <c r="B26" s="22" t="s">
         <v>328</v>
       </c>
-      <c r="C26" s="23" t="s">
+      <c r="C26" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="E26" s="15" t="s">
+      <c r="E26" s="22" t="s">
         <v>328</v>
       </c>
-      <c r="F26" s="15" t="s">
+      <c r="F26" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="G26" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="H26" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I26" s="15" t="s">
+      <c r="I26" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J26" s="23" t="s">
+      <c r="J26" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="18" t="n">
+      <c r="A27" s="24" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="15" t="s">
+      <c r="B27" s="22" t="s">
         <v>328</v>
       </c>
-      <c r="C27" s="23" t="s">
+      <c r="C27" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>330</v>
       </c>
-      <c r="E27" s="15" t="s">
+      <c r="E27" s="22" t="s">
         <v>328</v>
       </c>
-      <c r="F27" s="15" t="s">
+      <c r="F27" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G27" s="18" t="s">
+      <c r="G27" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H27" s="18" t="s">
+      <c r="H27" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I27" s="15" t="s">
+      <c r="I27" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J27" s="23" t="s">
+      <c r="J27" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="18" t="n">
+      <c r="A28" s="24" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="15" t="s">
+      <c r="B28" s="22" t="s">
         <v>331</v>
       </c>
-      <c r="C28" s="23" t="s">
+      <c r="C28" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="E28" s="15" t="s">
+      <c r="E28" s="22" t="s">
         <v>333</v>
       </c>
-      <c r="F28" s="15" t="s">
+      <c r="F28" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G28" s="18" t="s">
+      <c r="G28" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H28" s="18" t="s">
+      <c r="H28" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I28" s="15" t="s">
+      <c r="I28" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J28" s="23" t="s">
+      <c r="J28" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="18" t="n">
+      <c r="A29" s="24" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="15" t="s">
+      <c r="B29" s="22" t="s">
         <v>334</v>
       </c>
-      <c r="C29" s="23" t="s">
+      <c r="C29" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D29" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="E29" s="15" t="s">
+      <c r="E29" s="22" t="s">
         <v>336</v>
       </c>
-      <c r="F29" s="15" t="s">
+      <c r="F29" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G29" s="18" t="s">
+      <c r="G29" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H29" s="18" t="s">
+      <c r="H29" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I29" s="15" t="s">
+      <c r="I29" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J29" s="23" t="s">
+      <c r="J29" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="18" t="n">
+      <c r="A30" s="24" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="15" t="s">
+      <c r="B30" s="22" t="s">
         <v>337</v>
       </c>
-      <c r="C30" s="23" t="s">
+      <c r="C30" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D30" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="E30" s="15" t="s">
+      <c r="E30" s="22" t="s">
         <v>336</v>
       </c>
-      <c r="F30" s="15" t="s">
+      <c r="F30" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G30" s="18" t="s">
+      <c r="G30" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H30" s="18" t="s">
+      <c r="H30" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I30" s="15" t="s">
+      <c r="I30" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J30" s="23" t="s">
+      <c r="J30" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="18" t="n">
+      <c r="A31" s="24" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="22" t="s">
         <v>339</v>
       </c>
-      <c r="C31" s="23" t="s">
+      <c r="C31" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D31" s="15" t="s">
+      <c r="D31" s="22" t="s">
         <v>338</v>
       </c>
-      <c r="E31" s="15" t="s">
+      <c r="E31" s="22" t="s">
         <v>340</v>
       </c>
-      <c r="F31" s="15" t="s">
+      <c r="F31" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G31" s="18" t="s">
+      <c r="G31" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H31" s="18" t="s">
+      <c r="H31" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I31" s="15" t="s">
+      <c r="I31" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J31" s="23" t="s">
+      <c r="J31" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="18" t="n">
+      <c r="A32" s="24" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="15" t="s">
+      <c r="B32" s="22" t="s">
         <v>341</v>
       </c>
-      <c r="C32" s="23" t="s">
+      <c r="C32" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D32" s="15" t="s">
+      <c r="D32" s="22" t="s">
         <v>342</v>
       </c>
-      <c r="E32" s="15" t="s">
+      <c r="E32" s="22" t="s">
         <v>341</v>
       </c>
-      <c r="F32" s="15" t="s">
+      <c r="F32" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G32" s="18" t="s">
+      <c r="G32" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H32" s="18" t="s">
+      <c r="H32" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I32" s="15" t="s">
+      <c r="I32" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J32" s="23" t="s">
+      <c r="J32" s="27" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="18" t="n">
+      <c r="A33" s="24" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="22" t="s">
         <v>343</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="E33" s="15" t="s">
+      <c r="E33" s="22" t="s">
         <v>343</v>
       </c>
-      <c r="F33" s="15" t="s">
+      <c r="F33" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G33" s="18" t="s">
+      <c r="G33" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H33" s="18" t="s">
+      <c r="H33" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I33" s="15" t="s">
+      <c r="I33" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J33" s="23" t="s">
+      <c r="J33" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K33" s="18"/>
+      <c r="K33" s="24"/>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="18" t="n">
+      <c r="A34" s="24" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="22" t="s">
         <v>345</v>
       </c>
-      <c r="C34" s="23" t="s">
+      <c r="C34" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D34" s="15" t="s">
+      <c r="D34" s="22" t="s">
         <v>344</v>
       </c>
-      <c r="E34" s="15" t="s">
+      <c r="E34" s="22" t="s">
         <v>345</v>
       </c>
-      <c r="F34" s="15" t="s">
+      <c r="F34" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G34" s="18" t="s">
+      <c r="G34" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H34" s="18" t="s">
+      <c r="H34" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I34" s="15" t="s">
+      <c r="I34" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J34" s="23" t="s">
+      <c r="J34" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K34" s="18"/>
+      <c r="K34" s="24"/>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="18" t="n">
+      <c r="A35" s="24" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="15" t="s">
+      <c r="B35" s="22" t="s">
         <v>346</v>
       </c>
-      <c r="C35" s="23" t="s">
+      <c r="C35" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D35" s="15" t="s">
+      <c r="D35" s="22" t="s">
         <v>347</v>
       </c>
-      <c r="E35" s="15" t="s">
+      <c r="E35" s="22" t="s">
         <v>346</v>
       </c>
-      <c r="F35" s="15" t="s">
+      <c r="F35" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G35" s="18" t="s">
+      <c r="G35" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H35" s="18" t="s">
+      <c r="H35" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I35" s="15" t="s">
+      <c r="I35" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J35" s="23" t="s">
+      <c r="J35" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K35" s="18"/>
+      <c r="K35" s="24"/>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="18" t="n">
+      <c r="A36" s="24" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="15" t="s">
+      <c r="B36" s="22" t="s">
         <v>348</v>
       </c>
-      <c r="C36" s="23" t="s">
+      <c r="C36" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D36" s="15" t="s">
+      <c r="D36" s="22" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="15" t="s">
+      <c r="E36" s="22" t="s">
         <v>348</v>
       </c>
-      <c r="F36" s="15" t="s">
+      <c r="F36" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G36" s="18" t="s">
+      <c r="G36" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H36" s="18" t="s">
+      <c r="H36" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I36" s="15" t="s">
+      <c r="I36" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J36" s="23" t="s">
+      <c r="J36" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K36" s="18"/>
+      <c r="K36" s="24"/>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="18" t="n">
+      <c r="A37" s="24" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="15" t="s">
+      <c r="B37" s="22" t="s">
         <v>350</v>
       </c>
-      <c r="C37" s="23" t="s">
+      <c r="C37" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D37" s="15" t="s">
+      <c r="D37" s="22" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="15" t="s">
+      <c r="E37" s="22" t="s">
         <v>350</v>
       </c>
-      <c r="F37" s="15" t="s">
+      <c r="F37" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G37" s="18" t="s">
+      <c r="G37" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H37" s="18" t="s">
+      <c r="H37" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I37" s="15" t="s">
+      <c r="I37" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J37" s="23" t="s">
+      <c r="J37" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K37" s="18"/>
+      <c r="K37" s="24"/>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="18" t="n">
+      <c r="A38" s="24" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="22" t="s">
         <v>352</v>
       </c>
-      <c r="C38" s="23" t="s">
+      <c r="C38" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D38" s="15" t="s">
+      <c r="D38" s="22" t="s">
         <v>353</v>
       </c>
-      <c r="E38" s="15" t="s">
+      <c r="E38" s="22" t="s">
         <v>352</v>
       </c>
-      <c r="F38" s="15" t="s">
+      <c r="F38" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G38" s="18" t="s">
+      <c r="G38" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H38" s="18" t="s">
+      <c r="H38" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I38" s="15" t="s">
+      <c r="I38" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J38" s="23" t="s">
+      <c r="J38" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K38" s="18"/>
+      <c r="K38" s="24"/>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="18" t="n">
+      <c r="A39" s="24" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="15" t="s">
+      <c r="B39" s="22" t="s">
         <v>354</v>
       </c>
-      <c r="C39" s="23" t="s">
+      <c r="C39" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D39" s="15" t="s">
+      <c r="D39" s="22" t="s">
         <v>355</v>
       </c>
-      <c r="E39" s="15" t="s">
+      <c r="E39" s="22" t="s">
         <v>354</v>
       </c>
-      <c r="F39" s="15" t="s">
+      <c r="F39" s="22" t="s">
         <v>323</v>
       </c>
-      <c r="G39" s="18" t="s">
+      <c r="G39" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H39" s="18" t="s">
+      <c r="H39" s="24" t="s">
         <v>265</v>
       </c>
-      <c r="I39" s="15" t="s">
+      <c r="I39" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J39" s="23" t="s">
+      <c r="J39" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K39" s="18"/>
+      <c r="K39" s="24"/>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="18" t="n">
+      <c r="A40" s="24" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="15" t="s">
+      <c r="B40" s="22" t="s">
         <v>356</v>
       </c>
-      <c r="C40" s="23" t="s">
+      <c r="C40" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D40" s="15" t="s">
+      <c r="D40" s="22" t="s">
         <v>357</v>
       </c>
-      <c r="E40" s="15" t="s">
+      <c r="E40" s="22" t="s">
         <v>356</v>
       </c>
-      <c r="F40" s="15" t="s">
+      <c r="F40" s="22" t="s">
         <v>358</v>
       </c>
-      <c r="G40" s="18" t="s">
+      <c r="G40" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H40" s="18" t="s">
+      <c r="H40" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="I40" s="15" t="s">
+      <c r="I40" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J40" s="23" t="s">
+      <c r="J40" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="K40" s="18"/>
+      <c r="K40" s="24"/>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="18" t="n">
+      <c r="A41" s="24" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="15" t="s">
+      <c r="B41" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="C41" s="23" t="s">
+      <c r="C41" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D41" s="15" t="s">
+      <c r="D41" s="22" t="s">
         <v>361</v>
       </c>
-      <c r="E41" s="15" t="s">
+      <c r="E41" s="22" t="s">
         <v>360</v>
       </c>
-      <c r="F41" s="15" t="s">
+      <c r="F41" s="22" t="s">
         <v>362</v>
       </c>
-      <c r="G41" s="18" t="s">
+      <c r="G41" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H41" s="18" t="s">
+      <c r="H41" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="I41" s="15" t="s">
+      <c r="I41" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J41" s="23" t="s">
+      <c r="J41" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="K41" s="18"/>
+      <c r="K41" s="24"/>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="18" t="n">
+      <c r="A42" s="24" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="15" t="s">
+      <c r="B42" s="22" t="s">
         <v>363</v>
       </c>
-      <c r="C42" s="23" t="s">
+      <c r="C42" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D42" s="15" t="s">
+      <c r="D42" s="22" t="s">
         <v>364</v>
       </c>
-      <c r="E42" s="15" t="s">
+      <c r="E42" s="22" t="s">
         <v>363</v>
       </c>
-      <c r="F42" s="15" t="s">
+      <c r="F42" s="22" t="s">
         <v>365</v>
       </c>
-      <c r="G42" s="18" t="s">
+      <c r="G42" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H42" s="18" t="s">
+      <c r="H42" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="I42" s="15" t="s">
+      <c r="I42" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J42" s="23" t="s">
+      <c r="J42" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K42" s="18"/>
+      <c r="K42" s="24"/>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="18" t="n">
+      <c r="A43" s="24" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="15" t="s">
+      <c r="B43" s="22" t="s">
         <v>366</v>
       </c>
-      <c r="C43" s="23" t="s">
+      <c r="C43" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D43" s="15" t="s">
+      <c r="D43" s="22" t="s">
         <v>367</v>
       </c>
-      <c r="E43" s="15" t="s">
+      <c r="E43" s="22" t="s">
         <v>366</v>
       </c>
-      <c r="F43" s="15" t="s">
+      <c r="F43" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="G43" s="18" t="s">
+      <c r="G43" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H43" s="18" t="s">
+      <c r="H43" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="I43" s="15" t="s">
+      <c r="I43" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J43" s="23" t="s">
+      <c r="J43" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K43" s="18"/>
+      <c r="K43" s="24"/>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="18" t="n">
+      <c r="A44" s="24" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="15" t="s">
+      <c r="B44" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="C44" s="23" t="s">
+      <c r="C44" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D44" s="15" t="s">
+      <c r="D44" s="22" t="s">
         <v>370</v>
       </c>
-      <c r="E44" s="15" t="s">
+      <c r="E44" s="22" t="s">
         <v>369</v>
       </c>
-      <c r="F44" s="15" t="s">
+      <c r="F44" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="G44" s="18" t="s">
+      <c r="G44" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H44" s="18" t="s">
+      <c r="H44" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="I44" s="15" t="s">
+      <c r="I44" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J44" s="23" t="s">
+      <c r="J44" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K44" s="18"/>
+      <c r="K44" s="24"/>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="18" t="n">
+      <c r="A45" s="24" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="15" t="s">
+      <c r="B45" s="22" t="s">
         <v>371</v>
       </c>
-      <c r="C45" s="23" t="s">
+      <c r="C45" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D45" s="15" t="s">
+      <c r="D45" s="22" t="s">
         <v>372</v>
       </c>
-      <c r="E45" s="15" t="s">
+      <c r="E45" s="22" t="s">
         <v>371</v>
       </c>
-      <c r="F45" s="15" t="s">
+      <c r="F45" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="G45" s="18" t="s">
+      <c r="G45" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H45" s="18" t="s">
+      <c r="H45" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="I45" s="15" t="s">
+      <c r="I45" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J45" s="23" t="s">
+      <c r="J45" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K45" s="18"/>
+      <c r="K45" s="24"/>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="18" t="n">
+      <c r="A46" s="24" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="15" t="s">
+      <c r="B46" s="22" t="s">
         <v>373</v>
       </c>
-      <c r="C46" s="23" t="s">
+      <c r="C46" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="22" t="s">
         <v>374</v>
       </c>
-      <c r="E46" s="15" t="s">
+      <c r="E46" s="22" t="s">
         <v>373</v>
       </c>
-      <c r="F46" s="15" t="s">
+      <c r="F46" s="22" t="s">
         <v>375</v>
       </c>
-      <c r="G46" s="18" t="s">
+      <c r="G46" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H46" s="18" t="s">
+      <c r="H46" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="I46" s="15" t="s">
+      <c r="I46" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J46" s="23" t="s">
+      <c r="J46" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K46" s="18"/>
+      <c r="K46" s="24"/>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="18" t="n">
+      <c r="A47" s="24" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="15" t="s">
+      <c r="B47" s="22" t="s">
         <v>376</v>
       </c>
-      <c r="C47" s="23" t="s">
+      <c r="C47" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D47" s="15" t="s">
+      <c r="D47" s="22" t="s">
         <v>377</v>
       </c>
-      <c r="E47" s="15" t="s">
+      <c r="E47" s="22" t="s">
         <v>376</v>
       </c>
-      <c r="F47" s="15" t="s">
+      <c r="F47" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="G47" s="18" t="s">
+      <c r="G47" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H47" s="18" t="s">
+      <c r="H47" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="I47" s="15" t="s">
+      <c r="I47" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J47" s="23" t="s">
+      <c r="J47" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K47" s="18"/>
+      <c r="K47" s="24"/>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="18" t="n">
+      <c r="A48" s="24" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="15" t="s">
+      <c r="B48" s="22" t="s">
         <v>378</v>
       </c>
-      <c r="C48" s="23" t="s">
+      <c r="C48" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D48" s="15" t="s">
+      <c r="D48" s="22" t="s">
         <v>379</v>
       </c>
-      <c r="E48" s="15" t="s">
+      <c r="E48" s="22" t="s">
         <v>378</v>
       </c>
-      <c r="F48" s="15" t="s">
+      <c r="F48" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="G48" s="18" t="s">
+      <c r="G48" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H48" s="18" t="s">
+      <c r="H48" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="I48" s="15" t="s">
+      <c r="I48" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J48" s="23" t="s">
+      <c r="J48" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K48" s="18"/>
+      <c r="K48" s="24"/>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="18" t="n">
+      <c r="A49" s="24" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="15" t="s">
+      <c r="B49" s="22" t="s">
         <v>380</v>
       </c>
-      <c r="C49" s="23" t="s">
+      <c r="C49" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D49" s="15" t="s">
+      <c r="D49" s="22" t="s">
         <v>381</v>
       </c>
-      <c r="E49" s="15" t="s">
+      <c r="E49" s="22" t="s">
         <v>380</v>
       </c>
-      <c r="F49" s="15" t="s">
+      <c r="F49" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="G49" s="18" t="s">
+      <c r="G49" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H49" s="18" t="s">
+      <c r="H49" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="I49" s="15" t="s">
+      <c r="I49" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J49" s="23" t="s">
+      <c r="J49" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K49" s="18"/>
+      <c r="K49" s="24"/>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="18" t="n">
+      <c r="A50" s="24" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="15" t="s">
+      <c r="B50" s="22" t="s">
         <v>382</v>
       </c>
-      <c r="C50" s="23" t="s">
+      <c r="C50" s="27" t="s">
         <v>243</v>
       </c>
-      <c r="D50" s="15" t="s">
+      <c r="D50" s="22" t="s">
         <v>383</v>
       </c>
-      <c r="E50" s="15" t="s">
+      <c r="E50" s="22" t="s">
         <v>384</v>
       </c>
-      <c r="F50" s="15" t="s">
+      <c r="F50" s="22" t="s">
         <v>368</v>
       </c>
-      <c r="G50" s="18" t="s">
+      <c r="G50" s="24" t="s">
         <v>246</v>
       </c>
-      <c r="H50" s="18" t="s">
+      <c r="H50" s="24" t="s">
         <v>359</v>
       </c>
-      <c r="I50" s="15" t="s">
+      <c r="I50" s="22" t="s">
         <v>248</v>
       </c>
-      <c r="J50" s="23" t="s">
+      <c r="J50" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K50" s="18"/>
+      <c r="K50" s="24"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>

<commit_message>
Change the height of the rows on Bugs sheet
</commit_message>
<xml_diff>
--- a/Testing of the Registration Form.xlsx
+++ b/Testing of the Registration Form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" state="visible" r:id="rId2"/>
@@ -1822,7 +1822,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1935,6 +1935,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="5" fillId="2" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2030,7 +2034,7 @@
       <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.13"/>
@@ -5527,11 +5531,11 @@
   </sheetPr>
   <dimension ref="A1:F1009"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="G90" activeCellId="0" sqref="G90"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.88"/>
@@ -10688,1634 +10692,1635 @@
   </sheetPr>
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="bottomLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.66015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="3" style="0" width="15.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="28" width="15.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="0" width="15.75"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="28" t="s">
+    <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="29" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="29" t="s">
+      <c r="B1" s="30" t="s">
         <v>233</v>
       </c>
       <c r="C1" s="30" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="30" t="s">
         <v>235</v>
       </c>
-      <c r="E1" s="29" t="s">
+      <c r="E1" s="30" t="s">
         <v>236</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="31" t="s">
         <v>237</v>
       </c>
-      <c r="G1" s="30" t="s">
+      <c r="G1" s="31" t="s">
         <v>238</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="31" t="s">
         <v>239</v>
       </c>
-      <c r="I1" s="30" t="s">
+      <c r="I1" s="31" t="s">
         <v>240</v>
       </c>
-      <c r="J1" s="30" t="s">
+      <c r="J1" s="31" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="24" t="n">
+    <row r="2" s="19" customFormat="true" ht="115.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="17" t="n">
         <v>1</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="C2" s="27" t="s">
+      <c r="C2" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D2" s="22" t="s">
+      <c r="D2" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="E2" s="22" t="s">
+      <c r="E2" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="F2" s="22" t="s">
+      <c r="F2" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="G2" s="24" t="s">
+      <c r="G2" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="24" t="s">
+      <c r="H2" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="I2" s="22" t="s">
+      <c r="I2" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J2" s="27" t="s">
+      <c r="J2" s="26" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="24" t="n">
+    <row r="3" s="19" customFormat="true" ht="103.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="17" t="n">
         <v>2</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="B3" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="15" t="s">
         <v>251</v>
       </c>
-      <c r="E3" s="22" t="s">
+      <c r="E3" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="F3" s="22" t="s">
+      <c r="F3" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="G3" s="24" t="s">
+      <c r="G3" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H3" s="24" t="s">
+      <c r="H3" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="I3" s="22" t="s">
+      <c r="I3" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J3" s="27" t="s">
+      <c r="J3" s="26" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="24" t="n">
+    <row r="4" s="19" customFormat="true" ht="103.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="17" t="n">
         <v>3</v>
       </c>
-      <c r="B4" s="22" t="s">
+      <c r="B4" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D4" s="22" t="s">
+      <c r="D4" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="E4" s="22" t="s">
+      <c r="E4" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="F4" s="22" t="s">
+      <c r="F4" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="G4" s="24" t="s">
+      <c r="G4" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H4" s="24" t="s">
+      <c r="H4" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="I4" s="22" t="s">
+      <c r="I4" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J4" s="27" t="s">
+      <c r="J4" s="26" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="24" t="n">
+    <row r="5" s="19" customFormat="true" ht="115.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="17" t="n">
         <v>4</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D5" s="22" t="s">
+      <c r="D5" s="15" t="s">
         <v>259</v>
       </c>
-      <c r="E5" s="22" t="s">
+      <c r="E5" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="F5" s="22" t="s">
+      <c r="F5" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="G5" s="24" t="s">
+      <c r="G5" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H5" s="24" t="s">
+      <c r="H5" s="17" t="s">
         <v>247</v>
       </c>
-      <c r="I5" s="22" t="s">
+      <c r="I5" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="27" t="s">
+      <c r="J5" s="26" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="24" t="n">
+    <row r="6" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="17" t="n">
         <v>5</v>
       </c>
-      <c r="B6" s="22" t="s">
+      <c r="B6" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="C6" s="27" t="s">
+      <c r="C6" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D6" s="22" t="s">
+      <c r="D6" s="15" t="s">
         <v>263</v>
       </c>
-      <c r="E6" s="22" t="s">
+      <c r="E6" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="F6" s="22" t="s">
+      <c r="F6" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I6" s="22" t="s">
+      <c r="I6" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J6" s="27" t="s">
+      <c r="J6" s="26" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="24" t="n">
+    <row r="7" s="19" customFormat="true" ht="217.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="17" t="n">
         <v>6</v>
       </c>
-      <c r="B7" s="22" t="s">
+      <c r="B7" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="C7" s="27" t="s">
+      <c r="C7" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D7" s="22" t="s">
+      <c r="D7" s="15" t="s">
         <v>268</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="G7" s="24" t="s">
+      <c r="G7" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H7" s="24" t="s">
+      <c r="H7" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J7" s="27" t="s">
+      <c r="J7" s="26" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="24" t="n">
+    <row r="8" s="19" customFormat="true" ht="229.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="17" t="n">
         <v>7</v>
       </c>
-      <c r="B8" s="22" t="s">
+      <c r="B8" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D8" s="6" t="s">
+      <c r="D8" s="15" t="s">
         <v>272</v>
       </c>
-      <c r="E8" s="22" t="s">
+      <c r="E8" s="15" t="s">
         <v>273</v>
       </c>
-      <c r="F8" s="22" t="s">
+      <c r="F8" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="H8" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I8" s="22" t="s">
+      <c r="I8" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J8" s="27" t="s">
+      <c r="J8" s="26" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="24" t="n">
+    <row r="9" s="19" customFormat="true" ht="293.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="17" t="n">
         <v>8</v>
       </c>
-      <c r="B9" s="22" t="s">
+      <c r="B9" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="C9" s="27" t="s">
+      <c r="C9" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D9" s="6" t="s">
+      <c r="D9" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="E9" s="22" t="s">
+      <c r="E9" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="F9" s="22" t="s">
+      <c r="F9" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="G9" s="24" t="s">
+      <c r="G9" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H9" s="24" t="s">
+      <c r="H9" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I9" s="22" t="s">
+      <c r="I9" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J9" s="27" t="s">
+      <c r="J9" s="26" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="24" t="n">
+    <row r="10" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="17" t="n">
         <v>9</v>
       </c>
-      <c r="B10" s="22" t="s">
+      <c r="B10" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D10" s="6" t="s">
+      <c r="D10" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="E10" s="22" t="s">
+      <c r="E10" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="F10" s="22" t="s">
+      <c r="F10" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="G10" s="24" t="s">
+      <c r="G10" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H10" s="24" t="s">
+      <c r="H10" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I10" s="22" t="s">
+      <c r="I10" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J10" s="27" t="s">
+      <c r="J10" s="26" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="24" t="n">
+    <row r="11" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="17" t="n">
         <v>10</v>
       </c>
-      <c r="B11" s="22" t="s">
+      <c r="B11" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D11" s="6" t="s">
+      <c r="D11" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="E11" s="22" t="s">
+      <c r="E11" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="G11" s="24" t="s">
+      <c r="G11" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H11" s="24" t="s">
+      <c r="H11" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I11" s="22" t="s">
+      <c r="I11" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J11" s="27" t="s">
+      <c r="J11" s="26" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="24" t="n">
+    <row r="12" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="17" t="n">
         <v>11</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D12" s="6" t="s">
+      <c r="D12" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="E12" s="22" t="s">
+      <c r="E12" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="G12" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="H12" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I12" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J12" s="27" t="s">
+      <c r="J12" s="26" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="24" t="n">
+    <row r="13" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="17" t="n">
         <v>12</v>
       </c>
-      <c r="B13" s="22" t="s">
+      <c r="B13" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D13" s="22" t="s">
+      <c r="D13" s="15" t="s">
         <v>293</v>
       </c>
-      <c r="E13" s="22" t="s">
+      <c r="E13" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="F13" s="22" t="s">
+      <c r="F13" s="15" t="s">
         <v>294</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="H13" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I13" s="22" t="s">
+      <c r="I13" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J13" s="27" t="s">
+      <c r="J13" s="26" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="24" t="n">
+    <row r="14" s="19" customFormat="true" ht="331.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="17" t="n">
         <v>13</v>
       </c>
-      <c r="B14" s="22" t="s">
+      <c r="B14" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D14" s="22" t="s">
+      <c r="D14" s="15" t="s">
         <v>297</v>
       </c>
-      <c r="E14" s="22" t="s">
+      <c r="E14" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="F14" s="22" t="s">
+      <c r="F14" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="G14" s="24" t="s">
+      <c r="G14" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H14" s="24" t="s">
+      <c r="H14" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I14" s="22" t="s">
+      <c r="I14" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J14" s="27" t="s">
+      <c r="J14" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="24" t="n">
+    <row r="15" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="17" t="n">
         <v>14</v>
       </c>
-      <c r="B15" s="22" t="s">
+      <c r="B15" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D15" s="22" t="s">
+      <c r="D15" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="E15" s="22" t="s">
+      <c r="E15" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="F15" s="22" t="s">
+      <c r="F15" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I15" s="22" t="s">
+      <c r="I15" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J15" s="27" t="s">
+      <c r="J15" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K15" s="24"/>
     </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="24" t="n">
+    <row r="16" s="19" customFormat="true" ht="280.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="17" t="n">
         <v>15</v>
       </c>
-      <c r="B16" s="22" t="s">
+      <c r="B16" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="C16" s="27" t="s">
+      <c r="C16" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D16" s="22" t="s">
+      <c r="D16" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="E16" s="22" t="s">
+      <c r="E16" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="G16" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="H16" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="I16" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J16" s="27" t="s">
+      <c r="J16" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="24" t="n">
+    <row r="17" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="17" t="n">
         <v>16</v>
       </c>
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="C17" s="27" t="s">
+      <c r="C17" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D17" s="22" t="s">
+      <c r="D17" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="E17" s="22" t="s">
+      <c r="E17" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="G17" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="H17" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I17" s="22" t="s">
+      <c r="I17" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J17" s="27" t="s">
+      <c r="J17" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="24" t="n">
+    <row r="18" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="17" t="n">
         <v>17</v>
       </c>
-      <c r="B18" s="22" t="s">
+      <c r="B18" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="C18" s="27" t="s">
+      <c r="C18" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D18" s="22" t="s">
+      <c r="D18" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="E18" s="22" t="s">
+      <c r="E18" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="F18" s="22" t="s">
+      <c r="F18" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="G18" s="24" t="s">
+      <c r="G18" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H18" s="24" t="s">
+      <c r="H18" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I18" s="22" t="s">
+      <c r="I18" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J18" s="27" t="s">
+      <c r="J18" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="24" t="n">
+    <row r="19" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="17" t="n">
         <v>18</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="C19" s="27" t="s">
+      <c r="C19" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D19" s="22" t="s">
+      <c r="D19" s="15" t="s">
         <v>311</v>
       </c>
-      <c r="E19" s="22" t="s">
+      <c r="E19" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="F19" s="22" t="s">
+      <c r="F19" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="G19" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="H19" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I19" s="22" t="s">
+      <c r="I19" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J19" s="27" t="s">
+      <c r="J19" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="24" t="n">
+    <row r="20" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="17" t="n">
         <v>19</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B20" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="C20" s="27" t="s">
+      <c r="C20" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D20" s="22" t="s">
+      <c r="D20" s="15" t="s">
         <v>314</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E20" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="F20" s="22" t="s">
+      <c r="F20" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="G20" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="H20" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I20" s="22" t="s">
+      <c r="I20" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J20" s="27" t="s">
+      <c r="J20" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="24" t="n">
+    <row r="21" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="17" t="n">
         <v>20</v>
       </c>
-      <c r="B21" s="22" t="s">
+      <c r="B21" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="C21" s="27" t="s">
+      <c r="C21" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D21" s="22" t="s">
+      <c r="D21" s="15" t="s">
         <v>316</v>
       </c>
-      <c r="E21" s="22" t="s">
+      <c r="E21" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="F21" s="22" t="s">
+      <c r="F21" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="G21" s="24" t="s">
+      <c r="G21" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H21" s="24" t="s">
+      <c r="H21" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I21" s="22" t="s">
+      <c r="I21" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J21" s="27" t="s">
+      <c r="J21" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="24" t="n">
+    <row r="22" s="19" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="17" t="n">
         <v>21</v>
       </c>
-      <c r="B22" s="22" t="s">
+      <c r="B22" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="C22" s="27" t="s">
+      <c r="C22" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D22" s="6" t="s">
+      <c r="D22" s="15" t="s">
         <v>319</v>
       </c>
-      <c r="E22" s="22" t="s">
+      <c r="E22" s="15" t="s">
         <v>320</v>
       </c>
-      <c r="F22" s="22" t="s">
+      <c r="F22" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="G22" s="24" t="s">
+      <c r="G22" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H22" s="24" t="s">
+      <c r="H22" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I22" s="22" t="s">
+      <c r="I22" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J22" s="27" t="s">
+      <c r="J22" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="24" t="n">
+    <row r="23" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="17" t="n">
         <v>22</v>
       </c>
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="C23" s="27" t="s">
+      <c r="C23" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D23" s="6" t="s">
+      <c r="D23" s="15" t="s">
         <v>322</v>
       </c>
-      <c r="E23" s="22" t="s">
+      <c r="E23" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="F23" s="22" t="s">
+      <c r="F23" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G23" s="24" t="s">
+      <c r="G23" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H23" s="24" t="s">
+      <c r="H23" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I23" s="22" t="s">
+      <c r="I23" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J23" s="27" t="s">
+      <c r="J23" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="24" t="n">
+    <row r="24" s="19" customFormat="true" ht="318.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="17" t="n">
         <v>23</v>
       </c>
-      <c r="B24" s="22" t="s">
+      <c r="B24" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="C24" s="27" t="s">
+      <c r="C24" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D24" s="6" t="s">
+      <c r="D24" s="15" t="s">
         <v>325</v>
       </c>
-      <c r="E24" s="22" t="s">
+      <c r="E24" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="F24" s="22" t="s">
+      <c r="F24" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G24" s="24" t="s">
+      <c r="G24" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H24" s="24" t="s">
+      <c r="H24" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I24" s="22" t="s">
+      <c r="I24" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J24" s="27" t="s">
+      <c r="J24" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="24" t="n">
+    <row r="25" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="17" t="n">
         <v>24</v>
       </c>
-      <c r="B25" s="22" t="s">
+      <c r="B25" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="C25" s="27" t="s">
+      <c r="C25" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D25" s="6" t="s">
+      <c r="D25" s="15" t="s">
         <v>327</v>
       </c>
-      <c r="E25" s="22" t="s">
+      <c r="E25" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="F25" s="22" t="s">
+      <c r="F25" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G25" s="24" t="s">
+      <c r="G25" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H25" s="24" t="s">
+      <c r="H25" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I25" s="22" t="s">
+      <c r="I25" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J25" s="27" t="s">
+      <c r="J25" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="24" t="n">
+    <row r="26" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="17" t="n">
         <v>25</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="C26" s="27" t="s">
+      <c r="C26" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D26" s="6" t="s">
+      <c r="D26" s="15" t="s">
         <v>329</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="F26" s="22" t="s">
+      <c r="F26" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G26" s="24" t="s">
+      <c r="G26" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H26" s="24" t="s">
+      <c r="H26" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I26" s="22" t="s">
+      <c r="I26" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J26" s="27" t="s">
+      <c r="J26" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="24" t="n">
+    <row r="27" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="17" t="n">
         <v>26</v>
       </c>
-      <c r="B27" s="22" t="s">
+      <c r="B27" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="C27" s="27" t="s">
+      <c r="C27" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D27" s="6" t="s">
+      <c r="D27" s="15" t="s">
         <v>330</v>
       </c>
-      <c r="E27" s="22" t="s">
+      <c r="E27" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G27" s="24" t="s">
+      <c r="G27" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H27" s="24" t="s">
+      <c r="H27" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I27" s="22" t="s">
+      <c r="I27" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J27" s="27" t="s">
+      <c r="J27" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A28" s="24" t="n">
+    <row r="28" s="19" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="17" t="n">
         <v>27</v>
       </c>
-      <c r="B28" s="22" t="s">
+      <c r="B28" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="C28" s="27" t="s">
+      <c r="C28" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D28" s="6" t="s">
+      <c r="D28" s="15" t="s">
         <v>332</v>
       </c>
-      <c r="E28" s="22" t="s">
+      <c r="E28" s="15" t="s">
         <v>333</v>
       </c>
-      <c r="F28" s="22" t="s">
+      <c r="F28" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G28" s="24" t="s">
+      <c r="G28" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H28" s="24" t="s">
+      <c r="H28" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I28" s="22" t="s">
+      <c r="I28" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J28" s="27" t="s">
+      <c r="J28" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="24" t="n">
+    <row r="29" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="17" t="n">
         <v>28</v>
       </c>
-      <c r="B29" s="22" t="s">
+      <c r="B29" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="C29" s="27" t="s">
+      <c r="C29" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D29" s="6" t="s">
+      <c r="D29" s="15" t="s">
         <v>335</v>
       </c>
-      <c r="E29" s="22" t="s">
+      <c r="E29" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="F29" s="22" t="s">
+      <c r="F29" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G29" s="24" t="s">
+      <c r="G29" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H29" s="24" t="s">
+      <c r="H29" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I29" s="22" t="s">
+      <c r="I29" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J29" s="27" t="s">
+      <c r="J29" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="24" t="n">
+    <row r="30" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="17" t="n">
         <v>29</v>
       </c>
-      <c r="B30" s="22" t="s">
+      <c r="B30" s="15" t="s">
         <v>337</v>
       </c>
-      <c r="C30" s="27" t="s">
+      <c r="C30" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D30" s="6" t="s">
+      <c r="D30" s="15" t="s">
         <v>338</v>
       </c>
-      <c r="E30" s="22" t="s">
+      <c r="E30" s="15" t="s">
         <v>336</v>
       </c>
-      <c r="F30" s="22" t="s">
+      <c r="F30" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G30" s="24" t="s">
+      <c r="G30" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H30" s="24" t="s">
+      <c r="H30" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I30" s="22" t="s">
+      <c r="I30" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J30" s="27" t="s">
+      <c r="J30" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="24" t="n">
+    <row r="31" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="17" t="n">
         <v>30</v>
       </c>
-      <c r="B31" s="22" t="s">
+      <c r="B31" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="C31" s="27" t="s">
+      <c r="C31" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="15" t="s">
         <v>338</v>
       </c>
-      <c r="E31" s="22" t="s">
+      <c r="E31" s="15" t="s">
         <v>340</v>
       </c>
-      <c r="F31" s="22" t="s">
+      <c r="F31" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G31" s="24" t="s">
+      <c r="G31" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H31" s="24" t="s">
+      <c r="H31" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I31" s="22" t="s">
+      <c r="I31" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J31" s="27" t="s">
+      <c r="J31" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="24" t="n">
+    <row r="32" s="19" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="17" t="n">
         <v>31</v>
       </c>
-      <c r="B32" s="22" t="s">
+      <c r="B32" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="C32" s="27" t="s">
+      <c r="C32" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="15" t="s">
         <v>342</v>
       </c>
-      <c r="E32" s="22" t="s">
+      <c r="E32" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="F32" s="22" t="s">
+      <c r="F32" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G32" s="24" t="s">
+      <c r="G32" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H32" s="24" t="s">
+      <c r="H32" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I32" s="22" t="s">
+      <c r="I32" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J32" s="27" t="s">
+      <c r="J32" s="26" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="24" t="n">
+    <row r="33" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="17" t="n">
         <v>32</v>
       </c>
-      <c r="B33" s="22" t="s">
+      <c r="B33" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="C33" s="27" t="s">
+      <c r="C33" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="15" t="s">
         <v>344</v>
       </c>
-      <c r="E33" s="22" t="s">
+      <c r="E33" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="F33" s="22" t="s">
+      <c r="F33" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G33" s="24" t="s">
+      <c r="G33" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H33" s="24" t="s">
+      <c r="H33" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I33" s="22" t="s">
+      <c r="I33" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J33" s="27" t="s">
+      <c r="J33" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K33" s="24"/>
     </row>
-    <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="24" t="n">
+    <row r="34" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="17" t="n">
         <v>33</v>
       </c>
-      <c r="B34" s="22" t="s">
+      <c r="B34" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="C34" s="27" t="s">
+      <c r="C34" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="15" t="s">
         <v>344</v>
       </c>
-      <c r="E34" s="22" t="s">
+      <c r="E34" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="F34" s="22" t="s">
+      <c r="F34" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G34" s="24" t="s">
+      <c r="G34" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H34" s="24" t="s">
+      <c r="H34" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I34" s="22" t="s">
+      <c r="I34" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J34" s="27" t="s">
+      <c r="J34" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K34" s="24"/>
     </row>
-    <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="24" t="n">
+    <row r="35" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="17" t="n">
         <v>34</v>
       </c>
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="15" t="s">
         <v>346</v>
       </c>
-      <c r="C35" s="27" t="s">
+      <c r="C35" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="15" t="s">
         <v>347</v>
       </c>
-      <c r="E35" s="22" t="s">
+      <c r="E35" s="15" t="s">
         <v>346</v>
       </c>
-      <c r="F35" s="22" t="s">
+      <c r="F35" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G35" s="24" t="s">
+      <c r="G35" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H35" s="24" t="s">
+      <c r="H35" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I35" s="22" t="s">
+      <c r="I35" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J35" s="27" t="s">
+      <c r="J35" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K35" s="24"/>
     </row>
-    <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="24" t="n">
+    <row r="36" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="17" t="n">
         <v>35</v>
       </c>
-      <c r="B36" s="22" t="s">
+      <c r="B36" s="15" t="s">
         <v>348</v>
       </c>
-      <c r="C36" s="27" t="s">
+      <c r="C36" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="15" t="s">
         <v>349</v>
       </c>
-      <c r="E36" s="22" t="s">
+      <c r="E36" s="15" t="s">
         <v>348</v>
       </c>
-      <c r="F36" s="22" t="s">
+      <c r="F36" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G36" s="24" t="s">
+      <c r="G36" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H36" s="24" t="s">
+      <c r="H36" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I36" s="22" t="s">
+      <c r="I36" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J36" s="27" t="s">
+      <c r="J36" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K36" s="24"/>
     </row>
-    <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="24" t="n">
+    <row r="37" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="17" t="n">
         <v>36</v>
       </c>
-      <c r="B37" s="22" t="s">
+      <c r="B37" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="C37" s="27" t="s">
+      <c r="C37" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="15" t="s">
         <v>351</v>
       </c>
-      <c r="E37" s="22" t="s">
+      <c r="E37" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="F37" s="22" t="s">
+      <c r="F37" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G37" s="24" t="s">
+      <c r="G37" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H37" s="24" t="s">
+      <c r="H37" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I37" s="22" t="s">
+      <c r="I37" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J37" s="27" t="s">
+      <c r="J37" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K37" s="24"/>
     </row>
-    <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="24" t="n">
+    <row r="38" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="17" t="n">
         <v>37</v>
       </c>
-      <c r="B38" s="22" t="s">
+      <c r="B38" s="15" t="s">
         <v>352</v>
       </c>
-      <c r="C38" s="27" t="s">
+      <c r="C38" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="15" t="s">
         <v>353</v>
       </c>
-      <c r="E38" s="22" t="s">
+      <c r="E38" s="15" t="s">
         <v>352</v>
       </c>
-      <c r="F38" s="22" t="s">
+      <c r="F38" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G38" s="24" t="s">
+      <c r="G38" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H38" s="24" t="s">
+      <c r="H38" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I38" s="22" t="s">
+      <c r="I38" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J38" s="27" t="s">
+      <c r="J38" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K38" s="24"/>
     </row>
-    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="24" t="n">
+    <row r="39" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="17" t="n">
         <v>38</v>
       </c>
-      <c r="B39" s="22" t="s">
+      <c r="B39" s="15" t="s">
         <v>354</v>
       </c>
-      <c r="C39" s="27" t="s">
+      <c r="C39" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="15" t="s">
         <v>355</v>
       </c>
-      <c r="E39" s="22" t="s">
+      <c r="E39" s="15" t="s">
         <v>354</v>
       </c>
-      <c r="F39" s="22" t="s">
+      <c r="F39" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G39" s="24" t="s">
+      <c r="G39" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H39" s="24" t="s">
+      <c r="H39" s="17" t="s">
         <v>265</v>
       </c>
-      <c r="I39" s="22" t="s">
+      <c r="I39" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J39" s="27" t="s">
+      <c r="J39" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K39" s="24"/>
     </row>
-    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="24" t="n">
+    <row r="40" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="17" t="n">
         <v>39</v>
       </c>
-      <c r="B40" s="22" t="s">
+      <c r="B40" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C40" s="27" t="s">
+      <c r="C40" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="15" t="s">
         <v>357</v>
       </c>
-      <c r="E40" s="22" t="s">
+      <c r="E40" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="F40" s="22" t="s">
+      <c r="F40" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="G40" s="24" t="s">
+      <c r="G40" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H40" s="24" t="s">
+      <c r="H40" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="I40" s="22" t="s">
+      <c r="I40" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J40" s="27" t="s">
+      <c r="J40" s="26" t="s">
         <v>209</v>
       </c>
       <c r="K40" s="24"/>
     </row>
-    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="24" t="n">
+    <row r="41" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="17" t="n">
         <v>40</v>
       </c>
-      <c r="B41" s="22" t="s">
+      <c r="B41" s="15" t="s">
         <v>360</v>
       </c>
-      <c r="C41" s="27" t="s">
+      <c r="C41" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D41" s="15" t="s">
         <v>361</v>
       </c>
-      <c r="E41" s="22" t="s">
+      <c r="E41" s="15" t="s">
         <v>360</v>
       </c>
-      <c r="F41" s="22" t="s">
+      <c r="F41" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="G41" s="24" t="s">
+      <c r="G41" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H41" s="24" t="s">
+      <c r="H41" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="I41" s="22" t="s">
+      <c r="I41" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J41" s="27" t="s">
+      <c r="J41" s="26" t="s">
         <v>209</v>
       </c>
       <c r="K41" s="24"/>
     </row>
-    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="24" t="n">
+    <row r="42" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="17" t="n">
         <v>41</v>
       </c>
-      <c r="B42" s="22" t="s">
+      <c r="B42" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="C42" s="27" t="s">
+      <c r="C42" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D42" s="22" t="s">
+      <c r="D42" s="15" t="s">
         <v>364</v>
       </c>
-      <c r="E42" s="22" t="s">
+      <c r="E42" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="F42" s="22" t="s">
+      <c r="F42" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="G42" s="24" t="s">
+      <c r="G42" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H42" s="24" t="s">
+      <c r="H42" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="I42" s="22" t="s">
+      <c r="I42" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J42" s="27" t="s">
+      <c r="J42" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K42" s="24"/>
     </row>
-    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="24" t="n">
+    <row r="43" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="17" t="n">
         <v>42</v>
       </c>
-      <c r="B43" s="22" t="s">
+      <c r="B43" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="C43" s="27" t="s">
+      <c r="C43" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="D43" s="15" t="s">
         <v>367</v>
       </c>
-      <c r="E43" s="22" t="s">
+      <c r="E43" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="F43" s="22" t="s">
+      <c r="F43" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G43" s="24" t="s">
+      <c r="G43" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H43" s="24" t="s">
+      <c r="H43" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="I43" s="22" t="s">
+      <c r="I43" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J43" s="27" t="s">
+      <c r="J43" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K43" s="24"/>
     </row>
-    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="24" t="n">
+    <row r="44" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="17" t="n">
         <v>43</v>
       </c>
-      <c r="B44" s="22" t="s">
+      <c r="B44" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="C44" s="27" t="s">
+      <c r="C44" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D44" s="15" t="s">
         <v>370</v>
       </c>
-      <c r="E44" s="22" t="s">
+      <c r="E44" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="F44" s="22" t="s">
+      <c r="F44" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G44" s="24" t="s">
+      <c r="G44" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H44" s="24" t="s">
+      <c r="H44" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="I44" s="22" t="s">
+      <c r="I44" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J44" s="27" t="s">
+      <c r="J44" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K44" s="24"/>
     </row>
-    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="24" t="n">
+    <row r="45" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="17" t="n">
         <v>44</v>
       </c>
-      <c r="B45" s="22" t="s">
+      <c r="B45" s="15" t="s">
         <v>371</v>
       </c>
-      <c r="C45" s="27" t="s">
+      <c r="C45" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="15" t="s">
         <v>372</v>
       </c>
-      <c r="E45" s="22" t="s">
+      <c r="E45" s="15" t="s">
         <v>371</v>
       </c>
-      <c r="F45" s="22" t="s">
+      <c r="F45" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G45" s="24" t="s">
+      <c r="G45" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H45" s="24" t="s">
+      <c r="H45" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="I45" s="22" t="s">
+      <c r="I45" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J45" s="27" t="s">
+      <c r="J45" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K45" s="24"/>
     </row>
-    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="24" t="n">
+    <row r="46" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="17" t="n">
         <v>45</v>
       </c>
-      <c r="B46" s="22" t="s">
+      <c r="B46" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="C46" s="27" t="s">
+      <c r="C46" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="15" t="s">
         <v>374</v>
       </c>
-      <c r="E46" s="22" t="s">
+      <c r="E46" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="F46" s="22" t="s">
+      <c r="F46" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="G46" s="24" t="s">
+      <c r="G46" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H46" s="24" t="s">
+      <c r="H46" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="I46" s="22" t="s">
+      <c r="I46" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J46" s="27" t="s">
+      <c r="J46" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K46" s="24"/>
     </row>
-    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A47" s="24" t="n">
+    <row r="47" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="17" t="n">
         <v>46</v>
       </c>
-      <c r="B47" s="22" t="s">
+      <c r="B47" s="15" t="s">
         <v>376</v>
       </c>
-      <c r="C47" s="27" t="s">
+      <c r="C47" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="15" t="s">
         <v>377</v>
       </c>
-      <c r="E47" s="22" t="s">
+      <c r="E47" s="15" t="s">
         <v>376</v>
       </c>
-      <c r="F47" s="22" t="s">
+      <c r="F47" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G47" s="24" t="s">
+      <c r="G47" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H47" s="24" t="s">
+      <c r="H47" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="I47" s="22" t="s">
+      <c r="I47" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J47" s="27" t="s">
+      <c r="J47" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K47" s="24"/>
     </row>
-    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="24" t="n">
+    <row r="48" s="19" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="17" t="n">
         <v>47</v>
       </c>
-      <c r="B48" s="22" t="s">
+      <c r="B48" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="C48" s="27" t="s">
+      <c r="C48" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D48" s="22" t="s">
+      <c r="D48" s="15" t="s">
         <v>379</v>
       </c>
-      <c r="E48" s="22" t="s">
+      <c r="E48" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="F48" s="22" t="s">
+      <c r="F48" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G48" s="24" t="s">
+      <c r="G48" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H48" s="24" t="s">
+      <c r="H48" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="I48" s="22" t="s">
+      <c r="I48" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J48" s="27" t="s">
+      <c r="J48" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K48" s="24"/>
     </row>
-    <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="24" t="n">
+    <row r="49" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="17" t="n">
         <v>48</v>
       </c>
-      <c r="B49" s="22" t="s">
+      <c r="B49" s="15" t="s">
         <v>380</v>
       </c>
-      <c r="C49" s="27" t="s">
+      <c r="C49" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D49" s="22" t="s">
+      <c r="D49" s="15" t="s">
         <v>381</v>
       </c>
-      <c r="E49" s="22" t="s">
+      <c r="E49" s="15" t="s">
         <v>380</v>
       </c>
-      <c r="F49" s="22" t="s">
+      <c r="F49" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G49" s="24" t="s">
+      <c r="G49" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H49" s="24" t="s">
+      <c r="H49" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="I49" s="22" t="s">
+      <c r="I49" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J49" s="27" t="s">
+      <c r="J49" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K49" s="24"/>
     </row>
-    <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="24" t="n">
+    <row r="50" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="17" t="n">
         <v>49</v>
       </c>
-      <c r="B50" s="22" t="s">
+      <c r="B50" s="15" t="s">
         <v>382</v>
       </c>
-      <c r="C50" s="27" t="s">
+      <c r="C50" s="26" t="s">
         <v>243</v>
       </c>
-      <c r="D50" s="22" t="s">
+      <c r="D50" s="15" t="s">
         <v>383</v>
       </c>
-      <c r="E50" s="22" t="s">
+      <c r="E50" s="15" t="s">
         <v>384</v>
       </c>
-      <c r="F50" s="22" t="s">
+      <c r="F50" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G50" s="24" t="s">
+      <c r="G50" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H50" s="24" t="s">
+      <c r="H50" s="17" t="s">
         <v>359</v>
       </c>
-      <c r="I50" s="22" t="s">
+      <c r="I50" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J50" s="27" t="s">
+      <c r="J50" s="26" t="s">
         <v>299</v>
       </c>
       <c r="K50" s="24"/>

</xml_diff>

<commit_message>
Center the text in column D
</commit_message>
<xml_diff>
--- a/Testing of the Registration Form.xlsx
+++ b/Testing of the Registration Form.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Requirements" sheetId="1" state="visible" r:id="rId2"/>
@@ -1892,11 +1892,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1904,11 +1900,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="10" fillId="5" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -1916,7 +1912,11 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -2031,10 +2031,10 @@
   <dimension ref="A1:B1021"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
+      <selection pane="topLeft" activeCell="A83" activeCellId="1" sqref="D5:E91 A83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.13"/>
@@ -5531,11 +5531,11 @@
   </sheetPr>
   <dimension ref="A1:F1009"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G90" activeCellId="0" sqref="G90"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A90" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5:E91"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.88"/>
@@ -5577,7 +5577,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" s="19" customFormat="true" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" s="18" customFormat="true" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="n">
         <v>1</v>
       </c>
@@ -5590,9 +5590,9 @@
       <c r="D5" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="18"/>
-    </row>
-    <row r="6" s="19" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E5" s="17"/>
+    </row>
+    <row r="6" s="18" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="n">
         <v>2</v>
       </c>
@@ -5600,43 +5600,43 @@
         <v>68</v>
       </c>
       <c r="C6" s="14"/>
-      <c r="D6" s="20" t="s">
+      <c r="D6" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="21" t="n">
+      <c r="E6" s="20" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="22"/>
-    </row>
-    <row r="7" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F6" s="21"/>
+    </row>
+    <row r="7" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="n">
         <v>3</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="17"/>
+      <c r="C7" s="22"/>
       <c r="D7" s="17" t="s">
         <v>67</v>
       </c>
       <c r="E7" s="23"/>
     </row>
-    <row r="8" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="8" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="n">
         <v>4</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="17"/>
-      <c r="D8" s="20" t="s">
+      <c r="C8" s="22"/>
+      <c r="D8" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="21" t="n">
+      <c r="E8" s="20" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="9" s="19" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="18" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="n">
         <v>5</v>
       </c>
@@ -5644,14 +5644,14 @@
         <v>72</v>
       </c>
       <c r="C9" s="14"/>
-      <c r="D9" s="20" t="s">
+      <c r="D9" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="21" t="n">
+      <c r="E9" s="20" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="10" s="19" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" s="18" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="n">
         <v>6</v>
       </c>
@@ -5662,9 +5662,9 @@
       <c r="D10" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="18"/>
-    </row>
-    <row r="11" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E10" s="17"/>
+    </row>
+    <row r="11" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="n">
         <v>7</v>
       </c>
@@ -5675,9 +5675,9 @@
       <c r="D11" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="18"/>
-    </row>
-    <row r="12" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E11" s="17"/>
+    </row>
+    <row r="12" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="n">
         <v>8</v>
       </c>
@@ -5688,9 +5688,9 @@
       <c r="D12" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="18"/>
-    </row>
-    <row r="13" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E12" s="17"/>
+    </row>
+    <row r="13" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="n">
         <v>9</v>
       </c>
@@ -5703,9 +5703,9 @@
       <c r="D13" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="18"/>
-    </row>
-    <row r="14" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E13" s="17"/>
+    </row>
+    <row r="14" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="n">
         <v>10</v>
       </c>
@@ -5715,14 +5715,14 @@
       <c r="C14" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="21" t="n">
+      <c r="E14" s="20" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="15" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="n">
         <v>11</v>
       </c>
@@ -5733,9 +5733,9 @@
       <c r="D15" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="18"/>
-    </row>
-    <row r="16" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E15" s="17"/>
+    </row>
+    <row r="16" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="n">
         <v>12</v>
       </c>
@@ -5748,9 +5748,9 @@
       <c r="D16" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="18"/>
-    </row>
-    <row r="17" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E16" s="17"/>
+    </row>
+    <row r="17" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="n">
         <v>13</v>
       </c>
@@ -5763,9 +5763,9 @@
       <c r="D17" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="18"/>
-    </row>
-    <row r="18" s="19" customFormat="true" ht="98.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E17" s="17"/>
+    </row>
+    <row r="18" s="18" customFormat="true" ht="98.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="n">
         <v>14</v>
       </c>
@@ -5775,15 +5775,15 @@
       <c r="C18" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="20" t="s">
+      <c r="D18" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="21" t="n">
+      <c r="E18" s="20" t="n">
         <v>6</v>
       </c>
       <c r="F18" s="24"/>
     </row>
-    <row r="19" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="19" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="n">
         <v>15</v>
       </c>
@@ -5796,10 +5796,10 @@
       <c r="D19" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="18"/>
+      <c r="E19" s="17"/>
       <c r="F19" s="24"/>
     </row>
-    <row r="20" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="20" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="n">
         <v>16</v>
       </c>
@@ -5809,15 +5809,15 @@
       <c r="C20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="20" t="s">
+      <c r="D20" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="21" t="n">
+      <c r="E20" s="20" t="n">
         <v>7</v>
       </c>
       <c r="F20" s="24"/>
     </row>
-    <row r="21" s="19" customFormat="true" ht="200.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="21" s="18" customFormat="true" ht="200.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="n">
         <v>17</v>
       </c>
@@ -5827,15 +5827,15 @@
       <c r="C21" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="20" t="s">
+      <c r="D21" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="21" t="n">
+      <c r="E21" s="20" t="n">
         <v>8</v>
       </c>
       <c r="F21" s="24"/>
     </row>
-    <row r="22" s="19" customFormat="true" ht="200.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="22" s="18" customFormat="true" ht="200.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="n">
         <v>18</v>
       </c>
@@ -5848,10 +5848,10 @@
       <c r="D22" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="18"/>
+      <c r="E22" s="17"/>
       <c r="F22" s="24"/>
     </row>
-    <row r="23" s="19" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="23" s="18" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="n">
         <v>19</v>
       </c>
@@ -5861,15 +5861,15 @@
       <c r="C23" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="20" t="s">
+      <c r="D23" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="21" t="n">
+      <c r="E23" s="20" t="n">
         <v>9</v>
       </c>
       <c r="F23" s="24"/>
     </row>
-    <row r="24" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="24" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="n">
         <v>20</v>
       </c>
@@ -5879,14 +5879,14 @@
       <c r="C24" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="20" t="s">
+      <c r="D24" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="21" t="n">
+      <c r="E24" s="20" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="25" s="19" customFormat="true" ht="162.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" s="18" customFormat="true" ht="162.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="n">
         <v>21</v>
       </c>
@@ -5896,12 +5896,12 @@
       <c r="C25" s="15" t="s">
         <v>99</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="18"/>
-    </row>
-    <row r="26" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E25" s="17"/>
+    </row>
+    <row r="26" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="n">
         <v>22</v>
       </c>
@@ -5911,13 +5911,13 @@
       <c r="C26" s="15" t="s">
         <v>101</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="18"/>
+      <c r="E26" s="17"/>
       <c r="F26" s="24"/>
     </row>
-    <row r="27" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="27" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="n">
         <v>23</v>
       </c>
@@ -5927,15 +5927,15 @@
       <c r="C27" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="21" t="n">
+      <c r="E27" s="20" t="n">
         <v>11</v>
       </c>
       <c r="F27" s="24"/>
     </row>
-    <row r="28" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="28" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="14" t="n">
         <v>24</v>
       </c>
@@ -5948,10 +5948,10 @@
       <c r="D28" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="18"/>
+      <c r="E28" s="17"/>
       <c r="F28" s="24"/>
     </row>
-    <row r="29" s="19" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="29" s="18" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="14" t="n">
         <v>25</v>
       </c>
@@ -5964,10 +5964,10 @@
       <c r="D29" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="18"/>
+      <c r="E29" s="17"/>
       <c r="F29" s="24"/>
     </row>
-    <row r="30" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="30" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="14" t="n">
         <v>26</v>
       </c>
@@ -5980,10 +5980,10 @@
       <c r="D30" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="18"/>
+      <c r="E30" s="17"/>
       <c r="F30" s="24"/>
     </row>
-    <row r="31" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="31" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="14" t="n">
         <v>27</v>
       </c>
@@ -5996,10 +5996,10 @@
       <c r="D31" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="18"/>
+      <c r="E31" s="17"/>
       <c r="F31" s="24"/>
     </row>
-    <row r="32" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="32" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="n">
         <v>28</v>
       </c>
@@ -6012,10 +6012,10 @@
       <c r="D32" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="18"/>
+      <c r="E32" s="17"/>
       <c r="F32" s="24"/>
     </row>
-    <row r="33" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="33" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="14" t="n">
         <v>29</v>
       </c>
@@ -6028,10 +6028,10 @@
       <c r="D33" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="18"/>
+      <c r="E33" s="17"/>
       <c r="F33" s="24"/>
     </row>
-    <row r="34" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="34" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="14" t="n">
         <v>30</v>
       </c>
@@ -6041,14 +6041,14 @@
       <c r="C34" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="20" t="s">
+      <c r="D34" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="21" t="n">
+      <c r="E34" s="20" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="35" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="14" t="n">
         <v>31</v>
       </c>
@@ -6061,10 +6061,10 @@
       <c r="D35" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E35" s="18"/>
+      <c r="E35" s="17"/>
       <c r="F35" s="24"/>
     </row>
-    <row r="36" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="36" s="18" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="14" t="n">
         <v>32</v>
       </c>
@@ -6077,10 +6077,10 @@
       <c r="D36" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="18"/>
+      <c r="E36" s="17"/>
       <c r="F36" s="24"/>
     </row>
-    <row r="37" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="37" s="18" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="14" t="n">
         <v>33</v>
       </c>
@@ -6090,15 +6090,15 @@
       <c r="C37" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D37" s="20" t="s">
+      <c r="D37" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="21" t="n">
+      <c r="E37" s="20" t="n">
         <v>13</v>
       </c>
       <c r="F37" s="24"/>
     </row>
-    <row r="38" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="38" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="14" t="n">
         <v>34</v>
       </c>
@@ -6108,15 +6108,15 @@
       <c r="C38" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D38" s="20" t="s">
+      <c r="D38" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="21" t="n">
+      <c r="E38" s="20" t="n">
         <v>14</v>
       </c>
       <c r="F38" s="24"/>
     </row>
-    <row r="39" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="39" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="n">
         <v>35</v>
       </c>
@@ -6126,15 +6126,15 @@
       <c r="C39" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D39" s="20" t="s">
+      <c r="D39" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="21" t="n">
+      <c r="E39" s="20" t="n">
         <v>15</v>
       </c>
       <c r="F39" s="24"/>
     </row>
-    <row r="40" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="40" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="14" t="n">
         <v>36</v>
       </c>
@@ -6144,15 +6144,15 @@
       <c r="C40" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="D40" s="20" t="s">
+      <c r="D40" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E40" s="21" t="n">
+      <c r="E40" s="20" t="n">
         <v>16</v>
       </c>
       <c r="F40" s="24"/>
     </row>
-    <row r="41" s="19" customFormat="true" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="41" s="18" customFormat="true" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="14" t="n">
         <v>37</v>
       </c>
@@ -6168,7 +6168,7 @@
       <c r="E41" s="23"/>
       <c r="F41" s="24"/>
     </row>
-    <row r="42" s="19" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="42" s="18" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="14" t="n">
         <v>38</v>
       </c>
@@ -6181,10 +6181,10 @@
       <c r="D42" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="18"/>
+      <c r="E42" s="17"/>
       <c r="F42" s="24"/>
     </row>
-    <row r="43" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="43" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="14" t="n">
         <v>39</v>
       </c>
@@ -6197,10 +6197,10 @@
       <c r="D43" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="18"/>
+      <c r="E43" s="17"/>
       <c r="F43" s="24"/>
     </row>
-    <row r="44" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="44" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="14" t="n">
         <v>40</v>
       </c>
@@ -6213,9 +6213,9 @@
       <c r="D44" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="18"/>
-    </row>
-    <row r="45" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E44" s="17"/>
+    </row>
+    <row r="45" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="14" t="n">
         <v>41</v>
       </c>
@@ -6228,9 +6228,9 @@
       <c r="D45" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E45" s="18"/>
-    </row>
-    <row r="46" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E45" s="17"/>
+    </row>
+    <row r="46" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="14" t="n">
         <v>42</v>
       </c>
@@ -6243,10 +6243,10 @@
       <c r="D46" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E46" s="18"/>
+      <c r="E46" s="17"/>
       <c r="F46" s="24"/>
     </row>
-    <row r="47" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="47" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="14" t="n">
         <v>43</v>
       </c>
@@ -6256,15 +6256,15 @@
       <c r="C47" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D47" s="20" t="s">
+      <c r="D47" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E47" s="21" t="n">
+      <c r="E47" s="20" t="n">
         <v>17</v>
       </c>
       <c r="F47" s="24"/>
     </row>
-    <row r="48" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="14" t="n">
         <v>44</v>
       </c>
@@ -6274,15 +6274,15 @@
       <c r="C48" s="26" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="20" t="s">
+      <c r="D48" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E48" s="21" t="n">
+      <c r="E48" s="20" t="n">
         <v>18</v>
       </c>
       <c r="F48" s="24"/>
     </row>
-    <row r="49" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="49" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="14" t="n">
         <v>45</v>
       </c>
@@ -6292,14 +6292,14 @@
       <c r="C49" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="D49" s="20" t="s">
+      <c r="D49" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E49" s="21" t="n">
+      <c r="E49" s="20" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="50" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="14" t="n">
         <v>46</v>
       </c>
@@ -6309,14 +6309,14 @@
       <c r="C50" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D50" s="20" t="s">
+      <c r="D50" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E50" s="21" t="n">
+      <c r="E50" s="20" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="51" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" s="18" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="14" t="n">
         <v>47</v>
       </c>
@@ -6326,14 +6326,14 @@
       <c r="C51" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D51" s="20" t="s">
+      <c r="D51" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E51" s="21" t="n">
+      <c r="E51" s="20" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="52" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="14" t="n">
         <v>48</v>
       </c>
@@ -6343,14 +6343,14 @@
       <c r="C52" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="D52" s="20" t="s">
+      <c r="D52" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="21" t="n">
+      <c r="E52" s="20" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="53" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="14" t="n">
         <v>49</v>
       </c>
@@ -6363,9 +6363,9 @@
       <c r="D53" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E53" s="18"/>
-    </row>
-    <row r="54" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E53" s="17"/>
+    </row>
+    <row r="54" s="18" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="14" t="n">
         <v>50</v>
       </c>
@@ -6378,9 +6378,9 @@
       <c r="D54" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E54" s="18"/>
-    </row>
-    <row r="55" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E54" s="17"/>
+    </row>
+    <row r="55" s="18" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="14" t="n">
         <v>51</v>
       </c>
@@ -6390,14 +6390,14 @@
       <c r="C55" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="D55" s="20" t="s">
+      <c r="D55" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="21" t="n">
+      <c r="E55" s="20" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="56" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="14" t="n">
         <v>52</v>
       </c>
@@ -6407,14 +6407,14 @@
       <c r="C56" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="D56" s="20" t="s">
+      <c r="D56" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="21" t="n">
+      <c r="E56" s="20" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="57" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="14" t="n">
         <v>53</v>
       </c>
@@ -6424,14 +6424,14 @@
       <c r="C57" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="D57" s="20" t="s">
+      <c r="D57" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E57" s="21" t="n">
+      <c r="E57" s="20" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="58" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="14" t="n">
         <v>54</v>
       </c>
@@ -6441,14 +6441,14 @@
       <c r="C58" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="D58" s="20" t="s">
+      <c r="D58" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E58" s="21" t="n">
+      <c r="E58" s="20" t="n">
         <v>26</v>
       </c>
     </row>
-    <row r="59" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" s="18" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="14" t="n">
         <v>55</v>
       </c>
@@ -6458,14 +6458,14 @@
       <c r="C59" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="D59" s="20" t="s">
+      <c r="D59" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E59" s="21" t="n">
+      <c r="E59" s="20" t="n">
         <v>27</v>
       </c>
     </row>
-    <row r="60" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="14" t="n">
         <v>56</v>
       </c>
@@ -6478,9 +6478,9 @@
       <c r="D60" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E60" s="18"/>
-    </row>
-    <row r="61" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E60" s="17"/>
+    </row>
+    <row r="61" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="14" t="n">
         <v>57</v>
       </c>
@@ -6490,14 +6490,14 @@
       <c r="C61" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="D61" s="20" t="s">
+      <c r="D61" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E61" s="21" t="n">
+      <c r="E61" s="20" t="n">
         <v>28</v>
       </c>
     </row>
-    <row r="62" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" s="18" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="14" t="n">
         <v>58</v>
       </c>
@@ -6510,9 +6510,9 @@
       <c r="D62" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="18"/>
-    </row>
-    <row r="63" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E62" s="17"/>
+    </row>
+    <row r="63" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="14" t="n">
         <v>59</v>
       </c>
@@ -6522,14 +6522,14 @@
       <c r="C63" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="D63" s="20" t="s">
+      <c r="D63" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E63" s="21" t="n">
+      <c r="E63" s="20" t="n">
         <v>29</v>
       </c>
     </row>
-    <row r="64" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="14" t="n">
         <v>60</v>
       </c>
@@ -6539,14 +6539,14 @@
       <c r="C64" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="D64" s="20" t="s">
+      <c r="D64" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E64" s="21" t="n">
+      <c r="E64" s="20" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="65" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" s="18" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="14" t="n">
         <v>61</v>
       </c>
@@ -6556,14 +6556,14 @@
       <c r="C65" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="D65" s="20" t="s">
+      <c r="D65" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E65" s="21" t="n">
+      <c r="E65" s="20" t="n">
         <v>31</v>
       </c>
     </row>
-    <row r="66" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="14" t="n">
         <v>62</v>
       </c>
@@ -6573,14 +6573,14 @@
       <c r="C66" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="D66" s="20" t="s">
+      <c r="D66" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E66" s="21" t="n">
+      <c r="E66" s="20" t="n">
         <v>32</v>
       </c>
     </row>
-    <row r="67" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" s="18" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="14" t="n">
         <v>63</v>
       </c>
@@ -6593,9 +6593,9 @@
       <c r="D67" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E67" s="18"/>
-    </row>
-    <row r="68" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E67" s="17"/>
+    </row>
+    <row r="68" s="18" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="14" t="n">
         <v>64</v>
       </c>
@@ -6608,9 +6608,9 @@
       <c r="D68" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E68" s="18"/>
-    </row>
-    <row r="69" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E68" s="17"/>
+    </row>
+    <row r="69" s="18" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="14" t="n">
         <v>65</v>
       </c>
@@ -6620,14 +6620,14 @@
       <c r="C69" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="D69" s="20" t="s">
+      <c r="D69" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E69" s="21" t="n">
+      <c r="E69" s="20" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="70" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="14" t="n">
         <v>66</v>
       </c>
@@ -6640,9 +6640,9 @@
       <c r="D70" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E70" s="18"/>
-    </row>
-    <row r="71" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E70" s="17"/>
+    </row>
+    <row r="71" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="14" t="n">
         <v>67</v>
       </c>
@@ -6652,14 +6652,14 @@
       <c r="C71" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="D71" s="20" t="s">
+      <c r="D71" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E71" s="21" t="n">
+      <c r="E71" s="20" t="n">
         <v>34</v>
       </c>
     </row>
-    <row r="72" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="14" t="n">
         <v>68</v>
       </c>
@@ -6669,14 +6669,14 @@
       <c r="C72" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="D72" s="20" t="s">
+      <c r="D72" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E72" s="21" t="n">
+      <c r="E72" s="20" t="n">
         <v>35</v>
       </c>
     </row>
-    <row r="73" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="14" t="n">
         <v>69</v>
       </c>
@@ -6689,9 +6689,9 @@
       <c r="D73" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E73" s="18"/>
-    </row>
-    <row r="74" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E73" s="17"/>
+    </row>
+    <row r="74" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="14" t="n">
         <v>70</v>
       </c>
@@ -6701,14 +6701,14 @@
       <c r="C74" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="D74" s="20" t="s">
+      <c r="D74" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E74" s="21" t="n">
+      <c r="E74" s="20" t="n">
         <v>36</v>
       </c>
     </row>
-    <row r="75" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="14" t="n">
         <v>71</v>
       </c>
@@ -6721,9 +6721,9 @@
       <c r="D75" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E75" s="18"/>
-    </row>
-    <row r="76" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E75" s="17"/>
+    </row>
+    <row r="76" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="14" t="n">
         <v>72</v>
       </c>
@@ -6733,14 +6733,14 @@
       <c r="C76" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="D76" s="20" t="s">
+      <c r="D76" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E76" s="21" t="n">
+      <c r="E76" s="20" t="n">
         <v>37</v>
       </c>
     </row>
-    <row r="77" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="14" t="n">
         <v>73</v>
       </c>
@@ -6750,14 +6750,14 @@
       <c r="C77" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="D77" s="20" t="s">
+      <c r="D77" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E77" s="21" t="n">
+      <c r="E77" s="20" t="n">
         <v>38</v>
       </c>
     </row>
-    <row r="78" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="14" t="n">
         <v>74</v>
       </c>
@@ -6770,24 +6770,24 @@
       <c r="D78" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E78" s="18"/>
+      <c r="E78" s="17"/>
       <c r="F78" s="24"/>
     </row>
-    <row r="79" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="79" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="14" t="n">
         <v>75</v>
       </c>
       <c r="B79" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C79" s="17"/>
+      <c r="C79" s="22"/>
       <c r="D79" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E79" s="18"/>
+      <c r="E79" s="17"/>
       <c r="F79" s="24"/>
     </row>
-    <row r="80" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="80" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="14" t="n">
         <v>76</v>
       </c>
@@ -6797,17 +6797,17 @@
       <c r="C80" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="D80" s="20" t="s">
+      <c r="D80" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E80" s="21" t="n">
+      <c r="E80" s="20" t="n">
         <v>39</v>
       </c>
       <c r="F80" s="27" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="81" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="14" t="n">
         <v>77</v>
       </c>
@@ -6817,14 +6817,14 @@
       <c r="C81" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="D81" s="20" t="s">
+      <c r="D81" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E81" s="21" t="n">
+      <c r="E81" s="20" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="82" s="19" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" s="18" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="14" t="n">
         <v>78</v>
       </c>
@@ -6837,9 +6837,9 @@
       <c r="D82" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E82" s="18"/>
-    </row>
-    <row r="83" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E82" s="17"/>
+    </row>
+    <row r="83" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="14" t="n">
         <v>79</v>
       </c>
@@ -6849,14 +6849,14 @@
       <c r="C83" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="D83" s="20" t="s">
+      <c r="D83" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E83" s="21" t="n">
+      <c r="E83" s="20" t="n">
         <v>41</v>
       </c>
     </row>
-    <row r="84" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="14" t="n">
         <v>80</v>
       </c>
@@ -6866,14 +6866,14 @@
       <c r="C84" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="D84" s="20" t="s">
+      <c r="D84" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E84" s="21" t="n">
+      <c r="E84" s="20" t="n">
         <v>42</v>
       </c>
     </row>
-    <row r="85" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="14" t="n">
         <v>81</v>
       </c>
@@ -6883,14 +6883,14 @@
       <c r="C85" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="D85" s="20" t="s">
+      <c r="D85" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E85" s="21" t="n">
+      <c r="E85" s="20" t="n">
         <v>43</v>
       </c>
     </row>
-    <row r="86" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="14" t="n">
         <v>82</v>
       </c>
@@ -6900,14 +6900,14 @@
       <c r="C86" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="D86" s="20" t="s">
+      <c r="D86" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E86" s="21" t="n">
+      <c r="E86" s="20" t="n">
         <v>44</v>
       </c>
     </row>
-    <row r="87" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="14" t="n">
         <v>83</v>
       </c>
@@ -6917,14 +6917,14 @@
       <c r="C87" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="D87" s="20" t="s">
+      <c r="D87" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E87" s="21" t="n">
+      <c r="E87" s="20" t="n">
         <v>45</v>
       </c>
     </row>
-    <row r="88" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="14" t="n">
         <v>84</v>
       </c>
@@ -6934,14 +6934,14 @@
       <c r="C88" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="D88" s="20" t="s">
+      <c r="D88" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E88" s="21" t="n">
+      <c r="E88" s="20" t="n">
         <v>46</v>
       </c>
     </row>
-    <row r="89" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="89" s="18" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="14" t="n">
         <v>85</v>
       </c>
@@ -6951,14 +6951,14 @@
       <c r="C89" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="D89" s="20" t="s">
+      <c r="D89" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E89" s="21" t="n">
+      <c r="E89" s="20" t="n">
         <v>47</v>
       </c>
     </row>
-    <row r="90" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="14" t="n">
         <v>86</v>
       </c>
@@ -6968,14 +6968,14 @@
       <c r="C90" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="D90" s="20" t="s">
+      <c r="D90" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E90" s="21" t="n">
+      <c r="E90" s="20" t="n">
         <v>48</v>
       </c>
     </row>
-    <row r="91" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="14" t="n">
         <v>87</v>
       </c>
@@ -6985,10 +6985,10 @@
       <c r="C91" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="D91" s="20" t="s">
+      <c r="D91" s="19" t="s">
         <v>69</v>
       </c>
-      <c r="E91" s="21" t="n">
+      <c r="E91" s="20" t="n">
         <v>49</v>
       </c>
     </row>
@@ -10692,13 +10692,13 @@
   </sheetPr>
   <dimension ref="A1:K50"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+      <selection pane="bottomLeft" activeCell="H28" activeCellId="1" sqref="D5:E91 H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.38"/>
@@ -10738,8 +10738,8 @@
         <v>241</v>
       </c>
     </row>
-    <row r="2" s="19" customFormat="true" ht="115.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="17" t="n">
+    <row r="2" s="18" customFormat="true" ht="115.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="22" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
@@ -10757,10 +10757,10 @@
       <c r="F2" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="17" t="s">
+      <c r="H2" s="22" t="s">
         <v>247</v>
       </c>
       <c r="I2" s="15" t="s">
@@ -10770,8 +10770,8 @@
         <v>249</v>
       </c>
     </row>
-    <row r="3" s="19" customFormat="true" ht="103.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="17" t="n">
+    <row r="3" s="18" customFormat="true" ht="103.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="22" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
@@ -10789,10 +10789,10 @@
       <c r="F3" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="G3" s="17" t="s">
+      <c r="G3" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H3" s="17" t="s">
+      <c r="H3" s="22" t="s">
         <v>247</v>
       </c>
       <c r="I3" s="15" t="s">
@@ -10802,8 +10802,8 @@
         <v>253</v>
       </c>
     </row>
-    <row r="4" s="19" customFormat="true" ht="103.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="17" t="n">
+    <row r="4" s="18" customFormat="true" ht="103.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="22" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
@@ -10821,10 +10821,10 @@
       <c r="F4" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="G4" s="17" t="s">
+      <c r="G4" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H4" s="17" t="s">
+      <c r="H4" s="22" t="s">
         <v>247</v>
       </c>
       <c r="I4" s="15" t="s">
@@ -10834,8 +10834,8 @@
         <v>257</v>
       </c>
     </row>
-    <row r="5" s="19" customFormat="true" ht="115.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="17" t="n">
+    <row r="5" s="18" customFormat="true" ht="115.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="22" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
@@ -10853,10 +10853,10 @@
       <c r="F5" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="G5" s="17" t="s">
+      <c r="G5" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H5" s="17" t="s">
+      <c r="H5" s="22" t="s">
         <v>247</v>
       </c>
       <c r="I5" s="15" t="s">
@@ -10866,8 +10866,8 @@
         <v>261</v>
       </c>
     </row>
-    <row r="6" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="17" t="n">
+    <row r="6" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="22" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
@@ -10885,10 +10885,10 @@
       <c r="F6" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="G6" s="17" t="s">
+      <c r="G6" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H6" s="17" t="s">
+      <c r="H6" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I6" s="15" t="s">
@@ -10898,8 +10898,8 @@
         <v>266</v>
       </c>
     </row>
-    <row r="7" s="19" customFormat="true" ht="217.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="17" t="n">
+    <row r="7" s="18" customFormat="true" ht="217.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="22" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
@@ -10917,10 +10917,10 @@
       <c r="F7" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="G7" s="17" t="s">
+      <c r="G7" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H7" s="17" t="s">
+      <c r="H7" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I7" s="15" t="s">
@@ -10930,8 +10930,8 @@
         <v>270</v>
       </c>
     </row>
-    <row r="8" s="19" customFormat="true" ht="229.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="17" t="n">
+    <row r="8" s="18" customFormat="true" ht="229.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="22" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
@@ -10949,10 +10949,10 @@
       <c r="F8" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="G8" s="17" t="s">
+      <c r="G8" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H8" s="17" t="s">
+      <c r="H8" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I8" s="15" t="s">
@@ -10962,8 +10962,8 @@
         <v>275</v>
       </c>
     </row>
-    <row r="9" s="19" customFormat="true" ht="293.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="17" t="n">
+    <row r="9" s="18" customFormat="true" ht="293.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
@@ -10981,10 +10981,10 @@
       <c r="F9" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="G9" s="17" t="s">
+      <c r="G9" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H9" s="17" t="s">
+      <c r="H9" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I9" s="15" t="s">
@@ -10994,8 +10994,8 @@
         <v>279</v>
       </c>
     </row>
-    <row r="10" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="17" t="n">
+    <row r="10" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
@@ -11013,10 +11013,10 @@
       <c r="F10" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="G10" s="17" t="s">
+      <c r="G10" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H10" s="17" t="s">
+      <c r="H10" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I10" s="15" t="s">
@@ -11026,8 +11026,8 @@
         <v>283</v>
       </c>
     </row>
-    <row r="11" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="17" t="n">
+    <row r="11" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="22" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
@@ -11045,10 +11045,10 @@
       <c r="F11" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="G11" s="17" t="s">
+      <c r="G11" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H11" s="17" t="s">
+      <c r="H11" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I11" s="15" t="s">
@@ -11058,8 +11058,8 @@
         <v>287</v>
       </c>
     </row>
-    <row r="12" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="17" t="n">
+    <row r="12" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="22" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
@@ -11077,10 +11077,10 @@
       <c r="F12" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I12" s="15" t="s">
@@ -11090,8 +11090,8 @@
         <v>291</v>
       </c>
     </row>
-    <row r="13" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="17" t="n">
+    <row r="13" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="22" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
@@ -11109,10 +11109,10 @@
       <c r="F13" s="15" t="s">
         <v>294</v>
       </c>
-      <c r="G13" s="17" t="s">
+      <c r="G13" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H13" s="17" t="s">
+      <c r="H13" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I13" s="15" t="s">
@@ -11122,8 +11122,8 @@
         <v>295</v>
       </c>
     </row>
-    <row r="14" s="19" customFormat="true" ht="331.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="17" t="n">
+    <row r="14" s="18" customFormat="true" ht="331.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="22" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="15" t="s">
@@ -11141,10 +11141,10 @@
       <c r="F14" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I14" s="15" t="s">
@@ -11154,8 +11154,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="15" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="17" t="n">
+    <row r="15" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="22" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
@@ -11173,10 +11173,10 @@
       <c r="F15" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I15" s="15" t="s">
@@ -11187,8 +11187,8 @@
       </c>
       <c r="K15" s="24"/>
     </row>
-    <row r="16" s="19" customFormat="true" ht="280.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="17" t="n">
+    <row r="16" s="18" customFormat="true" ht="280.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="22" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
@@ -11206,10 +11206,10 @@
       <c r="F16" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="G16" s="17" t="s">
+      <c r="G16" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H16" s="17" t="s">
+      <c r="H16" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I16" s="15" t="s">
@@ -11219,8 +11219,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="17" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="17" t="n">
+    <row r="17" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="22" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
@@ -11238,10 +11238,10 @@
       <c r="F17" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="G17" s="17" t="s">
+      <c r="G17" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H17" s="17" t="s">
+      <c r="H17" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I17" s="15" t="s">
@@ -11251,8 +11251,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="18" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="17" t="n">
+    <row r="18" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="22" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="15" t="s">
@@ -11270,10 +11270,10 @@
       <c r="F18" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="G18" s="17" t="s">
+      <c r="G18" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H18" s="17" t="s">
+      <c r="H18" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I18" s="15" t="s">
@@ -11283,8 +11283,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="19" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="17" t="n">
+    <row r="19" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="22" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
@@ -11302,10 +11302,10 @@
       <c r="F19" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="G19" s="17" t="s">
+      <c r="G19" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H19" s="17" t="s">
+      <c r="H19" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I19" s="15" t="s">
@@ -11315,8 +11315,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="20" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="17" t="n">
+    <row r="20" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="22" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
@@ -11334,10 +11334,10 @@
       <c r="F20" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="G20" s="17" t="s">
+      <c r="G20" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H20" s="17" t="s">
+      <c r="H20" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I20" s="15" t="s">
@@ -11347,8 +11347,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="21" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="17" t="n">
+    <row r="21" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="22" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="15" t="s">
@@ -11366,10 +11366,10 @@
       <c r="F21" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H21" s="17" t="s">
+      <c r="H21" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I21" s="15" t="s">
@@ -11379,8 +11379,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="22" s="19" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="17" t="n">
+    <row r="22" s="18" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="22" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="15" t="s">
@@ -11398,10 +11398,10 @@
       <c r="F22" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="G22" s="17" t="s">
+      <c r="G22" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I22" s="15" t="s">
@@ -11411,8 +11411,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="23" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="17" t="n">
+    <row r="23" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="22" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
@@ -11430,10 +11430,10 @@
       <c r="F23" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G23" s="17" t="s">
+      <c r="G23" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H23" s="17" t="s">
+      <c r="H23" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I23" s="15" t="s">
@@ -11443,8 +11443,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="24" s="19" customFormat="true" ht="318.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="17" t="n">
+    <row r="24" s="18" customFormat="true" ht="318.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="22" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
@@ -11462,10 +11462,10 @@
       <c r="F24" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G24" s="17" t="s">
+      <c r="G24" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H24" s="17" t="s">
+      <c r="H24" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I24" s="15" t="s">
@@ -11475,8 +11475,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="25" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="17" t="n">
+    <row r="25" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="22" t="n">
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
@@ -11494,10 +11494,10 @@
       <c r="F25" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G25" s="17" t="s">
+      <c r="G25" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="H25" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I25" s="15" t="s">
@@ -11507,8 +11507,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="26" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="17" t="n">
+    <row r="26" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="22" t="n">
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
@@ -11526,10 +11526,10 @@
       <c r="F26" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G26" s="17" t="s">
+      <c r="G26" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H26" s="17" t="s">
+      <c r="H26" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I26" s="15" t="s">
@@ -11539,8 +11539,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="27" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="17" t="n">
+    <row r="27" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="22" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
@@ -11558,10 +11558,10 @@
       <c r="F27" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H27" s="17" t="s">
+      <c r="H27" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I27" s="15" t="s">
@@ -11571,8 +11571,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="28" s="19" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="17" t="n">
+    <row r="28" s="18" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="22" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
@@ -11590,10 +11590,10 @@
       <c r="F28" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="G28" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="H28" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I28" s="15" t="s">
@@ -11603,8 +11603,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="29" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="17" t="n">
+    <row r="29" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="22" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="15" t="s">
@@ -11622,10 +11622,10 @@
       <c r="F29" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G29" s="17" t="s">
+      <c r="G29" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H29" s="17" t="s">
+      <c r="H29" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I29" s="15" t="s">
@@ -11635,8 +11635,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="30" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="17" t="n">
+    <row r="30" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="22" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
@@ -11654,10 +11654,10 @@
       <c r="F30" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="G30" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H30" s="17" t="s">
+      <c r="H30" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I30" s="15" t="s">
@@ -11667,8 +11667,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="31" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="17" t="n">
+    <row r="31" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="22" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="15" t="s">
@@ -11686,10 +11686,10 @@
       <c r="F31" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G31" s="17" t="s">
+      <c r="G31" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="H31" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I31" s="15" t="s">
@@ -11699,8 +11699,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="32" s="19" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="17" t="n">
+    <row r="32" s="18" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="22" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="15" t="s">
@@ -11718,10 +11718,10 @@
       <c r="F32" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G32" s="17" t="s">
+      <c r="G32" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I32" s="15" t="s">
@@ -11731,8 +11731,8 @@
         <v>299</v>
       </c>
     </row>
-    <row r="33" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="17" t="n">
+    <row r="33" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="22" t="n">
         <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
@@ -11750,10 +11750,10 @@
       <c r="F33" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G33" s="17" t="s">
+      <c r="G33" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H33" s="17" t="s">
+      <c r="H33" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I33" s="15" t="s">
@@ -11764,8 +11764,8 @@
       </c>
       <c r="K33" s="24"/>
     </row>
-    <row r="34" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="17" t="n">
+    <row r="34" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="22" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="15" t="s">
@@ -11783,10 +11783,10 @@
       <c r="F34" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G34" s="17" t="s">
+      <c r="G34" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H34" s="17" t="s">
+      <c r="H34" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I34" s="15" t="s">
@@ -11797,8 +11797,8 @@
       </c>
       <c r="K34" s="24"/>
     </row>
-    <row r="35" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="17" t="n">
+    <row r="35" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="22" t="n">
         <v>34</v>
       </c>
       <c r="B35" s="15" t="s">
@@ -11816,10 +11816,10 @@
       <c r="F35" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G35" s="17" t="s">
+      <c r="G35" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H35" s="17" t="s">
+      <c r="H35" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I35" s="15" t="s">
@@ -11830,8 +11830,8 @@
       </c>
       <c r="K35" s="24"/>
     </row>
-    <row r="36" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="17" t="n">
+    <row r="36" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="22" t="n">
         <v>35</v>
       </c>
       <c r="B36" s="15" t="s">
@@ -11849,10 +11849,10 @@
       <c r="F36" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G36" s="17" t="s">
+      <c r="G36" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H36" s="17" t="s">
+      <c r="H36" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I36" s="15" t="s">
@@ -11863,8 +11863,8 @@
       </c>
       <c r="K36" s="24"/>
     </row>
-    <row r="37" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="17" t="n">
+    <row r="37" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="22" t="n">
         <v>36</v>
       </c>
       <c r="B37" s="15" t="s">
@@ -11882,10 +11882,10 @@
       <c r="F37" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G37" s="17" t="s">
+      <c r="G37" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H37" s="17" t="s">
+      <c r="H37" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I37" s="15" t="s">
@@ -11896,8 +11896,8 @@
       </c>
       <c r="K37" s="24"/>
     </row>
-    <row r="38" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="17" t="n">
+    <row r="38" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="22" t="n">
         <v>37</v>
       </c>
       <c r="B38" s="15" t="s">
@@ -11915,10 +11915,10 @@
       <c r="F38" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G38" s="17" t="s">
+      <c r="G38" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H38" s="17" t="s">
+      <c r="H38" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I38" s="15" t="s">
@@ -11929,8 +11929,8 @@
       </c>
       <c r="K38" s="24"/>
     </row>
-    <row r="39" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="17" t="n">
+    <row r="39" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="22" t="n">
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
@@ -11948,10 +11948,10 @@
       <c r="F39" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G39" s="17" t="s">
+      <c r="G39" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H39" s="17" t="s">
+      <c r="H39" s="22" t="s">
         <v>265</v>
       </c>
       <c r="I39" s="15" t="s">
@@ -11962,8 +11962,8 @@
       </c>
       <c r="K39" s="24"/>
     </row>
-    <row r="40" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="17" t="n">
+    <row r="40" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="22" t="n">
         <v>39</v>
       </c>
       <c r="B40" s="15" t="s">
@@ -11981,10 +11981,10 @@
       <c r="F40" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="G40" s="17" t="s">
+      <c r="G40" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="H40" s="22" t="s">
         <v>359</v>
       </c>
       <c r="I40" s="15" t="s">
@@ -11995,8 +11995,8 @@
       </c>
       <c r="K40" s="24"/>
     </row>
-    <row r="41" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="17" t="n">
+    <row r="41" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="22" t="n">
         <v>40</v>
       </c>
       <c r="B41" s="15" t="s">
@@ -12014,10 +12014,10 @@
       <c r="F41" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="G41" s="17" t="s">
+      <c r="G41" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H41" s="17" t="s">
+      <c r="H41" s="22" t="s">
         <v>359</v>
       </c>
       <c r="I41" s="15" t="s">
@@ -12028,8 +12028,8 @@
       </c>
       <c r="K41" s="24"/>
     </row>
-    <row r="42" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="17" t="n">
+    <row r="42" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="22" t="n">
         <v>41</v>
       </c>
       <c r="B42" s="15" t="s">
@@ -12047,10 +12047,10 @@
       <c r="F42" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="G42" s="17" t="s">
+      <c r="G42" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H42" s="17" t="s">
+      <c r="H42" s="22" t="s">
         <v>359</v>
       </c>
       <c r="I42" s="15" t="s">
@@ -12061,8 +12061,8 @@
       </c>
       <c r="K42" s="24"/>
     </row>
-    <row r="43" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="17" t="n">
+    <row r="43" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="22" t="n">
         <v>42</v>
       </c>
       <c r="B43" s="15" t="s">
@@ -12080,10 +12080,10 @@
       <c r="F43" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G43" s="17" t="s">
+      <c r="G43" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H43" s="17" t="s">
+      <c r="H43" s="22" t="s">
         <v>359</v>
       </c>
       <c r="I43" s="15" t="s">
@@ -12094,8 +12094,8 @@
       </c>
       <c r="K43" s="24"/>
     </row>
-    <row r="44" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="17" t="n">
+    <row r="44" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="22" t="n">
         <v>43</v>
       </c>
       <c r="B44" s="15" t="s">
@@ -12113,10 +12113,10 @@
       <c r="F44" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G44" s="17" t="s">
+      <c r="G44" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H44" s="17" t="s">
+      <c r="H44" s="22" t="s">
         <v>359</v>
       </c>
       <c r="I44" s="15" t="s">
@@ -12127,8 +12127,8 @@
       </c>
       <c r="K44" s="24"/>
     </row>
-    <row r="45" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="17" t="n">
+    <row r="45" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="22" t="n">
         <v>44</v>
       </c>
       <c r="B45" s="15" t="s">
@@ -12146,10 +12146,10 @@
       <c r="F45" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G45" s="17" t="s">
+      <c r="G45" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H45" s="17" t="s">
+      <c r="H45" s="22" t="s">
         <v>359</v>
       </c>
       <c r="I45" s="15" t="s">
@@ -12160,8 +12160,8 @@
       </c>
       <c r="K45" s="24"/>
     </row>
-    <row r="46" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="17" t="n">
+    <row r="46" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="22" t="n">
         <v>45</v>
       </c>
       <c r="B46" s="15" t="s">
@@ -12179,10 +12179,10 @@
       <c r="F46" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="G46" s="17" t="s">
+      <c r="G46" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H46" s="17" t="s">
+      <c r="H46" s="22" t="s">
         <v>359</v>
       </c>
       <c r="I46" s="15" t="s">
@@ -12193,8 +12193,8 @@
       </c>
       <c r="K46" s="24"/>
     </row>
-    <row r="47" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="17" t="n">
+    <row r="47" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="22" t="n">
         <v>46</v>
       </c>
       <c r="B47" s="15" t="s">
@@ -12212,10 +12212,10 @@
       <c r="F47" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G47" s="17" t="s">
+      <c r="G47" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H47" s="17" t="s">
+      <c r="H47" s="22" t="s">
         <v>359</v>
       </c>
       <c r="I47" s="15" t="s">
@@ -12226,8 +12226,8 @@
       </c>
       <c r="K47" s="24"/>
     </row>
-    <row r="48" s="19" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="17" t="n">
+    <row r="48" s="18" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="22" t="n">
         <v>47</v>
       </c>
       <c r="B48" s="15" t="s">
@@ -12245,10 +12245,10 @@
       <c r="F48" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G48" s="17" t="s">
+      <c r="G48" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H48" s="17" t="s">
+      <c r="H48" s="22" t="s">
         <v>359</v>
       </c>
       <c r="I48" s="15" t="s">
@@ -12259,8 +12259,8 @@
       </c>
       <c r="K48" s="24"/>
     </row>
-    <row r="49" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="17" t="n">
+    <row r="49" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="22" t="n">
         <v>48</v>
       </c>
       <c r="B49" s="15" t="s">
@@ -12278,10 +12278,10 @@
       <c r="F49" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G49" s="17" t="s">
+      <c r="G49" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H49" s="17" t="s">
+      <c r="H49" s="22" t="s">
         <v>359</v>
       </c>
       <c r="I49" s="15" t="s">
@@ -12292,8 +12292,8 @@
       </c>
       <c r="K49" s="24"/>
     </row>
-    <row r="50" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="17" t="n">
+    <row r="50" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="22" t="n">
         <v>49</v>
       </c>
       <c r="B50" s="15" t="s">
@@ -12311,10 +12311,10 @@
       <c r="F50" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G50" s="17" t="s">
+      <c r="G50" s="22" t="s">
         <v>246</v>
       </c>
-      <c r="H50" s="17" t="s">
+      <c r="H50" s="22" t="s">
         <v>359</v>
       </c>
       <c r="I50" s="15" t="s">

</xml_diff>

<commit_message>
Make the text bold in column D
</commit_message>
<xml_diff>
--- a/Testing of the Registration Form.xlsx
+++ b/Testing of the Registration Form.xlsx
@@ -1822,7 +1822,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1891,6 +1891,10 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1899,7 +1903,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2031,10 +2035,10 @@
   <dimension ref="A1:B1021"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A83" activeCellId="1" sqref="D5:E91 A83"/>
+      <selection pane="topLeft" activeCell="A83" activeCellId="0" sqref="A83"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="43.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.13"/>
@@ -5531,11 +5535,11 @@
   </sheetPr>
   <dimension ref="A1:F1009"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A90" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5:E91"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.88"/>
@@ -5577,7 +5581,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" s="18" customFormat="true" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="5" s="19" customFormat="true" ht="50.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="14" t="n">
         <v>1</v>
       </c>
@@ -5590,9 +5594,9 @@
       <c r="D5" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E5" s="17"/>
-    </row>
-    <row r="6" s="18" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E5" s="18"/>
+    </row>
+    <row r="6" s="19" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="14" t="n">
         <v>2</v>
       </c>
@@ -5600,43 +5604,43 @@
         <v>68</v>
       </c>
       <c r="C6" s="14"/>
-      <c r="D6" s="19" t="s">
+      <c r="D6" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E6" s="20" t="n">
+      <c r="E6" s="21" t="n">
         <v>1</v>
       </c>
-      <c r="F6" s="21"/>
-    </row>
-    <row r="7" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="14" t="n">
         <v>3</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="C7" s="22"/>
+      <c r="C7" s="23"/>
       <c r="D7" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E7" s="23"/>
-    </row>
-    <row r="8" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E7" s="24"/>
+    </row>
+    <row r="8" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="14" t="n">
         <v>4</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>71</v>
       </c>
-      <c r="C8" s="22"/>
-      <c r="D8" s="19" t="s">
+      <c r="C8" s="23"/>
+      <c r="D8" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E8" s="20" t="n">
+      <c r="E8" s="21" t="n">
         <v>3</v>
       </c>
     </row>
-    <row r="9" s="18" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="9" s="19" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="14" t="n">
         <v>5</v>
       </c>
@@ -5644,14 +5648,14 @@
         <v>72</v>
       </c>
       <c r="C9" s="14"/>
-      <c r="D9" s="19" t="s">
+      <c r="D9" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E9" s="20" t="n">
+      <c r="E9" s="21" t="n">
         <v>4</v>
       </c>
     </row>
-    <row r="10" s="18" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="10" s="19" customFormat="true" ht="48.15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="14" t="n">
         <v>6</v>
       </c>
@@ -5662,9 +5666,9 @@
       <c r="D10" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E10" s="17"/>
-    </row>
-    <row r="11" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E10" s="18"/>
+    </row>
+    <row r="11" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="14" t="n">
         <v>7</v>
       </c>
@@ -5675,9 +5679,9 @@
       <c r="D11" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E11" s="17"/>
-    </row>
-    <row r="12" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E11" s="18"/>
+    </row>
+    <row r="12" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="14" t="n">
         <v>8</v>
       </c>
@@ -5688,9 +5692,9 @@
       <c r="D12" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E12" s="17"/>
-    </row>
-    <row r="13" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E12" s="18"/>
+    </row>
+    <row r="13" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="14" t="n">
         <v>9</v>
       </c>
@@ -5703,9 +5707,9 @@
       <c r="D13" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E13" s="17"/>
-    </row>
-    <row r="14" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E13" s="18"/>
+    </row>
+    <row r="14" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="14" t="n">
         <v>10</v>
       </c>
@@ -5715,14 +5719,14 @@
       <c r="C14" s="15" t="s">
         <v>77</v>
       </c>
-      <c r="D14" s="19" t="s">
+      <c r="D14" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E14" s="20" t="n">
+      <c r="E14" s="21" t="n">
         <v>5</v>
       </c>
     </row>
-    <row r="15" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="15" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="14" t="n">
         <v>11</v>
       </c>
@@ -5733,9 +5737,9 @@
       <c r="D15" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E15" s="17"/>
-    </row>
-    <row r="16" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E15" s="18"/>
+    </row>
+    <row r="16" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="14" t="n">
         <v>12</v>
       </c>
@@ -5748,9 +5752,9 @@
       <c r="D16" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E16" s="17"/>
-    </row>
-    <row r="17" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E16" s="18"/>
+    </row>
+    <row r="17" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="14" t="n">
         <v>13</v>
       </c>
@@ -5763,9 +5767,9 @@
       <c r="D17" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E17" s="17"/>
-    </row>
-    <row r="18" s="18" customFormat="true" ht="98.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E17" s="18"/>
+    </row>
+    <row r="18" s="19" customFormat="true" ht="98.9" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="14" t="n">
         <v>14</v>
       </c>
@@ -5775,15 +5779,15 @@
       <c r="C18" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="D18" s="19" t="s">
+      <c r="D18" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E18" s="20" t="n">
+      <c r="E18" s="21" t="n">
         <v>6</v>
       </c>
-      <c r="F18" s="24"/>
-    </row>
-    <row r="19" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F18" s="25"/>
+    </row>
+    <row r="19" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="14" t="n">
         <v>15</v>
       </c>
@@ -5796,10 +5800,10 @@
       <c r="D19" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E19" s="17"/>
-      <c r="F19" s="24"/>
-    </row>
-    <row r="20" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E19" s="18"/>
+      <c r="F19" s="25"/>
+    </row>
+    <row r="20" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="14" t="n">
         <v>16</v>
       </c>
@@ -5809,15 +5813,15 @@
       <c r="C20" s="15" t="s">
         <v>89</v>
       </c>
-      <c r="D20" s="19" t="s">
+      <c r="D20" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E20" s="20" t="n">
+      <c r="E20" s="21" t="n">
         <v>7</v>
       </c>
-      <c r="F20" s="24"/>
-    </row>
-    <row r="21" s="18" customFormat="true" ht="200.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F20" s="25"/>
+    </row>
+    <row r="21" s="19" customFormat="true" ht="200.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="14" t="n">
         <v>17</v>
       </c>
@@ -5827,15 +5831,15 @@
       <c r="C21" s="15" t="s">
         <v>91</v>
       </c>
-      <c r="D21" s="19" t="s">
+      <c r="D21" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E21" s="20" t="n">
+      <c r="E21" s="21" t="n">
         <v>8</v>
       </c>
-      <c r="F21" s="24"/>
-    </row>
-    <row r="22" s="18" customFormat="true" ht="200.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F21" s="25"/>
+    </row>
+    <row r="22" s="19" customFormat="true" ht="200.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="14" t="n">
         <v>18</v>
       </c>
@@ -5848,10 +5852,10 @@
       <c r="D22" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="17"/>
-      <c r="F22" s="24"/>
-    </row>
-    <row r="23" s="18" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E22" s="18"/>
+      <c r="F22" s="25"/>
+    </row>
+    <row r="23" s="19" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="14" t="n">
         <v>19</v>
       </c>
@@ -5861,15 +5865,15 @@
       <c r="C23" s="15" t="s">
         <v>95</v>
       </c>
-      <c r="D23" s="19" t="s">
+      <c r="D23" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E23" s="20" t="n">
+      <c r="E23" s="21" t="n">
         <v>9</v>
       </c>
-      <c r="F23" s="24"/>
-    </row>
-    <row r="24" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F23" s="25"/>
+    </row>
+    <row r="24" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="14" t="n">
         <v>20</v>
       </c>
@@ -5879,14 +5883,14 @@
       <c r="C24" s="15" t="s">
         <v>97</v>
       </c>
-      <c r="D24" s="19" t="s">
+      <c r="D24" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E24" s="20" t="n">
+      <c r="E24" s="21" t="n">
         <v>10</v>
       </c>
     </row>
-    <row r="25" s="18" customFormat="true" ht="162.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="25" s="19" customFormat="true" ht="162.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="14" t="n">
         <v>21</v>
       </c>
@@ -5899,9 +5903,9 @@
       <c r="D25" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="17"/>
-    </row>
-    <row r="26" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E25" s="18"/>
+    </row>
+    <row r="26" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="14" t="n">
         <v>22</v>
       </c>
@@ -5914,10 +5918,10 @@
       <c r="D26" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="17"/>
-      <c r="F26" s="24"/>
-    </row>
-    <row r="27" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E26" s="18"/>
+      <c r="F26" s="25"/>
+    </row>
+    <row r="27" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="14" t="n">
         <v>23</v>
       </c>
@@ -5927,15 +5931,15 @@
       <c r="C27" s="15" t="s">
         <v>103</v>
       </c>
-      <c r="D27" s="19" t="s">
+      <c r="D27" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E27" s="20" t="n">
+      <c r="E27" s="21" t="n">
         <v>11</v>
       </c>
-      <c r="F27" s="24"/>
-    </row>
-    <row r="28" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F27" s="25"/>
+    </row>
+    <row r="28" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="14" t="n">
         <v>24</v>
       </c>
@@ -5948,10 +5952,10 @@
       <c r="D28" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="17"/>
-      <c r="F28" s="24"/>
-    </row>
-    <row r="29" s="18" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E28" s="18"/>
+      <c r="F28" s="25"/>
+    </row>
+    <row r="29" s="19" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="14" t="n">
         <v>25</v>
       </c>
@@ -5964,10 +5968,10 @@
       <c r="D29" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="17"/>
-      <c r="F29" s="24"/>
-    </row>
-    <row r="30" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E29" s="18"/>
+      <c r="F29" s="25"/>
+    </row>
+    <row r="30" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="14" t="n">
         <v>26</v>
       </c>
@@ -5980,10 +5984,10 @@
       <c r="D30" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E30" s="17"/>
-      <c r="F30" s="24"/>
-    </row>
-    <row r="31" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E30" s="18"/>
+      <c r="F30" s="25"/>
+    </row>
+    <row r="31" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="14" t="n">
         <v>27</v>
       </c>
@@ -5996,10 +6000,10 @@
       <c r="D31" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="17"/>
-      <c r="F31" s="24"/>
-    </row>
-    <row r="32" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E31" s="18"/>
+      <c r="F31" s="25"/>
+    </row>
+    <row r="32" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="14" t="n">
         <v>28</v>
       </c>
@@ -6012,10 +6016,10 @@
       <c r="D32" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E32" s="17"/>
-      <c r="F32" s="24"/>
-    </row>
-    <row r="33" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E32" s="18"/>
+      <c r="F32" s="25"/>
+    </row>
+    <row r="33" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="14" t="n">
         <v>29</v>
       </c>
@@ -6028,10 +6032,10 @@
       <c r="D33" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E33" s="17"/>
-      <c r="F33" s="24"/>
-    </row>
-    <row r="34" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E33" s="18"/>
+      <c r="F33" s="25"/>
+    </row>
+    <row r="34" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="14" t="n">
         <v>30</v>
       </c>
@@ -6041,14 +6045,14 @@
       <c r="C34" s="15" t="s">
         <v>117</v>
       </c>
-      <c r="D34" s="19" t="s">
+      <c r="D34" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E34" s="20" t="n">
+      <c r="E34" s="21" t="n">
         <v>12</v>
       </c>
     </row>
-    <row r="35" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="35" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="14" t="n">
         <v>31</v>
       </c>
@@ -6061,10 +6065,10 @@
       <c r="D35" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E35" s="17"/>
-      <c r="F35" s="24"/>
-    </row>
-    <row r="36" s="18" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E35" s="18"/>
+      <c r="F35" s="25"/>
+    </row>
+    <row r="36" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="14" t="n">
         <v>32</v>
       </c>
@@ -6077,10 +6081,10 @@
       <c r="D36" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E36" s="17"/>
-      <c r="F36" s="24"/>
-    </row>
-    <row r="37" s="18" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E36" s="18"/>
+      <c r="F36" s="25"/>
+    </row>
+    <row r="37" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="14" t="n">
         <v>33</v>
       </c>
@@ -6090,15 +6094,15 @@
       <c r="C37" s="15" t="s">
         <v>123</v>
       </c>
-      <c r="D37" s="19" t="s">
+      <c r="D37" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E37" s="20" t="n">
+      <c r="E37" s="21" t="n">
         <v>13</v>
       </c>
-      <c r="F37" s="24"/>
-    </row>
-    <row r="38" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F37" s="25"/>
+    </row>
+    <row r="38" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="14" t="n">
         <v>34</v>
       </c>
@@ -6108,33 +6112,33 @@
       <c r="C38" s="15" t="s">
         <v>125</v>
       </c>
-      <c r="D38" s="19" t="s">
+      <c r="D38" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E38" s="20" t="n">
+      <c r="E38" s="21" t="n">
         <v>14</v>
       </c>
-      <c r="F38" s="24"/>
-    </row>
-    <row r="39" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F38" s="25"/>
+    </row>
+    <row r="39" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="14" t="n">
         <v>35</v>
       </c>
-      <c r="B39" s="25" t="s">
+      <c r="B39" s="26" t="s">
         <v>126</v>
       </c>
       <c r="C39" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="D39" s="19" t="s">
+      <c r="D39" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E39" s="20" t="n">
+      <c r="E39" s="21" t="n">
         <v>15</v>
       </c>
-      <c r="F39" s="24"/>
-    </row>
-    <row r="40" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F39" s="25"/>
+    </row>
+    <row r="40" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="14" t="n">
         <v>36</v>
       </c>
@@ -6144,15 +6148,15 @@
       <c r="C40" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="D40" s="19" t="s">
+      <c r="D40" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E40" s="20" t="n">
+      <c r="E40" s="21" t="n">
         <v>16</v>
       </c>
-      <c r="F40" s="24"/>
-    </row>
-    <row r="41" s="18" customFormat="true" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F40" s="25"/>
+    </row>
+    <row r="41" s="19" customFormat="true" ht="86.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="14" t="n">
         <v>37</v>
       </c>
@@ -6165,10 +6169,10 @@
       <c r="D41" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E41" s="23"/>
-      <c r="F41" s="24"/>
-    </row>
-    <row r="42" s="18" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E41" s="24"/>
+      <c r="F41" s="25"/>
+    </row>
+    <row r="42" s="19" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="14" t="n">
         <v>38</v>
       </c>
@@ -6181,10 +6185,10 @@
       <c r="D42" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E42" s="17"/>
-      <c r="F42" s="24"/>
-    </row>
-    <row r="43" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E42" s="18"/>
+      <c r="F42" s="25"/>
+    </row>
+    <row r="43" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="14" t="n">
         <v>39</v>
       </c>
@@ -6197,10 +6201,10 @@
       <c r="D43" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E43" s="17"/>
-      <c r="F43" s="24"/>
-    </row>
-    <row r="44" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E43" s="18"/>
+      <c r="F43" s="25"/>
+    </row>
+    <row r="44" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="14" t="n">
         <v>40</v>
       </c>
@@ -6213,9 +6217,9 @@
       <c r="D44" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E44" s="17"/>
-    </row>
-    <row r="45" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E44" s="18"/>
+    </row>
+    <row r="45" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="14" t="n">
         <v>41</v>
       </c>
@@ -6228,9 +6232,9 @@
       <c r="D45" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E45" s="17"/>
-    </row>
-    <row r="46" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E45" s="18"/>
+    </row>
+    <row r="46" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="14" t="n">
         <v>42</v>
       </c>
@@ -6243,10 +6247,10 @@
       <c r="D46" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E46" s="17"/>
-      <c r="F46" s="24"/>
-    </row>
-    <row r="47" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E46" s="18"/>
+      <c r="F46" s="25"/>
+    </row>
+    <row r="47" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="14" t="n">
         <v>43</v>
       </c>
@@ -6256,33 +6260,33 @@
       <c r="C47" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="D47" s="19" t="s">
+      <c r="D47" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E47" s="20" t="n">
+      <c r="E47" s="21" t="n">
         <v>17</v>
       </c>
-      <c r="F47" s="24"/>
-    </row>
-    <row r="48" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F47" s="25"/>
+    </row>
+    <row r="48" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="14" t="n">
         <v>44</v>
       </c>
       <c r="B48" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="27" t="s">
         <v>145</v>
       </c>
-      <c r="D48" s="19" t="s">
+      <c r="D48" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E48" s="20" t="n">
+      <c r="E48" s="21" t="n">
         <v>18</v>
       </c>
-      <c r="F48" s="24"/>
-    </row>
-    <row r="49" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="F48" s="25"/>
+    </row>
+    <row r="49" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="14" t="n">
         <v>45</v>
       </c>
@@ -6292,14 +6296,14 @@
       <c r="C49" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="D49" s="19" t="s">
+      <c r="D49" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E49" s="20" t="n">
+      <c r="E49" s="21" t="n">
         <v>19</v>
       </c>
     </row>
-    <row r="50" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="50" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="14" t="n">
         <v>46</v>
       </c>
@@ -6309,14 +6313,14 @@
       <c r="C50" s="15" t="s">
         <v>149</v>
       </c>
-      <c r="D50" s="19" t="s">
+      <c r="D50" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E50" s="20" t="n">
+      <c r="E50" s="21" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="51" s="18" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="51" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="14" t="n">
         <v>47</v>
       </c>
@@ -6326,14 +6330,14 @@
       <c r="C51" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="D51" s="19" t="s">
+      <c r="D51" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E51" s="20" t="n">
+      <c r="E51" s="21" t="n">
         <v>21</v>
       </c>
     </row>
-    <row r="52" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="52" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="14" t="n">
         <v>48</v>
       </c>
@@ -6343,14 +6347,14 @@
       <c r="C52" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="D52" s="19" t="s">
+      <c r="D52" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="20" t="n">
+      <c r="E52" s="21" t="n">
         <v>22</v>
       </c>
     </row>
-    <row r="53" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="53" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="14" t="n">
         <v>49</v>
       </c>
@@ -6363,9 +6367,9 @@
       <c r="D53" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E53" s="17"/>
-    </row>
-    <row r="54" s="18" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E53" s="18"/>
+    </row>
+    <row r="54" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="14" t="n">
         <v>50</v>
       </c>
@@ -6378,9 +6382,9 @@
       <c r="D54" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E54" s="17"/>
-    </row>
-    <row r="55" s="18" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E54" s="18"/>
+    </row>
+    <row r="55" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="14" t="n">
         <v>51</v>
       </c>
@@ -6390,14 +6394,14 @@
       <c r="C55" s="15" t="s">
         <v>159</v>
       </c>
-      <c r="D55" s="19" t="s">
+      <c r="D55" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E55" s="20" t="n">
+      <c r="E55" s="21" t="n">
         <v>23</v>
       </c>
     </row>
-    <row r="56" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="56" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="14" t="n">
         <v>52</v>
       </c>
@@ -6407,14 +6411,14 @@
       <c r="C56" s="15" t="s">
         <v>161</v>
       </c>
-      <c r="D56" s="19" t="s">
+      <c r="D56" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E56" s="20" t="n">
+      <c r="E56" s="21" t="n">
         <v>24</v>
       </c>
     </row>
-    <row r="57" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="57" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="14" t="n">
         <v>53</v>
       </c>
@@ -6424,14 +6428,14 @@
       <c r="C57" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="D57" s="19" t="s">
+      <c r="D57" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E57" s="20" t="n">
+      <c r="E57" s="21" t="n">
         <v>25</v>
       </c>
     </row>
-    <row r="58" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="58" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="14" t="n">
         <v>54</v>
       </c>
@@ -6441,14 +6445,14 @@
       <c r="C58" s="15" t="s">
         <v>165</v>
       </c>
-      <c r="D58" s="19" t="s">
+      <c r="D58" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E58" s="20" t="n">
+      <c r="E58" s="21" t="n">
         <v>26</v>
       </c>
     </row>
-    <row r="59" s="18" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="59" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="14" t="n">
         <v>55</v>
       </c>
@@ -6458,14 +6462,14 @@
       <c r="C59" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="D59" s="19" t="s">
+      <c r="D59" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E59" s="20" t="n">
+      <c r="E59" s="21" t="n">
         <v>27</v>
       </c>
     </row>
-    <row r="60" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="60" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="14" t="n">
         <v>56</v>
       </c>
@@ -6478,9 +6482,9 @@
       <c r="D60" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E60" s="17"/>
-    </row>
-    <row r="61" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E60" s="18"/>
+    </row>
+    <row r="61" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="14" t="n">
         <v>57</v>
       </c>
@@ -6490,14 +6494,14 @@
       <c r="C61" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="D61" s="19" t="s">
+      <c r="D61" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E61" s="20" t="n">
+      <c r="E61" s="21" t="n">
         <v>28</v>
       </c>
     </row>
-    <row r="62" s="18" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="62" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="14" t="n">
         <v>58</v>
       </c>
@@ -6510,9 +6514,9 @@
       <c r="D62" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E62" s="17"/>
-    </row>
-    <row r="63" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E62" s="18"/>
+    </row>
+    <row r="63" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="14" t="n">
         <v>59</v>
       </c>
@@ -6522,14 +6526,14 @@
       <c r="C63" s="15" t="s">
         <v>175</v>
       </c>
-      <c r="D63" s="19" t="s">
+      <c r="D63" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E63" s="20" t="n">
+      <c r="E63" s="21" t="n">
         <v>29</v>
       </c>
     </row>
-    <row r="64" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="64" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="14" t="n">
         <v>60</v>
       </c>
@@ -6539,14 +6543,14 @@
       <c r="C64" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="D64" s="19" t="s">
+      <c r="D64" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E64" s="20" t="n">
+      <c r="E64" s="21" t="n">
         <v>30</v>
       </c>
     </row>
-    <row r="65" s="18" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="65" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="14" t="n">
         <v>61</v>
       </c>
@@ -6556,14 +6560,14 @@
       <c r="C65" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="D65" s="19" t="s">
+      <c r="D65" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E65" s="20" t="n">
+      <c r="E65" s="21" t="n">
         <v>31</v>
       </c>
     </row>
-    <row r="66" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="66" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="14" t="n">
         <v>62</v>
       </c>
@@ -6573,14 +6577,14 @@
       <c r="C66" s="15" t="s">
         <v>181</v>
       </c>
-      <c r="D66" s="19" t="s">
+      <c r="D66" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E66" s="20" t="n">
+      <c r="E66" s="21" t="n">
         <v>32</v>
       </c>
     </row>
-    <row r="67" s="18" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="67" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="14" t="n">
         <v>63</v>
       </c>
@@ -6593,9 +6597,9 @@
       <c r="D67" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E67" s="17"/>
-    </row>
-    <row r="68" s="18" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E67" s="18"/>
+    </row>
+    <row r="68" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="14" t="n">
         <v>64</v>
       </c>
@@ -6608,9 +6612,9 @@
       <c r="D68" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E68" s="17"/>
-    </row>
-    <row r="69" s="18" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E68" s="18"/>
+    </row>
+    <row r="69" s="19" customFormat="true" ht="187.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="14" t="n">
         <v>65</v>
       </c>
@@ -6620,14 +6624,14 @@
       <c r="C69" s="15" t="s">
         <v>187</v>
       </c>
-      <c r="D69" s="19" t="s">
+      <c r="D69" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E69" s="20" t="n">
+      <c r="E69" s="21" t="n">
         <v>33</v>
       </c>
     </row>
-    <row r="70" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="70" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="14" t="n">
         <v>66</v>
       </c>
@@ -6640,9 +6644,9 @@
       <c r="D70" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E70" s="17"/>
-    </row>
-    <row r="71" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E70" s="18"/>
+    </row>
+    <row r="71" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="14" t="n">
         <v>67</v>
       </c>
@@ -6652,14 +6656,14 @@
       <c r="C71" s="15" t="s">
         <v>191</v>
       </c>
-      <c r="D71" s="19" t="s">
+      <c r="D71" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E71" s="20" t="n">
+      <c r="E71" s="21" t="n">
         <v>34</v>
       </c>
     </row>
-    <row r="72" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="72" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A72" s="14" t="n">
         <v>68</v>
       </c>
@@ -6669,14 +6673,14 @@
       <c r="C72" s="15" t="s">
         <v>193</v>
       </c>
-      <c r="D72" s="19" t="s">
+      <c r="D72" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E72" s="20" t="n">
+      <c r="E72" s="21" t="n">
         <v>35</v>
       </c>
     </row>
-    <row r="73" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="73" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A73" s="14" t="n">
         <v>69</v>
       </c>
@@ -6689,9 +6693,9 @@
       <c r="D73" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E73" s="17"/>
-    </row>
-    <row r="74" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E73" s="18"/>
+    </row>
+    <row r="74" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A74" s="14" t="n">
         <v>70</v>
       </c>
@@ -6701,14 +6705,14 @@
       <c r="C74" s="15" t="s">
         <v>197</v>
       </c>
-      <c r="D74" s="19" t="s">
+      <c r="D74" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E74" s="20" t="n">
+      <c r="E74" s="21" t="n">
         <v>36</v>
       </c>
     </row>
-    <row r="75" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="75" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A75" s="14" t="n">
         <v>71</v>
       </c>
@@ -6721,9 +6725,9 @@
       <c r="D75" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E75" s="17"/>
-    </row>
-    <row r="76" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E75" s="18"/>
+    </row>
+    <row r="76" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A76" s="14" t="n">
         <v>72</v>
       </c>
@@ -6733,14 +6737,14 @@
       <c r="C76" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="D76" s="19" t="s">
+      <c r="D76" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E76" s="20" t="n">
+      <c r="E76" s="21" t="n">
         <v>37</v>
       </c>
     </row>
-    <row r="77" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="77" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A77" s="14" t="n">
         <v>73</v>
       </c>
@@ -6750,14 +6754,14 @@
       <c r="C77" s="15" t="s">
         <v>203</v>
       </c>
-      <c r="D77" s="19" t="s">
+      <c r="D77" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E77" s="20" t="n">
+      <c r="E77" s="21" t="n">
         <v>38</v>
       </c>
     </row>
-    <row r="78" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="78" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A78" s="14" t="n">
         <v>74</v>
       </c>
@@ -6770,24 +6774,24 @@
       <c r="D78" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E78" s="17"/>
-      <c r="F78" s="24"/>
-    </row>
-    <row r="79" s="18" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E78" s="18"/>
+      <c r="F78" s="25"/>
+    </row>
+    <row r="79" s="19" customFormat="true" ht="60.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A79" s="14" t="n">
         <v>75</v>
       </c>
       <c r="B79" s="15" t="s">
         <v>206</v>
       </c>
-      <c r="C79" s="22"/>
+      <c r="C79" s="23"/>
       <c r="D79" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E79" s="17"/>
-      <c r="F79" s="24"/>
-    </row>
-    <row r="80" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E79" s="18"/>
+      <c r="F79" s="25"/>
+    </row>
+    <row r="80" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A80" s="14" t="n">
         <v>76</v>
       </c>
@@ -6797,17 +6801,17 @@
       <c r="C80" s="15" t="s">
         <v>208</v>
       </c>
-      <c r="D80" s="19" t="s">
+      <c r="D80" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E80" s="20" t="n">
+      <c r="E80" s="21" t="n">
         <v>39</v>
       </c>
-      <c r="F80" s="27" t="s">
+      <c r="F80" s="28" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="81" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="81" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A81" s="14" t="n">
         <v>77</v>
       </c>
@@ -6817,14 +6821,14 @@
       <c r="C81" s="15" t="s">
         <v>211</v>
       </c>
-      <c r="D81" s="19" t="s">
+      <c r="D81" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E81" s="20" t="n">
+      <c r="E81" s="21" t="n">
         <v>40</v>
       </c>
     </row>
-    <row r="82" s="18" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="82" s="19" customFormat="true" ht="149.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A82" s="14" t="n">
         <v>78</v>
       </c>
@@ -6837,9 +6841,9 @@
       <c r="D82" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="E82" s="17"/>
-    </row>
-    <row r="83" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="E82" s="18"/>
+    </row>
+    <row r="83" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A83" s="14" t="n">
         <v>79</v>
       </c>
@@ -6849,14 +6853,14 @@
       <c r="C83" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="D83" s="19" t="s">
+      <c r="D83" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E83" s="20" t="n">
+      <c r="E83" s="21" t="n">
         <v>41</v>
       </c>
     </row>
-    <row r="84" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="84" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A84" s="14" t="n">
         <v>80</v>
       </c>
@@ -6866,14 +6870,14 @@
       <c r="C84" s="15" t="s">
         <v>217</v>
       </c>
-      <c r="D84" s="19" t="s">
+      <c r="D84" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E84" s="20" t="n">
+      <c r="E84" s="21" t="n">
         <v>42</v>
       </c>
     </row>
-    <row r="85" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="85" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A85" s="14" t="n">
         <v>81</v>
       </c>
@@ -6883,14 +6887,14 @@
       <c r="C85" s="15" t="s">
         <v>219</v>
       </c>
-      <c r="D85" s="19" t="s">
+      <c r="D85" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E85" s="20" t="n">
+      <c r="E85" s="21" t="n">
         <v>43</v>
       </c>
     </row>
-    <row r="86" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="86" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A86" s="14" t="n">
         <v>82</v>
       </c>
@@ -6900,14 +6904,14 @@
       <c r="C86" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="D86" s="19" t="s">
+      <c r="D86" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E86" s="20" t="n">
+      <c r="E86" s="21" t="n">
         <v>44</v>
       </c>
     </row>
-    <row r="87" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="87" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A87" s="14" t="n">
         <v>83</v>
       </c>
@@ -6917,14 +6921,14 @@
       <c r="C87" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="D87" s="19" t="s">
+      <c r="D87" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E87" s="20" t="n">
+      <c r="E87" s="21" t="n">
         <v>45</v>
       </c>
     </row>
-    <row r="88" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="88" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A88" s="14" t="n">
         <v>84</v>
       </c>
@@ -6934,14 +6938,14 @@
       <c r="C88" s="15" t="s">
         <v>225</v>
       </c>
-      <c r="D88" s="19" t="s">
+      <c r="D88" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E88" s="20" t="n">
+      <c r="E88" s="21" t="n">
         <v>46</v>
       </c>
     </row>
-    <row r="89" s="18" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="89" s="19" customFormat="true" ht="111.6" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A89" s="14" t="n">
         <v>85</v>
       </c>
@@ -6951,14 +6955,14 @@
       <c r="C89" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="D89" s="19" t="s">
+      <c r="D89" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E89" s="20" t="n">
+      <c r="E89" s="21" t="n">
         <v>47</v>
       </c>
     </row>
-    <row r="90" s="18" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" s="19" customFormat="true" ht="124.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A90" s="14" t="n">
         <v>86</v>
       </c>
@@ -6968,14 +6972,14 @@
       <c r="C90" s="15" t="s">
         <v>229</v>
       </c>
-      <c r="D90" s="19" t="s">
+      <c r="D90" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E90" s="20" t="n">
+      <c r="E90" s="21" t="n">
         <v>48</v>
       </c>
     </row>
-    <row r="91" s="18" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="91" s="19" customFormat="true" ht="136.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A91" s="14" t="n">
         <v>87</v>
       </c>
@@ -6985,41 +6989,41 @@
       <c r="C91" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="D91" s="19" t="s">
+      <c r="D91" s="20" t="s">
         <v>69</v>
       </c>
-      <c r="E91" s="20" t="n">
+      <c r="E91" s="21" t="n">
         <v>49</v>
       </c>
     </row>
     <row r="94" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B94" s="6"/>
-      <c r="C94" s="24"/>
+      <c r="C94" s="25"/>
       <c r="E94" s="8"/>
     </row>
     <row r="95" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B95" s="6"/>
-      <c r="C95" s="24"/>
+      <c r="C95" s="25"/>
       <c r="E95" s="8"/>
     </row>
     <row r="96" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B96" s="6"/>
-      <c r="C96" s="24"/>
+      <c r="C96" s="25"/>
       <c r="E96" s="8"/>
     </row>
     <row r="97" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B97" s="6"/>
-      <c r="C97" s="24"/>
+      <c r="C97" s="25"/>
       <c r="E97" s="8"/>
     </row>
     <row r="98" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B98" s="6"/>
-      <c r="C98" s="24"/>
+      <c r="C98" s="25"/>
       <c r="E98" s="8"/>
     </row>
     <row r="99" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B99" s="6"/>
-      <c r="C99" s="24"/>
+      <c r="C99" s="25"/>
       <c r="E99" s="8"/>
     </row>
     <row r="100" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10695,57 +10699,57 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="H28" activeCellId="1" sqref="D5:E91 H28"/>
+      <selection pane="bottomLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="3.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="31.38"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="28" width="15.75"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="3" style="29" width="15.75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="0" width="15.75"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="14.15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="29" t="s">
+      <c r="A1" s="30" t="s">
         <v>232</v>
       </c>
-      <c r="B1" s="30" t="s">
+      <c r="B1" s="31" t="s">
         <v>233</v>
       </c>
-      <c r="C1" s="30" t="s">
+      <c r="C1" s="31" t="s">
         <v>234</v>
       </c>
-      <c r="D1" s="30" t="s">
+      <c r="D1" s="31" t="s">
         <v>235</v>
       </c>
-      <c r="E1" s="30" t="s">
+      <c r="E1" s="31" t="s">
         <v>236</v>
       </c>
-      <c r="F1" s="31" t="s">
+      <c r="F1" s="32" t="s">
         <v>237</v>
       </c>
-      <c r="G1" s="31" t="s">
+      <c r="G1" s="32" t="s">
         <v>238</v>
       </c>
-      <c r="H1" s="31" t="s">
+      <c r="H1" s="32" t="s">
         <v>239</v>
       </c>
-      <c r="I1" s="31" t="s">
+      <c r="I1" s="32" t="s">
         <v>240</v>
       </c>
-      <c r="J1" s="31" t="s">
+      <c r="J1" s="32" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="2" s="18" customFormat="true" ht="115.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="22" t="n">
+    <row r="2" s="19" customFormat="true" ht="115.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="23" t="n">
         <v>1</v>
       </c>
       <c r="B2" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="C2" s="26" t="s">
+      <c r="C2" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D2" s="15" t="s">
@@ -10757,27 +10761,27 @@
       <c r="F2" s="15" t="s">
         <v>245</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H2" s="22" t="s">
+      <c r="H2" s="23" t="s">
         <v>247</v>
       </c>
       <c r="I2" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J2" s="26" t="s">
+      <c r="J2" s="27" t="s">
         <v>249</v>
       </c>
     </row>
-    <row r="3" s="18" customFormat="true" ht="103.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="22" t="n">
+    <row r="3" s="19" customFormat="true" ht="103.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="23" t="n">
         <v>2</v>
       </c>
       <c r="B3" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D3" s="15" t="s">
@@ -10789,27 +10793,27 @@
       <c r="F3" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="G3" s="22" t="s">
+      <c r="G3" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H3" s="22" t="s">
+      <c r="H3" s="23" t="s">
         <v>247</v>
       </c>
       <c r="I3" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J3" s="26" t="s">
+      <c r="J3" s="27" t="s">
         <v>253</v>
       </c>
     </row>
-    <row r="4" s="18" customFormat="true" ht="103.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="22" t="n">
+    <row r="4" s="19" customFormat="true" ht="103.1" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="23" t="n">
         <v>3</v>
       </c>
       <c r="B4" s="15" t="s">
         <v>254</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="C4" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D4" s="15" t="s">
@@ -10821,27 +10825,27 @@
       <c r="F4" s="15" t="s">
         <v>256</v>
       </c>
-      <c r="G4" s="22" t="s">
+      <c r="G4" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H4" s="22" t="s">
+      <c r="H4" s="23" t="s">
         <v>247</v>
       </c>
       <c r="I4" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J4" s="26" t="s">
+      <c r="J4" s="27" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="5" s="18" customFormat="true" ht="115.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="22" t="n">
+    <row r="5" s="19" customFormat="true" ht="115.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="23" t="n">
         <v>4</v>
       </c>
       <c r="B5" s="15" t="s">
         <v>258</v>
       </c>
-      <c r="C5" s="26" t="s">
+      <c r="C5" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D5" s="15" t="s">
@@ -10853,27 +10857,27 @@
       <c r="F5" s="15" t="s">
         <v>260</v>
       </c>
-      <c r="G5" s="22" t="s">
+      <c r="G5" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H5" s="22" t="s">
+      <c r="H5" s="23" t="s">
         <v>247</v>
       </c>
       <c r="I5" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J5" s="26" t="s">
+      <c r="J5" s="27" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="6" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="22" t="n">
+    <row r="6" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A6" s="23" t="n">
         <v>5</v>
       </c>
       <c r="B6" s="15" t="s">
         <v>262</v>
       </c>
-      <c r="C6" s="26" t="s">
+      <c r="C6" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D6" s="15" t="s">
@@ -10885,27 +10889,27 @@
       <c r="F6" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="G6" s="22" t="s">
+      <c r="G6" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H6" s="22" t="s">
+      <c r="H6" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I6" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J6" s="26" t="s">
+      <c r="J6" s="27" t="s">
         <v>266</v>
       </c>
     </row>
-    <row r="7" s="18" customFormat="true" ht="217.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="22" t="n">
+    <row r="7" s="19" customFormat="true" ht="217.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="23" t="n">
         <v>6</v>
       </c>
       <c r="B7" s="15" t="s">
         <v>267</v>
       </c>
-      <c r="C7" s="26" t="s">
+      <c r="C7" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D7" s="15" t="s">
@@ -10917,27 +10921,27 @@
       <c r="F7" s="15" t="s">
         <v>269</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I7" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J7" s="26" t="s">
+      <c r="J7" s="27" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="8" s="18" customFormat="true" ht="229.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="22" t="n">
+    <row r="8" s="19" customFormat="true" ht="229.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A8" s="23" t="n">
         <v>7</v>
       </c>
       <c r="B8" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="C8" s="26" t="s">
+      <c r="C8" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D8" s="15" t="s">
@@ -10949,27 +10953,27 @@
       <c r="F8" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="G8" s="22" t="s">
+      <c r="G8" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H8" s="22" t="s">
+      <c r="H8" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I8" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J8" s="26" t="s">
+      <c r="J8" s="27" t="s">
         <v>275</v>
       </c>
     </row>
-    <row r="9" s="18" customFormat="true" ht="293.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="n">
+    <row r="9" s="19" customFormat="true" ht="293.4" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="23" t="n">
         <v>8</v>
       </c>
       <c r="B9" s="15" t="s">
         <v>276</v>
       </c>
-      <c r="C9" s="26" t="s">
+      <c r="C9" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D9" s="15" t="s">
@@ -10981,27 +10985,27 @@
       <c r="F9" s="15" t="s">
         <v>278</v>
       </c>
-      <c r="G9" s="22" t="s">
+      <c r="G9" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H9" s="22" t="s">
+      <c r="H9" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I9" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J9" s="26" t="s">
+      <c r="J9" s="27" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="10" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="n">
+    <row r="10" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="23" t="n">
         <v>9</v>
       </c>
       <c r="B10" s="15" t="s">
         <v>280</v>
       </c>
-      <c r="C10" s="26" t="s">
+      <c r="C10" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D10" s="15" t="s">
@@ -11013,27 +11017,27 @@
       <c r="F10" s="15" t="s">
         <v>282</v>
       </c>
-      <c r="G10" s="22" t="s">
+      <c r="G10" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H10" s="22" t="s">
+      <c r="H10" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I10" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J10" s="26" t="s">
+      <c r="J10" s="27" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="11" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="n">
+    <row r="11" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="23" t="n">
         <v>10</v>
       </c>
       <c r="B11" s="15" t="s">
         <v>284</v>
       </c>
-      <c r="C11" s="26" t="s">
+      <c r="C11" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D11" s="15" t="s">
@@ -11045,27 +11049,27 @@
       <c r="F11" s="15" t="s">
         <v>286</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H11" s="22" t="s">
+      <c r="H11" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I11" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J11" s="26" t="s">
+      <c r="J11" s="27" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="12" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="22" t="n">
+    <row r="12" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="23" t="n">
         <v>11</v>
       </c>
       <c r="B12" s="15" t="s">
         <v>288</v>
       </c>
-      <c r="C12" s="26" t="s">
+      <c r="C12" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D12" s="15" t="s">
@@ -11077,27 +11081,27 @@
       <c r="F12" s="15" t="s">
         <v>290</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H12" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I12" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J12" s="26" t="s">
+      <c r="J12" s="27" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="13" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="22" t="n">
+    <row r="13" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="23" t="n">
         <v>12</v>
       </c>
       <c r="B13" s="15" t="s">
         <v>292</v>
       </c>
-      <c r="C13" s="26" t="s">
+      <c r="C13" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D13" s="15" t="s">
@@ -11109,27 +11113,27 @@
       <c r="F13" s="15" t="s">
         <v>294</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I13" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J13" s="26" t="s">
+      <c r="J13" s="27" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="14" s="18" customFormat="true" ht="331.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="22" t="n">
+    <row r="14" s="19" customFormat="true" ht="331.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A14" s="23" t="n">
         <v>13</v>
       </c>
       <c r="B14" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="C14" s="26" t="s">
+      <c r="C14" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D14" s="15" t="s">
@@ -11141,27 +11145,27 @@
       <c r="F14" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="G14" s="22" t="s">
+      <c r="G14" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H14" s="22" t="s">
+      <c r="H14" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I14" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J14" s="26" t="s">
+      <c r="J14" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="15" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="22" t="n">
+    <row r="15" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A15" s="23" t="n">
         <v>14</v>
       </c>
       <c r="B15" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="C15" s="26" t="s">
+      <c r="C15" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D15" s="15" t="s">
@@ -11173,28 +11177,28 @@
       <c r="F15" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="G15" s="22" t="s">
+      <c r="G15" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H15" s="22" t="s">
+      <c r="H15" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I15" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J15" s="26" t="s">
+      <c r="J15" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K15" s="24"/>
-    </row>
-    <row r="16" s="18" customFormat="true" ht="280.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="22" t="n">
+      <c r="K15" s="25"/>
+    </row>
+    <row r="16" s="19" customFormat="true" ht="280.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A16" s="23" t="n">
         <v>15</v>
       </c>
       <c r="B16" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="C16" s="26" t="s">
+      <c r="C16" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D16" s="15" t="s">
@@ -11206,27 +11210,27 @@
       <c r="F16" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H16" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I16" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J16" s="26" t="s">
+      <c r="J16" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="17" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="22" t="n">
+    <row r="17" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="23" t="n">
         <v>16</v>
       </c>
       <c r="B17" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="C17" s="26" t="s">
+      <c r="C17" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D17" s="15" t="s">
@@ -11238,27 +11242,27 @@
       <c r="F17" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H17" s="22" t="s">
+      <c r="H17" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I17" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J17" s="26" t="s">
+      <c r="J17" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="18" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="22" t="n">
+    <row r="18" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="23" t="n">
         <v>17</v>
       </c>
       <c r="B18" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="C18" s="26" t="s">
+      <c r="C18" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D18" s="15" t="s">
@@ -11270,27 +11274,27 @@
       <c r="F18" s="15" t="s">
         <v>309</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H18" s="22" t="s">
+      <c r="H18" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I18" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J18" s="26" t="s">
+      <c r="J18" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="19" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="22" t="n">
+    <row r="19" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A19" s="23" t="n">
         <v>18</v>
       </c>
       <c r="B19" s="15" t="s">
         <v>310</v>
       </c>
-      <c r="C19" s="26" t="s">
+      <c r="C19" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D19" s="15" t="s">
@@ -11302,27 +11306,27 @@
       <c r="F19" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="G19" s="22" t="s">
+      <c r="G19" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H19" s="22" t="s">
+      <c r="H19" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I19" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J19" s="26" t="s">
+      <c r="J19" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="20" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A20" s="22" t="n">
+    <row r="20" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A20" s="23" t="n">
         <v>19</v>
       </c>
       <c r="B20" s="15" t="s">
         <v>313</v>
       </c>
-      <c r="C20" s="26" t="s">
+      <c r="C20" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D20" s="15" t="s">
@@ -11334,27 +11338,27 @@
       <c r="F20" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="G20" s="22" t="s">
+      <c r="G20" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H20" s="22" t="s">
+      <c r="H20" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I20" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J20" s="26" t="s">
+      <c r="J20" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="21" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A21" s="22" t="n">
+    <row r="21" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="23" t="n">
         <v>20</v>
       </c>
       <c r="B21" s="15" t="s">
         <v>315</v>
       </c>
-      <c r="C21" s="26" t="s">
+      <c r="C21" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D21" s="15" t="s">
@@ -11366,27 +11370,27 @@
       <c r="F21" s="15" t="s">
         <v>317</v>
       </c>
-      <c r="G21" s="22" t="s">
+      <c r="G21" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H21" s="22" t="s">
+      <c r="H21" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I21" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J21" s="26" t="s">
+      <c r="J21" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="22" s="18" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A22" s="22" t="n">
+    <row r="22" s="19" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="23" t="n">
         <v>21</v>
       </c>
       <c r="B22" s="15" t="s">
         <v>318</v>
       </c>
-      <c r="C22" s="26" t="s">
+      <c r="C22" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D22" s="15" t="s">
@@ -11398,27 +11402,27 @@
       <c r="F22" s="15" t="s">
         <v>312</v>
       </c>
-      <c r="G22" s="22" t="s">
+      <c r="G22" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H22" s="22" t="s">
+      <c r="H22" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I22" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J22" s="26" t="s">
+      <c r="J22" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="23" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A23" s="22" t="n">
+    <row r="23" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="23" t="n">
         <v>22</v>
       </c>
       <c r="B23" s="15" t="s">
         <v>321</v>
       </c>
-      <c r="C23" s="26" t="s">
+      <c r="C23" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D23" s="15" t="s">
@@ -11430,27 +11434,27 @@
       <c r="F23" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G23" s="22" t="s">
+      <c r="G23" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H23" s="22" t="s">
+      <c r="H23" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I23" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J23" s="26" t="s">
+      <c r="J23" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="24" s="18" customFormat="true" ht="318.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A24" s="22" t="n">
+    <row r="24" s="19" customFormat="true" ht="318.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="23" t="n">
         <v>23</v>
       </c>
       <c r="B24" s="15" t="s">
         <v>324</v>
       </c>
-      <c r="C24" s="26" t="s">
+      <c r="C24" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D24" s="15" t="s">
@@ -11462,27 +11466,27 @@
       <c r="F24" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G24" s="22" t="s">
+      <c r="G24" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H24" s="22" t="s">
+      <c r="H24" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I24" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J24" s="26" t="s">
+      <c r="J24" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="25" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A25" s="22" t="n">
+    <row r="25" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A25" s="23" t="n">
         <v>24</v>
       </c>
       <c r="B25" s="15" t="s">
         <v>326</v>
       </c>
-      <c r="C25" s="26" t="s">
+      <c r="C25" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D25" s="15" t="s">
@@ -11494,27 +11498,27 @@
       <c r="F25" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G25" s="22" t="s">
+      <c r="G25" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H25" s="22" t="s">
+      <c r="H25" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I25" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J25" s="26" t="s">
+      <c r="J25" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="26" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A26" s="22" t="n">
+    <row r="26" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="23" t="n">
         <v>25</v>
       </c>
       <c r="B26" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="C26" s="26" t="s">
+      <c r="C26" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D26" s="15" t="s">
@@ -11526,27 +11530,27 @@
       <c r="F26" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G26" s="22" t="s">
+      <c r="G26" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H26" s="22" t="s">
+      <c r="H26" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I26" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J26" s="26" t="s">
+      <c r="J26" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="27" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A27" s="22" t="n">
+    <row r="27" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="23" t="n">
         <v>26</v>
       </c>
       <c r="B27" s="15" t="s">
         <v>328</v>
       </c>
-      <c r="C27" s="26" t="s">
+      <c r="C27" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D27" s="15" t="s">
@@ -11558,27 +11562,27 @@
       <c r="F27" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G27" s="22" t="s">
+      <c r="G27" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H27" s="22" t="s">
+      <c r="H27" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I27" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J27" s="26" t="s">
+      <c r="J27" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="28" s="18" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A28" s="22" t="n">
+    <row r="28" s="19" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="23" t="n">
         <v>27</v>
       </c>
       <c r="B28" s="15" t="s">
         <v>331</v>
       </c>
-      <c r="C28" s="26" t="s">
+      <c r="C28" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D28" s="15" t="s">
@@ -11590,27 +11594,27 @@
       <c r="F28" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G28" s="22" t="s">
+      <c r="G28" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H28" s="22" t="s">
+      <c r="H28" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I28" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J28" s="26" t="s">
+      <c r="J28" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="29" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A29" s="22" t="n">
+    <row r="29" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="23" t="n">
         <v>28</v>
       </c>
       <c r="B29" s="15" t="s">
         <v>334</v>
       </c>
-      <c r="C29" s="26" t="s">
+      <c r="C29" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D29" s="15" t="s">
@@ -11622,27 +11626,27 @@
       <c r="F29" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G29" s="22" t="s">
+      <c r="G29" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H29" s="22" t="s">
+      <c r="H29" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I29" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J29" s="26" t="s">
+      <c r="J29" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="30" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A30" s="22" t="n">
+    <row r="30" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="23" t="n">
         <v>29</v>
       </c>
       <c r="B30" s="15" t="s">
         <v>337</v>
       </c>
-      <c r="C30" s="26" t="s">
+      <c r="C30" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D30" s="15" t="s">
@@ -11654,27 +11658,27 @@
       <c r="F30" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G30" s="22" t="s">
+      <c r="G30" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H30" s="22" t="s">
+      <c r="H30" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I30" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J30" s="26" t="s">
+      <c r="J30" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="31" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A31" s="22" t="n">
+    <row r="31" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="23" t="n">
         <v>30</v>
       </c>
       <c r="B31" s="15" t="s">
         <v>339</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D31" s="15" t="s">
@@ -11686,27 +11690,27 @@
       <c r="F31" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G31" s="22" t="s">
+      <c r="G31" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H31" s="22" t="s">
+      <c r="H31" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I31" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J31" s="26" t="s">
+      <c r="J31" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="32" s="18" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A32" s="22" t="n">
+    <row r="32" s="19" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="23" t="n">
         <v>31</v>
       </c>
       <c r="B32" s="15" t="s">
         <v>341</v>
       </c>
-      <c r="C32" s="26" t="s">
+      <c r="C32" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D32" s="15" t="s">
@@ -11718,27 +11722,27 @@
       <c r="F32" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G32" s="22" t="s">
+      <c r="G32" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H32" s="22" t="s">
+      <c r="H32" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I32" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J32" s="26" t="s">
+      <c r="J32" s="27" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="33" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A33" s="22" t="n">
+    <row r="33" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="23" t="n">
         <v>32</v>
       </c>
       <c r="B33" s="15" t="s">
         <v>343</v>
       </c>
-      <c r="C33" s="26" t="s">
+      <c r="C33" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D33" s="15" t="s">
@@ -11750,28 +11754,28 @@
       <c r="F33" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G33" s="22" t="s">
+      <c r="G33" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H33" s="22" t="s">
+      <c r="H33" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I33" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J33" s="26" t="s">
+      <c r="J33" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K33" s="24"/>
-    </row>
-    <row r="34" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A34" s="22" t="n">
+      <c r="K33" s="25"/>
+    </row>
+    <row r="34" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="23" t="n">
         <v>33</v>
       </c>
       <c r="B34" s="15" t="s">
         <v>345</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C34" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D34" s="15" t="s">
@@ -11783,28 +11787,28 @@
       <c r="F34" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G34" s="22" t="s">
+      <c r="G34" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H34" s="22" t="s">
+      <c r="H34" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I34" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J34" s="26" t="s">
+      <c r="J34" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K34" s="24"/>
-    </row>
-    <row r="35" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A35" s="22" t="n">
+      <c r="K34" s="25"/>
+    </row>
+    <row r="35" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A35" s="23" t="n">
         <v>34</v>
       </c>
       <c r="B35" s="15" t="s">
         <v>346</v>
       </c>
-      <c r="C35" s="26" t="s">
+      <c r="C35" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D35" s="15" t="s">
@@ -11816,28 +11820,28 @@
       <c r="F35" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G35" s="22" t="s">
+      <c r="G35" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H35" s="22" t="s">
+      <c r="H35" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I35" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J35" s="26" t="s">
+      <c r="J35" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K35" s="24"/>
-    </row>
-    <row r="36" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A36" s="22" t="n">
+      <c r="K35" s="25"/>
+    </row>
+    <row r="36" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="23" t="n">
         <v>35</v>
       </c>
       <c r="B36" s="15" t="s">
         <v>348</v>
       </c>
-      <c r="C36" s="26" t="s">
+      <c r="C36" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D36" s="15" t="s">
@@ -11849,28 +11853,28 @@
       <c r="F36" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G36" s="22" t="s">
+      <c r="G36" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H36" s="22" t="s">
+      <c r="H36" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I36" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J36" s="26" t="s">
+      <c r="J36" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K36" s="24"/>
-    </row>
-    <row r="37" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A37" s="22" t="n">
+      <c r="K36" s="25"/>
+    </row>
+    <row r="37" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A37" s="23" t="n">
         <v>36</v>
       </c>
       <c r="B37" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="C37" s="26" t="s">
+      <c r="C37" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D37" s="15" t="s">
@@ -11882,28 +11886,28 @@
       <c r="F37" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G37" s="22" t="s">
+      <c r="G37" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H37" s="22" t="s">
+      <c r="H37" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I37" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J37" s="26" t="s">
+      <c r="J37" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K37" s="24"/>
-    </row>
-    <row r="38" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A38" s="22" t="n">
+      <c r="K37" s="25"/>
+    </row>
+    <row r="38" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A38" s="23" t="n">
         <v>37</v>
       </c>
       <c r="B38" s="15" t="s">
         <v>352</v>
       </c>
-      <c r="C38" s="26" t="s">
+      <c r="C38" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D38" s="15" t="s">
@@ -11915,28 +11919,28 @@
       <c r="F38" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G38" s="22" t="s">
+      <c r="G38" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H38" s="22" t="s">
+      <c r="H38" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I38" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J38" s="26" t="s">
+      <c r="J38" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K38" s="24"/>
-    </row>
-    <row r="39" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A39" s="22" t="n">
+      <c r="K38" s="25"/>
+    </row>
+    <row r="39" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="23" t="n">
         <v>38</v>
       </c>
       <c r="B39" s="15" t="s">
         <v>354</v>
       </c>
-      <c r="C39" s="26" t="s">
+      <c r="C39" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D39" s="15" t="s">
@@ -11948,28 +11952,28 @@
       <c r="F39" s="15" t="s">
         <v>323</v>
       </c>
-      <c r="G39" s="22" t="s">
+      <c r="G39" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H39" s="22" t="s">
+      <c r="H39" s="23" t="s">
         <v>265</v>
       </c>
       <c r="I39" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J39" s="26" t="s">
+      <c r="J39" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K39" s="24"/>
-    </row>
-    <row r="40" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A40" s="22" t="n">
+      <c r="K39" s="25"/>
+    </row>
+    <row r="40" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="23" t="n">
         <v>39</v>
       </c>
       <c r="B40" s="15" t="s">
         <v>356</v>
       </c>
-      <c r="C40" s="26" t="s">
+      <c r="C40" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D40" s="15" t="s">
@@ -11981,28 +11985,28 @@
       <c r="F40" s="15" t="s">
         <v>358</v>
       </c>
-      <c r="G40" s="22" t="s">
+      <c r="G40" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H40" s="22" t="s">
+      <c r="H40" s="23" t="s">
         <v>359</v>
       </c>
       <c r="I40" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J40" s="26" t="s">
+      <c r="J40" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="K40" s="24"/>
-    </row>
-    <row r="41" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A41" s="22" t="n">
+      <c r="K40" s="25"/>
+    </row>
+    <row r="41" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="23" t="n">
         <v>40</v>
       </c>
       <c r="B41" s="15" t="s">
         <v>360</v>
       </c>
-      <c r="C41" s="26" t="s">
+      <c r="C41" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D41" s="15" t="s">
@@ -12014,28 +12018,28 @@
       <c r="F41" s="15" t="s">
         <v>362</v>
       </c>
-      <c r="G41" s="22" t="s">
+      <c r="G41" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H41" s="22" t="s">
+      <c r="H41" s="23" t="s">
         <v>359</v>
       </c>
       <c r="I41" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J41" s="26" t="s">
+      <c r="J41" s="27" t="s">
         <v>209</v>
       </c>
-      <c r="K41" s="24"/>
-    </row>
-    <row r="42" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A42" s="22" t="n">
+      <c r="K41" s="25"/>
+    </row>
+    <row r="42" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="23" t="n">
         <v>41</v>
       </c>
       <c r="B42" s="15" t="s">
         <v>363</v>
       </c>
-      <c r="C42" s="26" t="s">
+      <c r="C42" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D42" s="15" t="s">
@@ -12047,28 +12051,28 @@
       <c r="F42" s="15" t="s">
         <v>365</v>
       </c>
-      <c r="G42" s="22" t="s">
+      <c r="G42" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H42" s="22" t="s">
+      <c r="H42" s="23" t="s">
         <v>359</v>
       </c>
       <c r="I42" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J42" s="26" t="s">
+      <c r="J42" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K42" s="24"/>
-    </row>
-    <row r="43" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A43" s="22" t="n">
+      <c r="K42" s="25"/>
+    </row>
+    <row r="43" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="23" t="n">
         <v>42</v>
       </c>
       <c r="B43" s="15" t="s">
         <v>366</v>
       </c>
-      <c r="C43" s="26" t="s">
+      <c r="C43" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D43" s="15" t="s">
@@ -12080,28 +12084,28 @@
       <c r="F43" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G43" s="22" t="s">
+      <c r="G43" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H43" s="22" t="s">
+      <c r="H43" s="23" t="s">
         <v>359</v>
       </c>
       <c r="I43" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J43" s="26" t="s">
+      <c r="J43" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K43" s="24"/>
-    </row>
-    <row r="44" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A44" s="22" t="n">
+      <c r="K43" s="25"/>
+    </row>
+    <row r="44" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="23" t="n">
         <v>43</v>
       </c>
       <c r="B44" s="15" t="s">
         <v>369</v>
       </c>
-      <c r="C44" s="26" t="s">
+      <c r="C44" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D44" s="15" t="s">
@@ -12113,28 +12117,28 @@
       <c r="F44" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G44" s="22" t="s">
+      <c r="G44" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H44" s="22" t="s">
+      <c r="H44" s="23" t="s">
         <v>359</v>
       </c>
       <c r="I44" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J44" s="26" t="s">
+      <c r="J44" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K44" s="24"/>
-    </row>
-    <row r="45" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A45" s="22" t="n">
+      <c r="K44" s="25"/>
+    </row>
+    <row r="45" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="23" t="n">
         <v>44</v>
       </c>
       <c r="B45" s="15" t="s">
         <v>371</v>
       </c>
-      <c r="C45" s="26" t="s">
+      <c r="C45" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D45" s="15" t="s">
@@ -12146,28 +12150,28 @@
       <c r="F45" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G45" s="22" t="s">
+      <c r="G45" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H45" s="22" t="s">
+      <c r="H45" s="23" t="s">
         <v>359</v>
       </c>
       <c r="I45" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J45" s="26" t="s">
+      <c r="J45" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K45" s="24"/>
-    </row>
-    <row r="46" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A46" s="22" t="n">
+      <c r="K45" s="25"/>
+    </row>
+    <row r="46" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="23" t="n">
         <v>45</v>
       </c>
       <c r="B46" s="15" t="s">
         <v>373</v>
       </c>
-      <c r="C46" s="26" t="s">
+      <c r="C46" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D46" s="15" t="s">
@@ -12179,28 +12183,28 @@
       <c r="F46" s="15" t="s">
         <v>375</v>
       </c>
-      <c r="G46" s="22" t="s">
+      <c r="G46" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H46" s="22" t="s">
+      <c r="H46" s="23" t="s">
         <v>359</v>
       </c>
       <c r="I46" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J46" s="26" t="s">
+      <c r="J46" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K46" s="24"/>
-    </row>
-    <row r="47" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A47" s="22" t="n">
+      <c r="K46" s="25"/>
+    </row>
+    <row r="47" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="23" t="n">
         <v>46</v>
       </c>
       <c r="B47" s="15" t="s">
         <v>376</v>
       </c>
-      <c r="C47" s="26" t="s">
+      <c r="C47" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D47" s="15" t="s">
@@ -12212,28 +12216,28 @@
       <c r="F47" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G47" s="22" t="s">
+      <c r="G47" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H47" s="22" t="s">
+      <c r="H47" s="23" t="s">
         <v>359</v>
       </c>
       <c r="I47" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J47" s="26" t="s">
+      <c r="J47" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K47" s="24"/>
-    </row>
-    <row r="48" s="18" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A48" s="22" t="n">
+      <c r="K47" s="25"/>
+    </row>
+    <row r="48" s="19" customFormat="true" ht="242.65" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="23" t="n">
         <v>47</v>
       </c>
       <c r="B48" s="15" t="s">
         <v>378</v>
       </c>
-      <c r="C48" s="26" t="s">
+      <c r="C48" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D48" s="15" t="s">
@@ -12245,28 +12249,28 @@
       <c r="F48" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G48" s="22" t="s">
+      <c r="G48" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H48" s="22" t="s">
+      <c r="H48" s="23" t="s">
         <v>359</v>
       </c>
       <c r="I48" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J48" s="26" t="s">
+      <c r="J48" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K48" s="24"/>
-    </row>
-    <row r="49" s="18" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A49" s="22" t="n">
+      <c r="K48" s="25"/>
+    </row>
+    <row r="49" s="19" customFormat="true" ht="255.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A49" s="23" t="n">
         <v>48</v>
       </c>
       <c r="B49" s="15" t="s">
         <v>380</v>
       </c>
-      <c r="C49" s="26" t="s">
+      <c r="C49" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D49" s="15" t="s">
@@ -12278,28 +12282,28 @@
       <c r="F49" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G49" s="22" t="s">
+      <c r="G49" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H49" s="22" t="s">
+      <c r="H49" s="23" t="s">
         <v>359</v>
       </c>
       <c r="I49" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J49" s="26" t="s">
+      <c r="J49" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K49" s="24"/>
-    </row>
-    <row r="50" s="18" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A50" s="22" t="n">
+      <c r="K49" s="25"/>
+    </row>
+    <row r="50" s="19" customFormat="true" ht="268" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="23" t="n">
         <v>49</v>
       </c>
       <c r="B50" s="15" t="s">
         <v>382</v>
       </c>
-      <c r="C50" s="26" t="s">
+      <c r="C50" s="27" t="s">
         <v>243</v>
       </c>
       <c r="D50" s="15" t="s">
@@ -12311,19 +12315,19 @@
       <c r="F50" s="15" t="s">
         <v>368</v>
       </c>
-      <c r="G50" s="22" t="s">
+      <c r="G50" s="23" t="s">
         <v>246</v>
       </c>
-      <c r="H50" s="22" t="s">
+      <c r="H50" s="23" t="s">
         <v>359</v>
       </c>
       <c r="I50" s="15" t="s">
         <v>248</v>
       </c>
-      <c r="J50" s="26" t="s">
+      <c r="J50" s="27" t="s">
         <v>299</v>
       </c>
-      <c r="K50" s="24"/>
+      <c r="K50" s="25"/>
     </row>
   </sheetData>
   <hyperlinks>

</xml_diff>